<commit_message>
Feat : commite all change
</commit_message>
<xml_diff>
--- a/interview problems.xlsx
+++ b/interview problems.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\Pradeeb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Spring\Pradeeb\java-practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1883" uniqueCount="988">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1886" uniqueCount="988">
   <si>
     <t>Curious freaks CODING SHEET by Nandhini</t>
   </si>
@@ -3550,6 +3550,30 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3565,30 +3589,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3873,7 +3873,7 @@
   <dimension ref="A1:G1508"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3885,103 +3885,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="52"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="46"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="55"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="46"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="24"/>
     </row>
     <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="55"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="58"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="33"/>
     </row>
     <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="38"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="36"/>
     </row>
     <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="41"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="38"/>
     </row>
     <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="44"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="41"/>
     </row>
     <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
@@ -3993,15 +3993,15 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="46"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="24"/>
     </row>
     <row r="12" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
@@ -4098,7 +4098,7 @@
       <c r="E19" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="59" t="s">
+      <c r="F19" s="21" t="s">
         <v>987</v>
       </c>
       <c r="G19" s="4"/>
@@ -4117,7 +4117,9 @@
       <c r="E20" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="4"/>
+      <c r="F20" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4134,7 +4136,9 @@
       <c r="E21" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="4"/>
+      <c r="F21" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4151,7 +4155,9 @@
       <c r="E22" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="4"/>
+      <c r="F22" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4861,12 +4867,12 @@
       <c r="A66" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B66" s="47" t="s">
+      <c r="B66" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="49"/>
+      <c r="C66" s="43"/>
+      <c r="D66" s="43"/>
+      <c r="E66" s="44"/>
       <c r="F66" s="12"/>
       <c r="G66" s="12"/>
     </row>
@@ -12484,24 +12490,24 @@
       <c r="G539" s="12"/>
     </row>
     <row r="540" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A540" s="45" t="s">
+      <c r="A540" s="22" t="s">
         <v>975</v>
       </c>
-      <c r="B540" s="40"/>
-      <c r="C540" s="40"/>
-      <c r="D540" s="40"/>
-      <c r="E540" s="46"/>
+      <c r="B540" s="23"/>
+      <c r="C540" s="23"/>
+      <c r="D540" s="23"/>
+      <c r="E540" s="24"/>
       <c r="F540" s="4"/>
       <c r="G540" s="4"/>
     </row>
     <row r="541" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A541" s="21" t="s">
+      <c r="A541" s="45" t="s">
         <v>986</v>
       </c>
-      <c r="B541" s="22"/>
-      <c r="C541" s="22"/>
-      <c r="D541" s="22"/>
-      <c r="E541" s="23"/>
+      <c r="B541" s="46"/>
+      <c r="C541" s="46"/>
+      <c r="D541" s="46"/>
+      <c r="E541" s="47"/>
       <c r="F541" s="17"/>
       <c r="G541" s="17"/>
     </row>
@@ -12527,12 +12533,12 @@
       <c r="A544" s="1" t="s">
         <v>976</v>
       </c>
-      <c r="B544" s="24" t="s">
+      <c r="B544" s="48" t="s">
         <v>977</v>
       </c>
-      <c r="C544" s="25"/>
-      <c r="D544" s="25"/>
-      <c r="E544" s="26"/>
+      <c r="C544" s="49"/>
+      <c r="D544" s="49"/>
+      <c r="E544" s="50"/>
       <c r="F544" s="17"/>
       <c r="G544" s="17"/>
     </row>
@@ -12540,12 +12546,12 @@
       <c r="A545" s="1" t="s">
         <v>978</v>
       </c>
-      <c r="B545" s="27" t="s">
+      <c r="B545" s="51" t="s">
         <v>979</v>
       </c>
-      <c r="C545" s="28"/>
-      <c r="D545" s="28"/>
-      <c r="E545" s="29"/>
+      <c r="C545" s="52"/>
+      <c r="D545" s="52"/>
+      <c r="E545" s="53"/>
       <c r="F545" s="17"/>
       <c r="G545" s="17"/>
     </row>
@@ -12553,25 +12559,25 @@
       <c r="A546" s="2" t="s">
         <v>980</v>
       </c>
-      <c r="B546" s="30" t="s">
+      <c r="B546" s="54" t="s">
         <v>981</v>
       </c>
-      <c r="C546" s="31"/>
-      <c r="D546" s="31"/>
-      <c r="E546" s="32"/>
+      <c r="C546" s="55"/>
+      <c r="D546" s="55"/>
+      <c r="E546" s="56"/>
       <c r="F546" s="17"/>
       <c r="G546" s="17"/>
     </row>
     <row r="547" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A547" s="33" t="s">
+      <c r="A547" s="57" t="s">
         <v>982</v>
       </c>
-      <c r="B547" s="34"/>
-      <c r="C547" s="34"/>
-      <c r="D547" s="34"/>
-      <c r="E547" s="34"/>
-      <c r="F547" s="34"/>
-      <c r="G547" s="35"/>
+      <c r="B547" s="58"/>
+      <c r="C547" s="58"/>
+      <c r="D547" s="58"/>
+      <c r="E547" s="58"/>
+      <c r="F547" s="58"/>
+      <c r="G547" s="59"/>
     </row>
     <row r="548" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A548" s="4"/>
@@ -21224,6 +21230,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A541:E541"/>
+    <mergeCell ref="B544:E544"/>
+    <mergeCell ref="B545:E545"/>
+    <mergeCell ref="B546:E546"/>
+    <mergeCell ref="A547:G547"/>
     <mergeCell ref="A540:E540"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:E2"/>
@@ -21236,11 +21247,6 @@
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="B66:E66"/>
-    <mergeCell ref="A541:E541"/>
-    <mergeCell ref="B544:E544"/>
-    <mergeCell ref="B545:E545"/>
-    <mergeCell ref="B546:E546"/>
-    <mergeCell ref="A547:G547"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="https://www.youtube.com/@curiousfreaks_"/>

</xml_diff>

<commit_message>
some changes are made
</commit_message>
<xml_diff>
--- a/interview problems.xlsx
+++ b/interview problems.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1886" uniqueCount="988">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1894" uniqueCount="989">
   <si>
     <t>Curious freaks CODING SHEET by Nandhini</t>
   </si>
@@ -3045,6 +3045,9 @@
   </si>
   <si>
     <t>YES</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -3123,7 +3126,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3145,6 +3148,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3522,7 +3531,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3551,6 +3560,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -3872,116 +3883,116 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="47" style="3" customWidth="1"/>
+    <col min="2" max="2" width="61.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="50.28515625" style="3" customWidth="1"/>
     <col min="4" max="16384" width="30.85546875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="26"/>
     </row>
     <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="32"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="33"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="35"/>
     </row>
     <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="36"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="38"/>
     </row>
     <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="38"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="40"/>
     </row>
     <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="41"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="43"/>
     </row>
     <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
@@ -3993,15 +4004,15 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="24"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="26"/>
     </row>
     <row r="12" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
@@ -4174,7 +4185,9 @@
       <c r="E23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="4"/>
+      <c r="F23" s="23" t="s">
+        <v>988</v>
+      </c>
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4182,7 +4195,7 @@
       <c r="B24" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="22" t="s">
         <v>32</v>
       </c>
       <c r="D24" s="15" t="s">
@@ -4191,7 +4204,9 @@
       <c r="E24" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="4"/>
+      <c r="F24" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4208,7 +4223,9 @@
       <c r="E25" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="4"/>
+      <c r="F25" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4225,7 +4242,9 @@
       <c r="E26" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F26" s="4"/>
+      <c r="F26" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4242,7 +4261,9 @@
       <c r="E27" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F27" s="4"/>
+      <c r="F27" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4259,7 +4280,9 @@
       <c r="E28" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="4"/>
+      <c r="F28" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4267,7 +4290,7 @@
       <c r="B29" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="22" t="s">
         <v>42</v>
       </c>
       <c r="D29" s="15" t="s">
@@ -4276,7 +4299,9 @@
       <c r="E29" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F29" s="4"/>
+      <c r="F29" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4293,7 +4318,9 @@
       <c r="E30" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F30" s="4"/>
+      <c r="F30" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4867,12 +4894,12 @@
       <c r="A66" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B66" s="42" t="s">
+      <c r="B66" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="C66" s="43"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="44"/>
+      <c r="C66" s="45"/>
+      <c r="D66" s="45"/>
+      <c r="E66" s="46"/>
       <c r="F66" s="12"/>
       <c r="G66" s="12"/>
     </row>
@@ -12490,24 +12517,24 @@
       <c r="G539" s="12"/>
     </row>
     <row r="540" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A540" s="22" t="s">
+      <c r="A540" s="24" t="s">
         <v>975</v>
       </c>
-      <c r="B540" s="23"/>
-      <c r="C540" s="23"/>
-      <c r="D540" s="23"/>
-      <c r="E540" s="24"/>
+      <c r="B540" s="25"/>
+      <c r="C540" s="25"/>
+      <c r="D540" s="25"/>
+      <c r="E540" s="26"/>
       <c r="F540" s="4"/>
       <c r="G540" s="4"/>
     </row>
     <row r="541" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A541" s="45" t="s">
+      <c r="A541" s="47" t="s">
         <v>986</v>
       </c>
-      <c r="B541" s="46"/>
-      <c r="C541" s="46"/>
-      <c r="D541" s="46"/>
-      <c r="E541" s="47"/>
+      <c r="B541" s="48"/>
+      <c r="C541" s="48"/>
+      <c r="D541" s="48"/>
+      <c r="E541" s="49"/>
       <c r="F541" s="17"/>
       <c r="G541" s="17"/>
     </row>
@@ -12533,12 +12560,12 @@
       <c r="A544" s="1" t="s">
         <v>976</v>
       </c>
-      <c r="B544" s="48" t="s">
+      <c r="B544" s="50" t="s">
         <v>977</v>
       </c>
-      <c r="C544" s="49"/>
-      <c r="D544" s="49"/>
-      <c r="E544" s="50"/>
+      <c r="C544" s="51"/>
+      <c r="D544" s="51"/>
+      <c r="E544" s="52"/>
       <c r="F544" s="17"/>
       <c r="G544" s="17"/>
     </row>
@@ -12546,12 +12573,12 @@
       <c r="A545" s="1" t="s">
         <v>978</v>
       </c>
-      <c r="B545" s="51" t="s">
+      <c r="B545" s="53" t="s">
         <v>979</v>
       </c>
-      <c r="C545" s="52"/>
-      <c r="D545" s="52"/>
-      <c r="E545" s="53"/>
+      <c r="C545" s="54"/>
+      <c r="D545" s="54"/>
+      <c r="E545" s="55"/>
       <c r="F545" s="17"/>
       <c r="G545" s="17"/>
     </row>
@@ -12559,25 +12586,25 @@
       <c r="A546" s="2" t="s">
         <v>980</v>
       </c>
-      <c r="B546" s="54" t="s">
+      <c r="B546" s="56" t="s">
         <v>981</v>
       </c>
-      <c r="C546" s="55"/>
-      <c r="D546" s="55"/>
-      <c r="E546" s="56"/>
+      <c r="C546" s="57"/>
+      <c r="D546" s="57"/>
+      <c r="E546" s="58"/>
       <c r="F546" s="17"/>
       <c r="G546" s="17"/>
     </row>
     <row r="547" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A547" s="57" t="s">
+      <c r="A547" s="59" t="s">
         <v>982</v>
       </c>
-      <c r="B547" s="58"/>
-      <c r="C547" s="58"/>
-      <c r="D547" s="58"/>
-      <c r="E547" s="58"/>
-      <c r="F547" s="58"/>
-      <c r="G547" s="59"/>
+      <c r="B547" s="60"/>
+      <c r="C547" s="60"/>
+      <c r="D547" s="60"/>
+      <c r="E547" s="60"/>
+      <c r="F547" s="60"/>
+      <c r="G547" s="61"/>
     </row>
     <row r="548" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A548" s="4"/>

</xml_diff>

<commit_message>
Array 4 question complte
</commit_message>
<xml_diff>
--- a/interview problems.xlsx
+++ b/interview problems.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="991">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="991">
   <si>
     <t>Curious freaks CODING SHEET by Nandhini</t>
   </si>
@@ -3568,6 +3568,21 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -3591,21 +3606,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3889,116 +3889,116 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="61.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="50.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="55.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="55.7109375" style="3" customWidth="1"/>
     <col min="4" max="16384" width="30.85546875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="29"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="32"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="26"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="41"/>
     </row>
     <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="32"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="47"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="35"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="50"/>
     </row>
     <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="38"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="53"/>
     </row>
     <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="55"/>
     </row>
     <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="43"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="58"/>
     </row>
     <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
@@ -4010,15 +4010,15 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="41"/>
     </row>
     <row r="12" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
@@ -4375,7 +4375,7 @@
       <c r="B34" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="22" t="s">
         <v>50</v>
       </c>
       <c r="D34" s="15" t="s">
@@ -4384,7 +4384,9 @@
       <c r="E34" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F34" s="4"/>
+      <c r="F34" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4392,7 +4394,7 @@
       <c r="B35" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="22" t="s">
         <v>52</v>
       </c>
       <c r="D35" s="15" t="s">
@@ -4401,7 +4403,9 @@
       <c r="E35" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F35" s="4"/>
+      <c r="F35" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4418,7 +4422,9 @@
       <c r="E36" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F36" s="4"/>
+      <c r="F36" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4435,7 +4441,9 @@
       <c r="E37" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F37" s="4"/>
+      <c r="F37" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G37" s="4"/>
     </row>
     <row r="38" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4902,12 +4910,12 @@
       <c r="A66" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B66" s="44" t="s">
+      <c r="B66" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="C66" s="45"/>
-      <c r="D66" s="45"/>
-      <c r="E66" s="46"/>
+      <c r="C66" s="60"/>
+      <c r="D66" s="60"/>
+      <c r="E66" s="61"/>
       <c r="F66" s="12"/>
       <c r="G66" s="12"/>
     </row>
@@ -12525,24 +12533,24 @@
       <c r="G539" s="12"/>
     </row>
     <row r="540" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A540" s="24" t="s">
+      <c r="A540" s="39" t="s">
         <v>975</v>
       </c>
-      <c r="B540" s="25"/>
-      <c r="C540" s="25"/>
-      <c r="D540" s="25"/>
-      <c r="E540" s="26"/>
+      <c r="B540" s="40"/>
+      <c r="C540" s="40"/>
+      <c r="D540" s="40"/>
+      <c r="E540" s="41"/>
       <c r="F540" s="4"/>
       <c r="G540" s="4"/>
     </row>
     <row r="541" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A541" s="47" t="s">
+      <c r="A541" s="24" t="s">
         <v>986</v>
       </c>
-      <c r="B541" s="48"/>
-      <c r="C541" s="48"/>
-      <c r="D541" s="48"/>
-      <c r="E541" s="49"/>
+      <c r="B541" s="25"/>
+      <c r="C541" s="25"/>
+      <c r="D541" s="25"/>
+      <c r="E541" s="26"/>
       <c r="F541" s="17"/>
       <c r="G541" s="17"/>
     </row>
@@ -12568,12 +12576,12 @@
       <c r="A544" s="1" t="s">
         <v>976</v>
       </c>
-      <c r="B544" s="50" t="s">
+      <c r="B544" s="27" t="s">
         <v>977</v>
       </c>
-      <c r="C544" s="51"/>
-      <c r="D544" s="51"/>
-      <c r="E544" s="52"/>
+      <c r="C544" s="28"/>
+      <c r="D544" s="28"/>
+      <c r="E544" s="29"/>
       <c r="F544" s="17"/>
       <c r="G544" s="17"/>
     </row>
@@ -12581,12 +12589,12 @@
       <c r="A545" s="1" t="s">
         <v>978</v>
       </c>
-      <c r="B545" s="53" t="s">
+      <c r="B545" s="30" t="s">
         <v>979</v>
       </c>
-      <c r="C545" s="54"/>
-      <c r="D545" s="54"/>
-      <c r="E545" s="55"/>
+      <c r="C545" s="31"/>
+      <c r="D545" s="31"/>
+      <c r="E545" s="32"/>
       <c r="F545" s="17"/>
       <c r="G545" s="17"/>
     </row>
@@ -12594,25 +12602,25 @@
       <c r="A546" s="2" t="s">
         <v>980</v>
       </c>
-      <c r="B546" s="56" t="s">
+      <c r="B546" s="33" t="s">
         <v>981</v>
       </c>
-      <c r="C546" s="57"/>
-      <c r="D546" s="57"/>
-      <c r="E546" s="58"/>
+      <c r="C546" s="34"/>
+      <c r="D546" s="34"/>
+      <c r="E546" s="35"/>
       <c r="F546" s="17"/>
       <c r="G546" s="17"/>
     </row>
     <row r="547" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A547" s="59" t="s">
+      <c r="A547" s="36" t="s">
         <v>982</v>
       </c>
-      <c r="B547" s="60"/>
-      <c r="C547" s="60"/>
-      <c r="D547" s="60"/>
-      <c r="E547" s="60"/>
-      <c r="F547" s="60"/>
-      <c r="G547" s="61"/>
+      <c r="B547" s="37"/>
+      <c r="C547" s="37"/>
+      <c r="D547" s="37"/>
+      <c r="E547" s="37"/>
+      <c r="F547" s="37"/>
+      <c r="G547" s="38"/>
     </row>
     <row r="548" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A548" s="4"/>
@@ -21265,11 +21273,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A541:E541"/>
-    <mergeCell ref="B544:E544"/>
-    <mergeCell ref="B545:E545"/>
-    <mergeCell ref="B546:E546"/>
-    <mergeCell ref="A547:G547"/>
     <mergeCell ref="A540:E540"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:E2"/>
@@ -21282,6 +21285,11 @@
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="B66:E66"/>
+    <mergeCell ref="A541:E541"/>
+    <mergeCell ref="B544:E544"/>
+    <mergeCell ref="B545:E545"/>
+    <mergeCell ref="B546:E546"/>
+    <mergeCell ref="A547:G547"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="https://www.youtube.com/@curiousfreaks_"/>
@@ -21324,1170 +21332,1170 @@
     <hyperlink ref="E30" r:id="rId38" display="https://www.geeksforgeeks.org/perfect-number/"/>
     <hyperlink ref="D33" r:id="rId39" display="https://youtu.be/37E9ckMDdTk?si=0TR032zkFFRqHymE"/>
     <hyperlink ref="E33" r:id="rId40" display="https://www.geeksforgeeks.org/what-is-array/"/>
-    <hyperlink ref="C34" r:id="rId41"/>
-    <hyperlink ref="D34" r:id="rId42" display="https://youtu.be/37E9ckMDdTk?si=0TR032zkFFRqHymE"/>
-    <hyperlink ref="E34" r:id="rId43" display="https://www.geeksforgeeks.org/maximum-and-minimum-in-an-array/"/>
-    <hyperlink ref="C35" r:id="rId44"/>
-    <hyperlink ref="D35" r:id="rId45" display="https://youtu.be/37E9ckMDdTk?si=0TR032zkFFRqHymE"/>
-    <hyperlink ref="E35" r:id="rId46" display="https://www.geeksforgeeks.org/third-largest-element-array-distinct-elements/"/>
-    <hyperlink ref="C36" r:id="rId47"/>
-    <hyperlink ref="D36" r:id="rId48" display="https://youtu.be/wvcQg43_V8U?si=duJ5xqerLGj0IR7R"/>
-    <hyperlink ref="E36" r:id="rId49" display="https://www.geeksforgeeks.org/c-program-to-traverse-an-array/"/>
-    <hyperlink ref="C37" r:id="rId50"/>
-    <hyperlink ref="D37" r:id="rId51" display="https://youtu.be/2D0D8HE6uak?si=HL1gv_qVc7mUaHoJ"/>
-    <hyperlink ref="E37" r:id="rId52" display="https://www.geeksforgeeks.org/find-the-missing-number/"/>
-    <hyperlink ref="D38" r:id="rId53" display="https://youtu.be/2D0D8HE6uak?si=HL1gv_qVc7mUaHoJ"/>
-    <hyperlink ref="C39" r:id="rId54" display="https://www.geeksforgeeks.org/problems/sort-an-array-of-0s-1s-and-2s4231/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D39" r:id="rId55" display="https://youtu.be/tp8JIuCXBaU?si=8iicmWUzbNMzAapK"/>
-    <hyperlink ref="E39" r:id="rId56" display="https://www.geeksforgeeks.org/sort-an-array-of-0s-1s-and-2s/"/>
-    <hyperlink ref="C40" r:id="rId57" display="https://www.geeksforgeeks.org/problems/check-if-two-arrays-are-equal-or-not3847/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="E40" r:id="rId58" display="https://www.geeksforgeeks.org/check-if-two-arrays-are-equal-or-not/"/>
-    <hyperlink ref="C41" r:id="rId59" display="https://www.geeksforgeeks.org/problems/cyclically-rotate-an-array-by-one2614/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D41" r:id="rId60" display="https://youtu.be/BHr381Guz3Y?si=LxSVwsQemuIvjvdu"/>
-    <hyperlink ref="E41" r:id="rId61" display="https://www.geeksforgeeks.org/c-program-cyclically-rotate-array-one/"/>
-    <hyperlink ref="C42" r:id="rId62"/>
-    <hyperlink ref="D42" r:id="rId63" display="https://youtu.be/wvcQg43_V8U?si=sd6dy_KO9X1yvwQY"/>
-    <hyperlink ref="E42" r:id="rId64" display="https://www.geeksforgeeks.org/print-array-after-it-is-right-rotated-k-times/"/>
-    <hyperlink ref="C43" r:id="rId65"/>
-    <hyperlink ref="E43" r:id="rId66" display="https://www.geeksforgeeks.org/find-whether-an-array-is-subset-of-another-array-set-1/"/>
-    <hyperlink ref="D44" r:id="rId67" display="https://youtu.be/KEs5UyBJ39g?si=RVR7_pJUEOH4dlUZ"/>
-    <hyperlink ref="E44" r:id="rId68" display="https://www.geeksforgeeks.org/introduction-to-map-data-structure-and-algorithm-tutorials/"/>
-    <hyperlink ref="C45" r:id="rId69"/>
-    <hyperlink ref="E45" r:id="rId70" display="https://www.geeksforgeeks.org/counting-frequencies-of-array-elements/"/>
-    <hyperlink ref="C47" r:id="rId71" display="https://www.geeksforgeeks.org/problems/key-pair5616/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D47" r:id="rId72" display="https://youtu.be/UXDSeD9mN-k?si=0OalQrKPSoSeO6io"/>
-    <hyperlink ref="E47" r:id="rId73" display="https://www.geeksforgeeks.org/check-if-pair-with-given-sum-exists-in-array/"/>
-    <hyperlink ref="C48" r:id="rId74" display="https://www.geeksforgeeks.org/problems/triplet-sum-in-array-1587115621/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D48" r:id="rId75" display="https://youtu.be/DhFh8Kw7ymk?si=Fwh27YWXIuwurZjz"/>
-    <hyperlink ref="E48" r:id="rId76" display="https://www.geeksforgeeks.org/find-a-triplet-that-sum-to-a-given-value/"/>
-    <hyperlink ref="C49" r:id="rId77"/>
-    <hyperlink ref="D49" r:id="rId78" display="https://youtu.be/eD95WRfh81c?si=01Uliqaf14HWboWE"/>
-    <hyperlink ref="E49" r:id="rId79" display="https://www.geeksforgeeks.org/find-four-elements-that-sum-to-a-given-value-set-2/"/>
-    <hyperlink ref="C50" r:id="rId80"/>
-    <hyperlink ref="D50" r:id="rId81" display="https://youtu.be/cJlJwroDw6o?si=UzoMg7WQXEX_-nQL"/>
-    <hyperlink ref="E50" r:id="rId82" display="https://www.geeksforgeeks.org/find-triplets-array-whose-sum-equal-zero/"/>
-    <hyperlink ref="C51" r:id="rId83" display="https://practice.geeksforgeeks.org/problems/count-the-triplets4615/1"/>
-    <hyperlink ref="D51" r:id="rId84" display="https://youtu.be/jqI7kKIJVF8?si=tN1E706NtO33ZE29"/>
-    <hyperlink ref="E51" r:id="rId85" display="https://www.geeksforgeeks.org/count-triplets-such-that-one-of-the-numbers-can-be-written-as-sum-of-the-other-two/"/>
-    <hyperlink ref="C52" r:id="rId86"/>
-    <hyperlink ref="D52" r:id="rId87" display="https://youtu.be/wvcQg43_V8U?si=sd6dy_KO9X1yvwQY"/>
-    <hyperlink ref="E52" r:id="rId88" display="https://www.geeksforgeeks.org/find-union-and-intersection-of-two-unsorted-arrays/"/>
-    <hyperlink ref="C53" r:id="rId89" display="https://www.geeksforgeeks.org/problems/intersection-of-two-arrays2404/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D53" r:id="rId90" display="https://youtu.be/wvcQg43_V8U?si=sd6dy_KO9X1yvwQY"/>
-    <hyperlink ref="E53" r:id="rId91" display="https://www.geeksforgeeks.org/find-union-and-intersection-of-two-unsorted-arrays/"/>
-    <hyperlink ref="C54" r:id="rId92" display="https://www.geeksforgeeks.org/problems/remove-duplicate-elements-from-sorted-array/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D54" r:id="rId93" display="https://youtu.be/37E9ckMDdTk?si=sgQG1IPqP4_lMLI7"/>
-    <hyperlink ref="E54" r:id="rId94" display="https://www.geeksforgeeks.org/remove-duplicates-sorted-array/"/>
-    <hyperlink ref="C55" r:id="rId95" display="https://www.geeksforgeeks.org/problems/k-th-element-of-two-sorted-array1317/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="E55" r:id="rId96" display="https://www.geeksforgeeks.org/k-th-element-two-sorted-arrays/"/>
-    <hyperlink ref="C56" r:id="rId97"/>
-    <hyperlink ref="D56" r:id="rId98" display="https://youtu.be/frf7qxiN2qU?si=JPQuhDD95ggmdzkh"/>
-    <hyperlink ref="E56" r:id="rId99" display="https://www.geeksforgeeks.org/length-of-longest-subarray-with-increasing-contiguous-elements/"/>
-    <hyperlink ref="C57" r:id="rId100" display="https://www.geeksforgeeks.org/problems/trapping-rain-water-1587115621/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D57" r:id="rId101" display="https://youtu.be/m18Hntz4go8?si=ciSWVbyZK9fRqwlD"/>
-    <hyperlink ref="E57" r:id="rId102" display="https://www.geeksforgeeks.org/trapping-rain-water/"/>
-    <hyperlink ref="C59" r:id="rId103"/>
-    <hyperlink ref="D59" r:id="rId104" display="https://youtu.be/nP_ns3uSh80?si=7StWyumzZ4xALf_n"/>
-    <hyperlink ref="E59" r:id="rId105" display="https://www.geeksforgeeks.org/majority-element/"/>
-    <hyperlink ref="C60" r:id="rId106"/>
-    <hyperlink ref="D60" r:id="rId107" display="https://youtu.be/AHZpyENo7k4?si=Gedgrb5NcCsKTvpr"/>
-    <hyperlink ref="E60" r:id="rId108" display="https://www.geeksforgeeks.org/largest-sum-contiguous-subarray/"/>
-    <hyperlink ref="C61" r:id="rId109"/>
-    <hyperlink ref="D61" r:id="rId110" display="https://youtu.be/AseUmwVNaoY?si=ryexsr9Pkd2oEqLb"/>
-    <hyperlink ref="E61" r:id="rId111" display="https://www.geeksforgeeks.org/inversion-count-in-array-using-merge-sort/"/>
-    <hyperlink ref="C62" r:id="rId112"/>
-    <hyperlink ref="D62" r:id="rId113" display="https://youtu.be/IexN60k62jo?si=fTYDjb_XUvQNSMQK"/>
-    <hyperlink ref="E62" r:id="rId114" display="https://www.geeksforgeeks.org/merging-intervals/"/>
-    <hyperlink ref="C63" r:id="rId115"/>
-    <hyperlink ref="D63" r:id="rId116" display="https://youtu.be/hnswaLJvr6g?si=dsjYUnsya81zUUoU"/>
-    <hyperlink ref="E63" r:id="rId117" display="https://www.geeksforgeeks.org/maximum-product-subarray/"/>
-    <hyperlink ref="C64" r:id="rId118"/>
-    <hyperlink ref="D64" r:id="rId119" display="https://youtu.be/JDOXKqF60RQ?si=N0kQyEkb3HU3cAFN"/>
-    <hyperlink ref="E64" r:id="rId120" display="https://www.geeksforgeeks.org/next-permutation/"/>
-    <hyperlink ref="C65" r:id="rId121"/>
-    <hyperlink ref="D65" r:id="rId122" display="https://youtu.be/QDFM7Mjk2mc?si=N-KRLLlVPFDbP7ig"/>
-    <hyperlink ref="E65" r:id="rId123" display="https://www.geeksforgeeks.org/sieve-of-eratosthenes/"/>
-    <hyperlink ref="B66" r:id="rId124" display="https://youtu.be/FPu9Uld7W-E?si=s_d6cjdb6UtlVg16"/>
-    <hyperlink ref="D69" r:id="rId125" display="https://youtu.be/J1aQ9JN4vZY?si=Zyvvj50RIqnHS_dI"/>
-    <hyperlink ref="E69" r:id="rId126" display="https://www.geeksforgeeks.org/multidimensional-arrays-in-c/"/>
-    <hyperlink ref="C70" r:id="rId127"/>
-    <hyperlink ref="D70" r:id="rId128" display="https://youtu.be/JXU4Akft7yk?si=ftzaCZifMOyqSHYd"/>
-    <hyperlink ref="E70" r:id="rId129" display="https://www.geeksforgeeks.org/search-element-sorted-matrix/"/>
-    <hyperlink ref="C71" r:id="rId130"/>
-    <hyperlink ref="D71" r:id="rId131" display="https://youtu.be/Z0R2u6gd3GU?si=09YatNJUpyE7ZCjg"/>
-    <hyperlink ref="E71" r:id="rId132" display="https://www.geeksforgeeks.org/rotate-a-matrix-by-90-degree-in-clockwise-direction-without-using-any-extra-space/"/>
-    <hyperlink ref="C72" r:id="rId133" display="https://www.geeksforgeeks.org/problems/row-with-minimum-number-of-1s5430/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D72" r:id="rId134" display="https://youtu.be/SCz-1TtYxDI?si=XeAz7btJ6r2MbZuh"/>
-    <hyperlink ref="E72" r:id="rId135" display="https://www.geeksforgeeks.org/find-the-row-with-maximum-number-1s/"/>
-    <hyperlink ref="C73" r:id="rId136"/>
-    <hyperlink ref="D73" r:id="rId137" display="https://youtu.be/Z0R2u6gd3GU?si=7sxqBk_sUWTCigqc"/>
-    <hyperlink ref="E73" r:id="rId138" display="https://www.geeksforgeeks.org/rotate-matrix-right-k-times/"/>
-    <hyperlink ref="C74" r:id="rId139" display="https://www.geeksforgeeks.org/problems/print-matrix-in-diagonal-pattern/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="E74" r:id="rId140" display="https://www.geeksforgeeks.org/print-matrix-diagonal-pattern/"/>
-    <hyperlink ref="C75" r:id="rId141"/>
-    <hyperlink ref="D75" r:id="rId142" display="https://youtu.be/N0MgLvceX7M?si=jJ_jUtmeE5mb0LB0"/>
-    <hyperlink ref="E75" r:id="rId143" display="https://takeuforward.org/data-structure/set-matrix-zero/"/>
-    <hyperlink ref="D77" r:id="rId144" display="https://youtu.be/yVdKa8dnKiE?si=SRrnZral-975-l3T"/>
-    <hyperlink ref="E77" r:id="rId145" display="https://www.geeksforgeeks.org/how-to-solve-time-complexity-recurrence-relations-using-recursion-tree-method/"/>
-    <hyperlink ref="C78" r:id="rId146"/>
-    <hyperlink ref="D78" r:id="rId147" display="https://youtu.be/un6PLygfXrA?si=lTiOfyUrTigDKJuT"/>
-    <hyperlink ref="E78" r:id="rId148" display="https://takeuforward.org/data-structure/print-n-to-1-and-1-to-n-using-recursion/"/>
-    <hyperlink ref="C79" r:id="rId149"/>
-    <hyperlink ref="D79" r:id="rId150" display="https://youtu.be/69ZCDFy-OUo?si=ZSOqIZK0c4L27ad2"/>
-    <hyperlink ref="E79" r:id="rId151" display="https://www.geeksforgeeks.org/program-for-factorial-of-a-number/"/>
-    <hyperlink ref="C80" r:id="rId152" display="https://www.geeksforgeeks.org/problems/nth-fibonacci-number1335/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D80" r:id="rId153" display="https://youtu.be/kvRjNm4rVBE?si=HoIm_q77BpGtePSF"/>
-    <hyperlink ref="E80" r:id="rId154" display="https://www.geeksforgeeks.org/program-for-nth-fibonacci-number/"/>
-    <hyperlink ref="C81" r:id="rId155" display="https://www.geeksforgeeks.org/problems/power-of-numbers-1587115620/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D81" r:id="rId156" display="https://youtu.be/l0YC3876qxg?si=gpooiy_1Voz_M2b6"/>
-    <hyperlink ref="E81" r:id="rId157" display="https://www.geeksforgeeks.org/write-a-c-program-to-calculate-powxn/"/>
-    <hyperlink ref="C82" r:id="rId158"/>
-    <hyperlink ref="D82" r:id="rId159" display="https://youtu.be/tNm_NNSB3_w?si=qRueLOLTmrBAtTTC"/>
-    <hyperlink ref="E82" r:id="rId160" display="https://www.geeksforgeeks.org/c-programs-print-interesting-patterns/"/>
-    <hyperlink ref="C83" r:id="rId161" display="https://practice.geeksforgeeks.org/problems/implement-atoi/1?utm_source=geeksforgeeks&amp;utm_medium=ml_article_practice_tab&amp;utm_campaign=article_practice_tab"/>
-    <hyperlink ref="D83" r:id="rId162" display="https://youtu.be/cXf7NKgT13s?si=7CiE2Yq4IRTwI3vh"/>
-    <hyperlink ref="E83" r:id="rId163" display="https://www.geeksforgeeks.org/recursive-implementation-of-atoi/"/>
-    <hyperlink ref="C84" r:id="rId164"/>
-    <hyperlink ref="D84" r:id="rId165" display="https://youtu.be/bR7mQgwQ_o8?si=sqnpPOV603FTpnTr"/>
-    <hyperlink ref="E84" r:id="rId166" display="https://www.geeksforgeeks.org/pascal-triangle/"/>
-    <hyperlink ref="C87" r:id="rId167"/>
-    <hyperlink ref="D87" r:id="rId168" display="https://youtu.be/MHf6awe89xw?si=SZFA7hgK2TgcOc0p"/>
-    <hyperlink ref="E87" r:id="rId169" display="https://www.geeksforgeeks.org/search-an-element-in-a-sorted-and-pivoted-array/"/>
-    <hyperlink ref="C88" r:id="rId170"/>
-    <hyperlink ref="D88" r:id="rId171" display="https://youtu.be/6zhGS79oQ4k?si=HTYRycV3VAbAV7wJ"/>
-    <hyperlink ref="E88" r:id="rId172" display="https://takeuforward.org/arrays/floor-and-ceil-in-sorted-array/"/>
-    <hyperlink ref="C89" r:id="rId173"/>
-    <hyperlink ref="D89" r:id="rId174" display="https://youtu.be/hjR1IYVx9lY?si=LvMcs8L77aY4RPsP"/>
-    <hyperlink ref="E89" r:id="rId175" display="https://www.geeksforgeeks.org/search-an-element-in-a-sorted-and-pivoted-array/"/>
-    <hyperlink ref="C90" r:id="rId176"/>
-    <hyperlink ref="D90" r:id="rId177" display="https://youtu.be/2D0D8HE6uak?si=lL-NPH7ot2zCdWFk"/>
-    <hyperlink ref="E90" r:id="rId178" display="https://www.geeksforgeeks.org/find-the-missing-number/"/>
-    <hyperlink ref="C91" r:id="rId179" display="https://www.geeksforgeeks.org/problems/square-root/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D91" r:id="rId180" display="https://youtu.be/Bsv3FPUX_BA?si=pkOV3citxe_BydNv"/>
-    <hyperlink ref="E91" r:id="rId181" display="https://www.geeksforgeeks.org/square-root-of-an-integer/"/>
-    <hyperlink ref="C92" r:id="rId182"/>
-    <hyperlink ref="D92" r:id="rId183" display="https://youtu.be/W9QJ8HaRvJQ?si=7qkUdUy7sHugcc-4"/>
-    <hyperlink ref="E92" r:id="rId184" display="https://takeuforward.org/data-structure/search-in-an-infinite-sorted-array/"/>
-    <hyperlink ref="C94" r:id="rId185"/>
-    <hyperlink ref="D94" r:id="rId186" display="https://youtu.be/5qGrJbHhqFs?si=BQOhDElObCoMlfNF"/>
-    <hyperlink ref="E94" r:id="rId187" display="https://www.geeksforgeeks.org/search-an-element-in-a-sorted-and-rotated-array-with-duplicates/"/>
-    <hyperlink ref="C95" r:id="rId188"/>
-    <hyperlink ref="D95" r:id="rId189" display="https://youtu.be/nhEMDKMB44g?si=oulPpoG2QvlG0YgL"/>
-    <hyperlink ref="E95" r:id="rId190" display="https://www.geeksforgeeks.org/find-minimum-element-in-a-sorted-and-rotated-array/"/>
-    <hyperlink ref="C96" r:id="rId191" display="https://www.geeksforgeeks.org/problems/rotation4723/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D96" r:id="rId192" display="https://youtu.be/jtSiWTPLwd0?si=-rI5dZ-3sY3qDsS6"/>
-    <hyperlink ref="E96" r:id="rId193" display="https://www.geeksforgeeks.org/find-rotation-count-rotated-sorted-array/"/>
-    <hyperlink ref="E97" r:id="rId194" display="https://www.geeksforgeeks.org/maximum-element-in-a-sorted-and-rotated-array/"/>
-    <hyperlink ref="C99" r:id="rId195"/>
-    <hyperlink ref="D99" r:id="rId196" display="https://youtu.be/cXxmbemS6XM?si=uuZ5GDVRhz1DuRpp"/>
-    <hyperlink ref="E99" r:id="rId197" display="https://www.geeksforgeeks.org/find-a-peak-in-a-given-array/"/>
-    <hyperlink ref="C100" r:id="rId198"/>
-    <hyperlink ref="D100" r:id="rId199" display="https://youtu.be/W9QJ8HaRvJQ?si=7qkUdUy7sHugcc-4"/>
-    <hyperlink ref="E100" r:id="rId200" display="https://www.geeksforgeeks.org/find-element-bitonic-array/"/>
-    <hyperlink ref="C102" r:id="rId201"/>
-    <hyperlink ref="D102" r:id="rId202" display="https://youtu.be/SCz-1TtYxDI?si=U_jEDIFYaa8QGnxo"/>
-    <hyperlink ref="E102" r:id="rId203" display="https://www.geeksforgeeks.org/find-the-row-with-maximum-number-1s/"/>
-    <hyperlink ref="C103" r:id="rId204" display="https://www.geeksforgeeks.org/problems/search-in-a-matrix-1587115621/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D103" r:id="rId205" display="https://youtu.be/JXU4Akft7yk?si=oY5y29BNgKveTd7q"/>
-    <hyperlink ref="E103" r:id="rId206" display="https://www.geeksforgeeks.org/search-in-row-wise-and-column-wise-sorted-matrix/"/>
-    <hyperlink ref="C104" r:id="rId207"/>
-    <hyperlink ref="D104" r:id="rId208" display="https://youtu.be/9ZbB397jU4k?si=LYzHu6tpjUc5D73I"/>
-    <hyperlink ref="E104" r:id="rId209" display="https://www.geeksforgeeks.org/search-in-a-sorted-2d-matrix-stored-in-row-major-order/"/>
-    <hyperlink ref="C105" r:id="rId210"/>
-    <hyperlink ref="D105" r:id="rId211" display="https://youtu.be/9ZbB397jU4k?si=wSh6BEJiQjJRFuhD"/>
-    <hyperlink ref="E105" r:id="rId212" display="https://www.geeksforgeeks.org/find-peak-element-2d-array/"/>
-    <hyperlink ref="C107" r:id="rId213"/>
-    <hyperlink ref="D107" r:id="rId214" display="https://youtu.be/R_Mfw4ew-Vo?si=5YexrvejL-U8Lp9e"/>
-    <hyperlink ref="E107" r:id="rId215" display="https://www.geeksforgeeks.org/assign-stalls-to-k-cows-to-maximize-the-minimum-distance-between-them/"/>
-    <hyperlink ref="C108" r:id="rId216" display="https://www.geeksforgeeks.org/problems/allocate-minimum-number-of-pages0937/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D108" r:id="rId217" display="https://youtu.be/Z0hwjftStI4?si=md6pnkK1gK2OydeX"/>
-    <hyperlink ref="E108" r:id="rId218" display="https://www.geeksforgeeks.org/allocate-minimum-number-pages/"/>
-    <hyperlink ref="C109" r:id="rId219"/>
-    <hyperlink ref="D109" r:id="rId220" display="https://youtu.be/thUd_WJn6wk?si=83_t-BSmFO1JPtFX"/>
-    <hyperlink ref="E109" r:id="rId221" display="https://www.geeksforgeeks.org/painters-partition-problem/"/>
-    <hyperlink ref="C110" r:id="rId222"/>
-    <hyperlink ref="D110" r:id="rId223" display="https://youtu.be/thUd_WJn6wk?si=83_t-BSmFO1JPtFX"/>
-    <hyperlink ref="E110" r:id="rId224" display="https://www.geeksforgeeks.org/split-the-given-array-into-k-sub-arrays-such-that-maximum-sum-of-all-sub-arrays-is-minimum/"/>
-    <hyperlink ref="C111" r:id="rId225"/>
-    <hyperlink ref="D111" r:id="rId226" display="https://youtu.be/TXAuxeYBTdg?si=am2Vhrx6NzRn666i"/>
-    <hyperlink ref="E111" r:id="rId227" display="https://takeuforward.org/arrays/minimum-days-to-make-m-bouquets/"/>
-    <hyperlink ref="C112" r:id="rId228"/>
-    <hyperlink ref="D112" r:id="rId229" display="https://youtu.be/MG-Ac4TAvTY?si=AZ1NbXoBg0WpOIVu"/>
-    <hyperlink ref="E112" r:id="rId230" display="https://www.geeksforgeeks.org/capacity-to-ship-packages-within-d-days/"/>
-    <hyperlink ref="C113" r:id="rId231"/>
-    <hyperlink ref="D113" r:id="rId232" display="https://youtu.be/qyfekrNni90?si=jMI1EAu9QbNoPwdL"/>
-    <hyperlink ref="E113" r:id="rId233" display="https://www.geeksforgeeks.org/koko-eating-bananas/"/>
-    <hyperlink ref="C114" r:id="rId234"/>
-    <hyperlink ref="D114" r:id="rId235" display="https://youtu.be/N-7biZf7a0I?si=CfkbhxMALJCEo69w"/>
-    <hyperlink ref="E114" r:id="rId236" display="https://www.geeksforgeeks.org/kth-smallest-number-in-multiplication-table/"/>
-    <hyperlink ref="C115" r:id="rId237"/>
-    <hyperlink ref="D115" r:id="rId238" display="https://youtu.be/veu_Q-da6ZY?si=T0MVODyANtV8Q8jE"/>
-    <hyperlink ref="E115" r:id="rId239" display="https://www.geeksforgeeks.org/k-th-smallest-absolute-difference-two-elements-array/"/>
-    <hyperlink ref="C116" r:id="rId240"/>
-    <hyperlink ref="D116" r:id="rId241" display="https://youtu.be/X5SuOsIWCoI?si=EQTTz3FlzY37wihS"/>
-    <hyperlink ref="E116" r:id="rId242" display="https://www.geeksforgeeks.org/ugly-numbers/"/>
-    <hyperlink ref="C117" r:id="rId243" display="https://www.geeksforgeeks.org/problems/median-of-2-sorted-arrays-of-different-sizes/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D117" r:id="rId244" display="https://youtu.be/F9c7LpRZWVQ?si=UBBKqg6vDwaEPBla"/>
-    <hyperlink ref="E117" r:id="rId245" display="https://www.geeksforgeeks.org/median-of-two-sorted-arrays-of-different-sizes/"/>
-    <hyperlink ref="C118" r:id="rId246" display="https://leetcode.com/problems/find-the-smallest-divisor-given-a-threshold/"/>
-    <hyperlink ref="D118" r:id="rId247" display="https://youtu.be/UvBKTVaG6U8?si=U-dfjanJFfqbEEOE"/>
-    <hyperlink ref="E118" r:id="rId248" display="https://takeuforward.org/arrays/find-the-smallest-divisor-given-a-threshold/"/>
-    <hyperlink ref="C120" r:id="rId249" display="https://www.geeksforgeeks.org/problems/bubble-sort/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D120" r:id="rId250" display="https://youtu.be/HGk_ypEuS24?si=7Y4nO0hu37rPwmjB"/>
-    <hyperlink ref="E120" r:id="rId251" display="https://www.geeksforgeeks.org/bubble-sort/"/>
-    <hyperlink ref="C121" r:id="rId252" display="https://www.geeksforgeeks.org/problems/selection-sort/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D121" r:id="rId253" display="https://youtu.be/HGk_ypEuS24?si=7Y4nO0hu37rPwmjB"/>
-    <hyperlink ref="E121" r:id="rId254" display="https://www.geeksforgeeks.org/selection-sort/"/>
-    <hyperlink ref="C122" r:id="rId255" display="https://www.geeksforgeeks.org/problems/insertion-sort/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D122" r:id="rId256" display="https://youtu.be/HGk_ypEuS24?si=7Y4nO0hu37rPwmjB"/>
-    <hyperlink ref="E122" r:id="rId257" display="https://www.geeksforgeeks.org/insertion-sort/"/>
-    <hyperlink ref="C123" r:id="rId258" display="https://www.geeksforgeeks.org/problems/merge-sort/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D123" r:id="rId259" display="https://youtu.be/ogjf7ORKfd8?si=nHB5zJMfQf-fmOim"/>
-    <hyperlink ref="E123" r:id="rId260" display="https://www.geeksforgeeks.org/merge-sort/"/>
-    <hyperlink ref="C124" r:id="rId261" display="https://www.geeksforgeeks.org/problems/quick-sort/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D124" r:id="rId262" display="https://youtu.be/WIrA4YexLRQ?si=IBwwb6xHsi3YGOSN"/>
-    <hyperlink ref="E124" r:id="rId263" display="https://www.geeksforgeeks.org/quick-sort/"/>
-    <hyperlink ref="D126" r:id="rId264" display="https://youtu.be/Nq7ok-OyEpg?si=ryFFMk9gQcXMephl"/>
-    <hyperlink ref="E126" r:id="rId265" display="https://www.geeksforgeeks.org/what-is-linked-list/"/>
-    <hyperlink ref="D127" r:id="rId266" display="https://youtu.be/VaECK03Dz-g?si=-81fgfc9CAs2P-yg"/>
-    <hyperlink ref="E127" r:id="rId267" display="https://www.programiz.com/dsa/linked-list-operations"/>
-    <hyperlink ref="C128" r:id="rId268"/>
-    <hyperlink ref="D128" r:id="rId269" display="https://youtu.be/Nq7ok-OyEpg?si=oiwMXSQZwVteQp7t"/>
-    <hyperlink ref="E128" r:id="rId270" display="https://www.geeksforgeeks.org/search-an-element-in-a-linked-list-iterative-and-recursive/"/>
-    <hyperlink ref="C129" r:id="rId271"/>
-    <hyperlink ref="D129" r:id="rId272" display="https://youtu.be/D2vI2DNJGd8?si=vljGaBvoeAzu2yjH"/>
-    <hyperlink ref="E129" r:id="rId273" display="https://www.geeksforgeeks.org/reverse-a-linked-list/"/>
-    <hyperlink ref="C130" r:id="rId274"/>
-    <hyperlink ref="D130" r:id="rId275" display="https://youtu.be/lRY_G-u_8jk?si=NpNIWRnrnLxtwvHc"/>
-    <hyperlink ref="E130" r:id="rId276" display="https://www.geeksforgeeks.org/function-to-check-if-a-singly-linked-list-is-palindrome/"/>
-    <hyperlink ref="C131" r:id="rId277"/>
-    <hyperlink ref="D131" r:id="rId278" display="https://youtu.be/7LjQ57RqgEc?si=7TB3YSJldSkveCM6"/>
-    <hyperlink ref="E131" r:id="rId279" display="https://www.geeksforgeeks.org/insert-node-middle-linked-list/"/>
-    <hyperlink ref="C132" r:id="rId280"/>
-    <hyperlink ref="D132" r:id="rId281" display="https://youtu.be/0DYoPz2Tpt4?si=kwaZaI8b848cqh7q"/>
-    <hyperlink ref="E132" r:id="rId282" display="https://www.geeksforgeeks.org/write-a-function-to-get-the-intersection-point-of-two-linked-lists/"/>
-    <hyperlink ref="C133" r:id="rId283" display="https://www.geeksforgeeks.org/problems/union-of-two-linked-list/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D133" r:id="rId284" display="https://youtu.be/wvcQg43_V8U?si=hnKPSWEqSjHN9dNn"/>
-    <hyperlink ref="E133" r:id="rId285" display="https://www.geeksforgeeks.org/union-and-intersection-of-two-linked-lists/"/>
-    <hyperlink ref="C134" r:id="rId286"/>
-    <hyperlink ref="D134" r:id="rId287" display="https://youtu.be/icnp4FJdZ_c?si=NZr1bzvtR_ARASzF"/>
-    <hyperlink ref="E134" r:id="rId288" display="https://www.geeksforgeeks.org/delete-a-node-from-linked-list-without-head-pointer/"/>
-    <hyperlink ref="C135" r:id="rId289"/>
-    <hyperlink ref="E135" r:id="rId290" display="https://www.geeksforgeeks.org/count-pairs-two-linked-lists-whose-sum-equal-given-value/"/>
-    <hyperlink ref="C136" r:id="rId291"/>
-    <hyperlink ref="D136" r:id="rId292" display="https://youtu.be/lIar1skcQYI?si=maRDPjLBH_7lm7XJ"/>
-    <hyperlink ref="E136" r:id="rId293" display="https://www.geeksforgeeks.org/reverse-a-linked-list-in-groups-of-given-size/"/>
-    <hyperlink ref="C138" r:id="rId294"/>
-    <hyperlink ref="D138" r:id="rId295" display="https://youtu.be/wiOo4DC5GGA?si=8SqmTgLyYwgXw95f"/>
-    <hyperlink ref="E138" r:id="rId296" display="https://www.geeksforgeeks.org/detect-loop-in-a-linked-list/"/>
-    <hyperlink ref="C139" r:id="rId297"/>
-    <hyperlink ref="D139" r:id="rId298" display="https://youtu.be/I4g1qbkTPus?si=YqFJkeqopml7lRkN"/>
-    <hyperlink ref="E139" r:id="rId299" display="https://www.geeksforgeeks.org/find-length-of-loop-in-linked-list/"/>
-    <hyperlink ref="C140" r:id="rId300"/>
-    <hyperlink ref="D140" r:id="rId301" display="https://youtu.be/2Kd0KKmmHFc?si=G-cVazaPJN8XjgfB"/>
-    <hyperlink ref="E140" r:id="rId302" display="https://www.geeksforgeeks.org/find-first-node-of-loop-in-a-linked-list/"/>
-    <hyperlink ref="C141" r:id="rId303"/>
-    <hyperlink ref="D141" r:id="rId304" display="https://youtu.be/_BG9rjkAXj8?si=egrP9V6ROMAip9jT"/>
-    <hyperlink ref="E141" r:id="rId305" display="https://www.geeksforgeeks.org/detect-and-remove-loop-in-a-linked-list/"/>
-    <hyperlink ref="C143" r:id="rId306"/>
-    <hyperlink ref="D143" r:id="rId307" display="https://youtu.be/gRII7LhdJWc?si=q-xNQeYvdXPR8WWj"/>
-    <hyperlink ref="E143" r:id="rId308" display="https://www.geeksforgeeks.org/sort-a-linked-list-of-0s-1s-or-2s/"/>
-    <hyperlink ref="C144" r:id="rId309"/>
-    <hyperlink ref="D144" r:id="rId310" display="https://youtu.be/bN8nk4ZXzK0?si=iA2AjojAqKG9d_WU"/>
-    <hyperlink ref="E144" r:id="rId311" display="https://www.geeksforgeeks.org/pairwise-swap-elements-of-a-given-linked-list/"/>
-    <hyperlink ref="C145" r:id="rId312"/>
-    <hyperlink ref="D145" r:id="rId313" display="https://youtu.be/q5a5OiGbT6Q?si=IMmJI7RvGvEP59_C"/>
-    <hyperlink ref="E145" r:id="rId314" display="https://www.geeksforgeeks.org/merge-two-sorted-linked-lists/"/>
-    <hyperlink ref="C146" r:id="rId315"/>
-    <hyperlink ref="D146" r:id="rId316" display="https://youtu.be/ogjf7ORKfd8?si=rzOnEXKe2To-rSdw"/>
-    <hyperlink ref="E146" r:id="rId317" display="https://www.geeksforgeeks.org/merge-sort-for-linked-list/"/>
-    <hyperlink ref="C147" r:id="rId318" display="https://www.geeksforgeeks.org/problems/quick-sort-on-linked-list/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D147" r:id="rId319" display="https://youtu.be/WIrA4YexLRQ?si=-NZqIbzEpb-6OARV"/>
-    <hyperlink ref="E147" r:id="rId320" display="https://www.geeksforgeeks.org/quicksort-on-singly-linked-list/"/>
-    <hyperlink ref="D148" r:id="rId321" display="https://youtu.be/YJKVTnOJXSY?si=v8RSH10efQJUvW0C"/>
-    <hyperlink ref="E148" r:id="rId322" display="https://www.geeksforgeeks.org/remove-duplicates-from-a-sorted-linked-list/"/>
-    <hyperlink ref="C149" r:id="rId323"/>
-    <hyperlink ref="D149" r:id="rId324" display="https://www.youtube.com/live/JfWROTUQcn8?si=o9X1KOCltap_orbJ"/>
-    <hyperlink ref="E149" r:id="rId325" display="https://www.geeksforgeeks.org/segregate-even-and-odd-elements-in-a-linked-list/"/>
-    <hyperlink ref="C151" r:id="rId326"/>
-    <hyperlink ref="D151" r:id="rId327" display="https://youtu.be/aXQWhbvT3w0?si=YWdIiQXsrfQHnrYn"/>
-    <hyperlink ref="E151" r:id="rId328" display="https://www.geeksforgeeks.org/add-1-number-represented-linked-list/"/>
-    <hyperlink ref="C152" r:id="rId329"/>
-    <hyperlink ref="D152" r:id="rId330" display="https://youtu.be/LBVsXSMOIk4?si=iIQRk_sF9zAtwknT"/>
-    <hyperlink ref="E152" r:id="rId331" display="https://www.geeksforgeeks.org/add-two-numbers-represented-by-linked-list/"/>
-    <hyperlink ref="C153" r:id="rId332"/>
-    <hyperlink ref="E153" r:id="rId333" display="https://www.geeksforgeeks.org/subtract-two-numbers-represented-as-linked-lists/"/>
-    <hyperlink ref="C155" r:id="rId334"/>
-    <hyperlink ref="D155" r:id="rId335" display="https://youtu.be/uT7YI7XbTY8?si=ueKdt7ev8rjshlGW"/>
-    <hyperlink ref="E155" r:id="rId336" display="https://www.geeksforgeeks.org/rearrange-a-given-linked-list-in-place/"/>
-    <hyperlink ref="C156" r:id="rId337"/>
-    <hyperlink ref="D156" r:id="rId338" display="https://youtu.be/ysytSSXpAI0?si=K3PCYAXGifgKqL1p"/>
-    <hyperlink ref="E156" r:id="rId339" display="https://www.geeksforgeeks.org/flattening-a-linked-list/"/>
-    <hyperlink ref="C157" r:id="rId340"/>
-    <hyperlink ref="D157" r:id="rId341" display="https://youtu.be/jDPrM5XIqzM?si=w0IEUl9Y2qmXSdtC"/>
-    <hyperlink ref="E157" r:id="rId342" display="https://www.geeksforgeeks.org/delete-nodes-which-have-a-greater-value-on-right-side/"/>
-    <hyperlink ref="C158" r:id="rId343"/>
-    <hyperlink ref="D158" r:id="rId344" display="https://youtu.be/icnp4FJdZ_c?si=a2BJWMCc9ETeevAO"/>
-    <hyperlink ref="E158" r:id="rId345" display="https://www.geeksforgeeks.org/delete-n-nodes-after-m-nodes-of-a-linked-list/"/>
-    <hyperlink ref="D159" r:id="rId346" display="https://youtu.be/Mh0NH_SD92k?si=_jaOPDZKpnHohet2"/>
-    <hyperlink ref="C160" r:id="rId347"/>
-    <hyperlink ref="D160" r:id="rId348" display="https://youtu.be/VNf6VynfpdM?si=e1slTowpTqIc---M"/>
-    <hyperlink ref="E160" r:id="rId349" display="https://www.geeksforgeeks.org/a-linked-list-with-next-and-arbit-pointer/"/>
-    <hyperlink ref="C161" r:id="rId350"/>
-    <hyperlink ref="D161" r:id="rId351" display="https://youtu.be/6i_T5kkfv4A?si=L6rVlrvdYuSXGiWa"/>
-    <hyperlink ref="E161" r:id="rId352" display="https://www.geeksforgeeks.org/length-longest-palindrome-list-linked-list-using-o1-extra-space/"/>
-    <hyperlink ref="E162" r:id="rId353" display="https://www.geeksforgeeks.org/circular-linked-list/"/>
-    <hyperlink ref="D164" r:id="rId354" display="https://youtu.be/Nq7ok-OyEpg?si=dDrqbUkV_lKFkLSV"/>
-    <hyperlink ref="E164" r:id="rId355" display="https://www.geeksforgeeks.org/what-is-linked-list/"/>
-    <hyperlink ref="C165" r:id="rId356"/>
-    <hyperlink ref="D165" r:id="rId357" display="https://youtu.be/u3WUW2qe6ww?si=hAazIXgy1oPd1_KJ"/>
-    <hyperlink ref="E165" r:id="rId358" display="https://www.geeksforgeeks.org/reverse-a-doubly-linked-list/"/>
-    <hyperlink ref="C166" r:id="rId359"/>
-    <hyperlink ref="D166" r:id="rId360" display="https://youtu.be/YitR4dQsddE?si=mrZaT1w0xdI_VKYJ"/>
-    <hyperlink ref="E166" r:id="rId361" display="https://www.geeksforgeeks.org/find-pairs-given-sum-doubly-linked-list/"/>
-    <hyperlink ref="C169" r:id="rId362"/>
-    <hyperlink ref="E169" r:id="rId363" display="https://www.geeksforgeeks.org/introduction-to-stack-data-structure-and-algorithm-tutorials/"/>
-    <hyperlink ref="C170" r:id="rId364"/>
-    <hyperlink ref="D170" r:id="rId365" display="https://youtu.be/GYptUgnIM_I?si=YEr87UrxZw1xaMk3"/>
-    <hyperlink ref="E170" r:id="rId366" display="https://www.geeksforgeeks.org/implement-two-stacks-in-an-array/"/>
-    <hyperlink ref="C171" r:id="rId367"/>
-    <hyperlink ref="D171" r:id="rId368" display="https://youtu.be/wkDfsKijrZ8?si=xmSeeK82cI-4hsWZ"/>
-    <hyperlink ref="E171" r:id="rId369" display="https://www.geeksforgeeks.org/check-if-given-parentheses-expression-is-balanced-or-not/"/>
-    <hyperlink ref="C172" r:id="rId370"/>
-    <hyperlink ref="E172" r:id="rId371" display="https://www.geeksforgeeks.org/design-a-stack-that-supports-getmin-in-o1-time-and-o1-extra-space/"/>
-    <hyperlink ref="C174" r:id="rId372"/>
-    <hyperlink ref="D174" r:id="rId373" display="https://youtu.be/Du881K7Jtk8?si=1KDoD1_Ke3mzxlL1"/>
-    <hyperlink ref="E174" r:id="rId374" display="https://www.geeksforgeeks.org/next-greater-element/"/>
-    <hyperlink ref="C175" r:id="rId375"/>
-    <hyperlink ref="E175" r:id="rId376" display="https://www.geeksforgeeks.org/find-the-next-greater-element-in-a-circular-array/"/>
-    <hyperlink ref="C177" r:id="rId377"/>
-    <hyperlink ref="D177" r:id="rId378" display="https://youtu.be/_RtghJnM1Qo?si=4qrv3aDDwijeRm_o"/>
-    <hyperlink ref="E177" r:id="rId379" display="https://www.geeksforgeeks.org/find-the-nearest-smaller-numbers-on-left-side-in-an-array/"/>
-    <hyperlink ref="C178" r:id="rId380"/>
-    <hyperlink ref="D178" r:id="rId381" display="https://youtu.be/_RtghJnM1Qo?si=4qrv3aDDwijeRm_o"/>
-    <hyperlink ref="E178" r:id="rId382" display="https://www.procoding.org/nearest-smaller-to-right"/>
-    <hyperlink ref="C179" r:id="rId383"/>
-    <hyperlink ref="D179" r:id="rId384" display="https://youtu.be/slYh0ZNEqSw?si=Bb04H9MqRP1wTDDl"/>
-    <hyperlink ref="E179" r:id="rId385" display="https://www.geeksforgeeks.org/the-stock-span-problem/"/>
-    <hyperlink ref="C180" r:id="rId386" display="https://www.geeksforgeeks.org/problems/trapping-rain-water-1587115621/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D180" r:id="rId387" display="https://youtu.be/m18Hntz4go8?si=7qLelcwMU1zX_f8T"/>
-    <hyperlink ref="E180" r:id="rId388" display="https://www.geeksforgeeks.org/trapping-rain-water/"/>
-    <hyperlink ref="C181" r:id="rId389"/>
-    <hyperlink ref="D181" r:id="rId390" display="https://youtu.be/X0X6G-eWgQ8?si=MRIKghS-DLv_7Pi2"/>
-    <hyperlink ref="E181" r:id="rId391" display="https://www.geeksforgeeks.org/largest-rectangular-area-in-a-histogram-using-stack/"/>
-    <hyperlink ref="C182" r:id="rId392"/>
-    <hyperlink ref="D182" r:id="rId393" display="https://youtu.be/tOylVCugy9k?si=5qpEF2oU_iQyv1yp"/>
-    <hyperlink ref="E182" r:id="rId394" display="https://www.geeksforgeeks.org/maximum-size-rectangle-binary-sub-matrix-1s/"/>
-    <hyperlink ref="C184" r:id="rId395"/>
-    <hyperlink ref="D184" r:id="rId396" display="https://youtu.be/PAceaOSnxQs?si=LFGbZRMkHTMthAqQ"/>
-    <hyperlink ref="E184" r:id="rId397" display="https://www.geeksforgeeks.org/convert-infix-expression-to-postfix-expression/"/>
-    <hyperlink ref="C185" r:id="rId398"/>
-    <hyperlink ref="D185" r:id="rId399" display="https://youtu.be/u3paQa8KXu0?si=v-QZxZvRK7yRTdnm"/>
-    <hyperlink ref="E185" r:id="rId400" display="https://www.geeksforgeeks.org/evaluation-of-postfix-expression/"/>
-    <hyperlink ref="C186" r:id="rId401"/>
-    <hyperlink ref="D186" r:id="rId402" display="https://youtu.be/RY4GkLahbCI?si=PxZ0CNQSmPe5Iri2"/>
-    <hyperlink ref="E186" r:id="rId403" display="https://www.geeksforgeeks.org/prefix-postfix-conversion/"/>
-    <hyperlink ref="C187" r:id="rId404"/>
-    <hyperlink ref="E187" r:id="rId405" display="https://www.geeksforgeeks.org/arithmetic-expression-evalution/"/>
-    <hyperlink ref="C189" r:id="rId406"/>
-    <hyperlink ref="D189" r:id="rId407" display="https://youtu.be/BmZnJehDzyU?si=bZejmkHrQhG9nc-D"/>
-    <hyperlink ref="E189" r:id="rId408" display="https://www.geeksforgeeks.org/program-to-insert-an-element-at-the-bottom-of-a-stack/"/>
-    <hyperlink ref="C190" r:id="rId409"/>
-    <hyperlink ref="D190" r:id="rId410" display="https://youtu.be/SW14tOda_kI?si=8j5-licSNQkxX7GW"/>
-    <hyperlink ref="E190" r:id="rId411" display="https://www.geeksforgeeks.org/reverse-a-stack-using-recursion/"/>
-    <hyperlink ref="C191" r:id="rId412"/>
-    <hyperlink ref="D191" r:id="rId413" display="https://youtu.be/SjDq1xYxC44?si=Y3th_GK9E5TE4LQt"/>
-    <hyperlink ref="E191" r:id="rId414" display="https://www.geeksforgeeks.org/sort-a-stack-using-recursion/"/>
-    <hyperlink ref="C193" r:id="rId415"/>
-    <hyperlink ref="D193" r:id="rId416" display="https://youtu.be/9u2BJfmWNEg?si=6KkJHm8rjX6xTOsm"/>
-    <hyperlink ref="E193" r:id="rId417" display="https://www.geeksforgeeks.org/the-celebrity-problem/"/>
-    <hyperlink ref="C194" r:id="rId418"/>
-    <hyperlink ref="D194" r:id="rId419" display="https://youtu.be/fIdNHd5nEqI?si=AX5qTxIvmvKKlyRf"/>
-    <hyperlink ref="E194" r:id="rId420" display="https://www.geeksforgeeks.org/reduce-the-string-by-removing-k-consecutive-identical-characters/"/>
-    <hyperlink ref="C195" r:id="rId421"/>
-    <hyperlink ref="D195" r:id="rId422" display="https://www.youtube.com/live/Bg0Y9__J8UE?si=bR4Jmm1QtbwHocbQ"/>
-    <hyperlink ref="E195" r:id="rId423" display="https://www.geeksforgeeks.org/minimum-number-of-bracket-reversals-needed-to-make-an-expression-balanced/"/>
-    <hyperlink ref="C198" r:id="rId424"/>
-    <hyperlink ref="D198" r:id="rId425" display="https://youtu.be/M6GnoUDpqEE?si=_dqoKIYUU275Hcmv"/>
-    <hyperlink ref="E198" r:id="rId426" display="https://www.geeksforgeeks.org/array-implementation-of-queue-simple/"/>
-    <hyperlink ref="C199" r:id="rId427"/>
-    <hyperlink ref="E199" r:id="rId428" display="https://www.geeksforgeeks.org/queue-linked-list-implementation/"/>
-    <hyperlink ref="C200" r:id="rId429"/>
-    <hyperlink ref="D200" r:id="rId430" display="https://youtu.be/3Et9MrMc02A?si=voYSp9_jK2S7pkFr"/>
-    <hyperlink ref="E200" r:id="rId431" display="https://www.geeksforgeeks.org/implement-stack-using-queue/"/>
-    <hyperlink ref="C201" r:id="rId432"/>
-    <hyperlink ref="D201" r:id="rId433" display="https://youtu.be/jDZQKzEtbYQ?si=-3eKyh6SDVQXJPIv"/>
-    <hyperlink ref="E201" r:id="rId434" display="https://www.geeksforgeeks.org/implement-stack-using-queue/"/>
-    <hyperlink ref="C202" r:id="rId435"/>
-    <hyperlink ref="E202" r:id="rId436" display="https://www.geeksforgeeks.org/reversing-a-queue/"/>
-    <hyperlink ref="C204" r:id="rId437"/>
-    <hyperlink ref="D204" r:id="rId438" display="https://youtu.be/_gJ3to4RyeQ?si=qK6-vjLpG1O_jjW3"/>
-    <hyperlink ref="E204" r:id="rId439" display="https://www.geeksforgeeks.org/find-a-tour-that-visits-all-stations/"/>
-    <hyperlink ref="C205" r:id="rId440"/>
-    <hyperlink ref="D205" r:id="rId441" display="https://youtu.be/_gJ3to4RyeQ?si=qK6-vjLpG1O_jjW3"/>
-    <hyperlink ref="E205" r:id="rId442" display="https://www.geeksforgeeks.org/find-first-non-repeating-character-stream-characters/"/>
-    <hyperlink ref="C206" r:id="rId443"/>
-    <hyperlink ref="D206" r:id="rId444" display="https://www.youtube.com/watch?v=_gJ3to4RyeQ&amp;t=4244s"/>
-    <hyperlink ref="E206" r:id="rId445" display="https://www.geeksforgeeks.org/reversing-first-k-elements-queue/"/>
-    <hyperlink ref="C207" r:id="rId446"/>
-    <hyperlink ref="D207" r:id="rId447" display="https://youtu.be/xDEuM5qa0zg?si=1I7GJk3ep77i7dN3"/>
-    <hyperlink ref="E207" r:id="rId448" display="https://www.geeksforgeeks.org/lru-cache-implementation/"/>
-    <hyperlink ref="C208" r:id="rId449"/>
-    <hyperlink ref="E208" r:id="rId450" display="https://www.geeksforgeeks.org/connect-n-ropes-minimum-cost/"/>
-    <hyperlink ref="C209" r:id="rId451"/>
-    <hyperlink ref="E209" r:id="rId452" display="https://www.geeksforgeeks.org/nearly-sorted-algorithm/"/>
-    <hyperlink ref="C212" r:id="rId453" display="https://www.geeksforgeeks.org/problems/max-sum-subarray-of-size-k5313/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D212" r:id="rId454" display="https://youtu.be/TCHSXAu5pls?si=ZP_jrOEraTJAophE"/>
-    <hyperlink ref="E212" r:id="rId455" display="https://www.geeksforgeeks.org/find-maximum-minimum-sum-subarray-size-k/"/>
-    <hyperlink ref="C213" r:id="rId456"/>
-    <hyperlink ref="D213" r:id="rId457" display="https://www.youtube.com/live/3QSvHEmJAkc?si=O76LO8eM72LpKL4s"/>
-    <hyperlink ref="E213" r:id="rId458" display="https://www.geeksforgeeks.org/count-distinct-elements-in-every-window-of-size-k/"/>
-    <hyperlink ref="C214" r:id="rId459"/>
-    <hyperlink ref="D214" r:id="rId460" display="https://www.youtube.com/live/QIDV7m1JrnA?si=Lmr9b8Zi6H06MCTS"/>
-    <hyperlink ref="E214" r:id="rId461" display="https://www.geeksforgeeks.org/first-negative-integer-every-window-size-k/"/>
-    <hyperlink ref="C215" r:id="rId462"/>
-    <hyperlink ref="D215" r:id="rId463" display="https://youtu.be/CZQGRp93K4k?si=7zprdiDcdlnC9vmM"/>
-    <hyperlink ref="E215" r:id="rId464" display="https://www.geeksforgeeks.org/sliding-window-maximum-maximum-of-all-subarrays-of-size-k/"/>
-    <hyperlink ref="C216" r:id="rId465"/>
-    <hyperlink ref="D216" r:id="rId466" display="https://youtu.be/WIkO_t1Kam8?si=u2P3Mo1qvBqxwfRv"/>
-    <hyperlink ref="E216" r:id="rId467" display="https://www.geeksforgeeks.org/count-of-substrings-of-length-k-with-exactly-k-distinct-characters/"/>
-    <hyperlink ref="C217" r:id="rId468"/>
-    <hyperlink ref="D217" r:id="rId469" display="https://www.youtube.com/live/CK8PIAF-m2E?si=t61U2qRD6k7jeFwn"/>
-    <hyperlink ref="E217" r:id="rId470" display="https://www.geeksforgeeks.org/find-the-maximum-of-minimums-for-every-window-size-in-a-given-array/"/>
-    <hyperlink ref="C219" r:id="rId471"/>
-    <hyperlink ref="D219" r:id="rId472" display="https://youtu.be/Ofl4KgFhLsM?si=68FBAztFdbHbV_CF"/>
-    <hyperlink ref="E219" r:id="rId473" display="https://www.geeksforgeeks.org/find-subarray-with-given-sum/"/>
-    <hyperlink ref="C220" r:id="rId474"/>
-    <hyperlink ref="D220" r:id="rId475" display="https://youtu.be/frf7qxiN2qU?si=3VDd0PuUXyWxTFTr"/>
-    <hyperlink ref="E220" r:id="rId476" display="https://www.geeksforgeeks.org/longest-sub-array-sum-k/"/>
-    <hyperlink ref="C221" r:id="rId477"/>
-    <hyperlink ref="D221" r:id="rId478" display="https://youtu.be/xmguZ6GbatA?si=Zxs8fEIzorVIa5_X"/>
-    <hyperlink ref="E221" r:id="rId479" display="https://www.geeksforgeeks.org/find-if-there-is-a-subarray-with-0-sum/"/>
-    <hyperlink ref="C222" r:id="rId480"/>
-    <hyperlink ref="D222" r:id="rId481" display="https://youtu.be/zm50uGBsSz4?si=hGS8FZK2mWMPg-vX"/>
-    <hyperlink ref="E222" r:id="rId482" display="https://www.geeksforgeeks.org/smallest-window-contains-characters-string/"/>
-    <hyperlink ref="C223" r:id="rId483"/>
-    <hyperlink ref="D223" r:id="rId484" display="https://www.youtube.com/live/FMxJQqWaD28?si=py1VR3QKmYSdtQWy"/>
-    <hyperlink ref="E223" r:id="rId485" display="https://www.geeksforgeeks.org/smallest-window-containing-0-1-and-2/"/>
-    <hyperlink ref="C224" r:id="rId486"/>
-    <hyperlink ref="D224" r:id="rId487" display="https://youtu.be/jSto0O4AJbM?si=y-lWXYWB4yZZ9cVQ"/>
-    <hyperlink ref="E224" r:id="rId488" display="https://www.geeksforgeeks.org/find-the-smallest-window-in-a-string-containing-all-characters-of-another-string/"/>
-    <hyperlink ref="C225" r:id="rId489"/>
-    <hyperlink ref="D225" r:id="rId490" display="https://youtu.be/qtVh-XEpsJo?si=DdoYedxtXw0DDrNf"/>
-    <hyperlink ref="E225" r:id="rId491" display="https://www.geeksforgeeks.org/length-of-the-longest-substring-without-repeating-characters/"/>
-    <hyperlink ref="C226" r:id="rId492"/>
-    <hyperlink ref="D226" r:id="rId493" display="https://youtu.be/xmguZ6GbatA?si=x29mj29byvR_FBBd"/>
-    <hyperlink ref="E226" r:id="rId494" display="https://www.geeksforgeeks.org/largest-subarray-with-equal-number-of-0s-and-1s/"/>
-    <hyperlink ref="C227" r:id="rId495"/>
-    <hyperlink ref="D227" r:id="rId496" display="https://youtu.be/fYgU6Bi2fRg?si=q45yqwde54whHlR2"/>
-    <hyperlink ref="E227" r:id="rId497" display="https://www.geeksforgeeks.org/count-occurrences-of-anagrams/"/>
-    <hyperlink ref="C228" r:id="rId498"/>
-    <hyperlink ref="D228" r:id="rId499" display="https://youtu.be/Mo33MjjMlyA?si=01XiyS0oBtaaFenb"/>
-    <hyperlink ref="E228" r:id="rId500" display="https://www.geeksforgeeks.org/maximum-consecutive-ones-formed-by-deleting-at-most-k-0s/"/>
-    <hyperlink ref="C229" r:id="rId501"/>
-    <hyperlink ref="C230" r:id="rId502"/>
-    <hyperlink ref="D230" r:id="rId503" display="https://youtu.be/gqXU1UyA8pk?si=ytPr4mkVqLJfD7v4"/>
-    <hyperlink ref="C231" r:id="rId504"/>
-    <hyperlink ref="D231" r:id="rId505" display="https://youtu.be/gqXU1UyA8pk?si=rMwzYE99DsiO2Gj-"/>
-    <hyperlink ref="C232" r:id="rId506"/>
-    <hyperlink ref="D232" r:id="rId507" display="https://youtu.be/jSto0O4AJbM?si=-ls0q5Dhw9uqf-cF"/>
-    <hyperlink ref="C233" r:id="rId508"/>
-    <hyperlink ref="D233" r:id="rId509" display="https://youtu.be/jSto0O4AJbM?si=-ls0q5Dhw9uqf-cF"/>
-    <hyperlink ref="C234" r:id="rId510"/>
-    <hyperlink ref="D234" r:id="rId511" display="https://youtu.be/akwRFY2eyXs?si=AKnbBikPvDJtF2lA"/>
-    <hyperlink ref="D236" r:id="rId512" display="https://youtu.be/_ANrF3FJm7I?si=U4__gOBVdaEBZwJ9"/>
-    <hyperlink ref="C237" r:id="rId513"/>
-    <hyperlink ref="D237" r:id="rId514" display="https://youtu.be/RlUu72JrOCQ?si=Vfh9JTBxwgVQGeIk"/>
-    <hyperlink ref="E237" r:id="rId515" display="https://www.geeksforgeeks.org/preorder-traversal-of-binary-tree/"/>
-    <hyperlink ref="C238" r:id="rId516"/>
-    <hyperlink ref="D238" r:id="rId517" display="https://youtu.be/Z_NEgBgbRVI?si=Ji2rLUtTb7-6OylN"/>
-    <hyperlink ref="E238" r:id="rId518" display="https://www.geeksforgeeks.org/inorder-traversal-of-binary-tree/"/>
-    <hyperlink ref="C239" r:id="rId519"/>
-    <hyperlink ref="D239" r:id="rId520" display="https://youtu.be/COQOU6klsBg?si=0yuM-upS3qmX2kWF"/>
-    <hyperlink ref="E239" r:id="rId521" display="https://www.geeksforgeeks.org/postorder-traversal-of-binary-tree/"/>
-    <hyperlink ref="C240" r:id="rId522"/>
-    <hyperlink ref="D240" r:id="rId523" display="https://youtu.be/EoAsWbO7sqg?si=1NSXTiOBM6LObxiN"/>
-    <hyperlink ref="E240" r:id="rId524" display="https://www.geeksforgeeks.org/level-order-tree-traversal/"/>
-    <hyperlink ref="C241" r:id="rId525"/>
-    <hyperlink ref="D241" r:id="rId526" display="https://youtu.be/0ca1nvR0be4?si=53I0bM9ppRbgnF0x"/>
-    <hyperlink ref="E241" r:id="rId527" display="https://www.geeksforgeeks.org/boundary-traversal-of-binary-tree/"/>
-    <hyperlink ref="C242" r:id="rId528"/>
-    <hyperlink ref="D242" r:id="rId529" display="https://youtu.be/q_a6lpbKJdw?si=uewd5ll1X-h-GTzT"/>
-    <hyperlink ref="E242" r:id="rId530" display="https://www.geeksforgeeks.org/vertical-order-traversal-of-binary-tree-using-map/"/>
-    <hyperlink ref="C243" r:id="rId531"/>
-    <hyperlink ref="D243" r:id="rId532" display="https://youtu.be/Et9OCDNvJ78?si=oeOojp-R7oWt1IVF"/>
-    <hyperlink ref="E243" r:id="rId533" display="https://www.geeksforgeeks.org/print-nodes-top-view-binary-tree/"/>
-    <hyperlink ref="C244" r:id="rId534"/>
-    <hyperlink ref="D244" r:id="rId535" display="https://youtu.be/0FtVY6I4pB8?si=hfNz5XIojTt16c5K"/>
-    <hyperlink ref="E244" r:id="rId536" display="http://v/"/>
-    <hyperlink ref="C245" r:id="rId537"/>
-    <hyperlink ref="D245" r:id="rId538" display="https://youtu.be/KV4mRzTjlAk?si=_fgLNgJSstGTAq5h"/>
-    <hyperlink ref="E245" r:id="rId539" display="https://www.geeksforgeeks.org/print-left-view-binary-tree/"/>
-    <hyperlink ref="C246" r:id="rId540"/>
-    <hyperlink ref="D246" r:id="rId541" display="https://youtu.be/KV4mRzTjlAk?si=_fgLNgJSstGTAq5h"/>
-    <hyperlink ref="E246" r:id="rId542" display="https://www.geeksforgeeks.org/print-right-view-binary-tree-2/"/>
-    <hyperlink ref="C247" r:id="rId543"/>
-    <hyperlink ref="E247" r:id="rId544" display="https://www.geeksforgeeks.org/diagonal-traversal-of-binary-tree/"/>
-    <hyperlink ref="E249" r:id="rId545" display="https://www.geeksforgeeks.org/insertion-in-binary-search-tree/"/>
-    <hyperlink ref="C250" r:id="rId546"/>
-    <hyperlink ref="D250" r:id="rId547" display="https://youtu.be/eD3tmO66aBA?si=USzVxf8j_Bh8cF9s"/>
-    <hyperlink ref="E250" r:id="rId548" display="https://www.geeksforgeeks.org/find-the-maximum-depth-or-height-of-a-tree/"/>
-    <hyperlink ref="C251" r:id="rId549"/>
-    <hyperlink ref="D251" r:id="rId550" display="https://youtu.be/Rezetez59Nk?si=1PPe8FweQ_aY4r5R"/>
-    <hyperlink ref="E251" r:id="rId551" display="https://www.geeksforgeeks.org/diameter-of-a-binary-tree/"/>
-    <hyperlink ref="C252" r:id="rId552"/>
-    <hyperlink ref="D252" r:id="rId553" display="https://youtu.be/BhuvF_-PWS0?si=jkA1zhLsZjSM3As8"/>
-    <hyperlink ref="E252" r:id="rId554" display="https://www.geeksforgeeks.org/write-c-code-to-determine-if-two-trees-are-identical/"/>
-    <hyperlink ref="C253" r:id="rId555"/>
-    <hyperlink ref="D253" r:id="rId556" display="https://youtu.be/E36O5SWp-LE?si=cIhKUJ-T11II1wJx"/>
-    <hyperlink ref="E253" r:id="rId557" display="https://www.geeksforgeeks.org/check-if-a-binary-tree-is-subtree-of-another-binary-tree/"/>
-    <hyperlink ref="C254" r:id="rId558"/>
-    <hyperlink ref="D254" r:id="rId559" display="https://youtu.be/Yt50Jfbd8Po?si=W4TpdW3XaW-S4cFc"/>
-    <hyperlink ref="E254" r:id="rId560" display="https://www.geeksforgeeks.org/how-to-determine-if-a-binary-tree-is-balanced/"/>
-    <hyperlink ref="C255" r:id="rId561"/>
-    <hyperlink ref="D255" r:id="rId562" display="https://youtu.be/_-QHfMDde90?si=HJ5h-9Tm18BT0ezj"/>
-    <hyperlink ref="E255" r:id="rId563" display="https://www.geeksforgeeks.org/lowest-common-ancestor-binary-tree-set-1/"/>
-    <hyperlink ref="C256" r:id="rId564"/>
-    <hyperlink ref="E256" r:id="rId565" display="https://www.geeksforgeeks.org/check-if-a-given-binary-tree-is-sumtree/"/>
-    <hyperlink ref="C257" r:id="rId566"/>
-    <hyperlink ref="D257" r:id="rId567" display="https://youtu.be/nKggNAiEpBE?si=dUY7QGWwUBs3XxYs"/>
-    <hyperlink ref="E257" r:id="rId568" display="https://www.geeksforgeeks.org/symmetric-tree-tree-which-is-mirror-image-of-itself/"/>
-    <hyperlink ref="C258" r:id="rId569"/>
-    <hyperlink ref="D258" r:id="rId570" display="https://youtu.be/FtdyIHBaKjc?si=pf4peCzMbF56N5UF"/>
-    <hyperlink ref="E258" r:id="rId571" display="https://www.geeksforgeeks.org/write-an-efficient-c-function-to-convert-a-tree-into-its-mirror-tree/"/>
-    <hyperlink ref="C259" r:id="rId572"/>
-    <hyperlink ref="D259" r:id="rId573" display="https://youtu.be/Q9Np3-FX91U?si=ioypQwgjldt1tCGQ"/>
-    <hyperlink ref="C261" r:id="rId574"/>
-    <hyperlink ref="D261" r:id="rId575" display="https://youtu.be/fmflMqVOC7k?si=iSdK8HdoNEeKJARf"/>
-    <hyperlink ref="E261" r:id="rId576" display="https://www.geeksforgeeks.org/given-a-binary-tree-print-all-root-to-leaf-paths/"/>
-    <hyperlink ref="C262" r:id="rId577"/>
-    <hyperlink ref="E262" r:id="rId578" display="https://www.geeksforgeeks.org/root-to-leaf-path-sum-equal-to-a-given-number/"/>
-    <hyperlink ref="C263" r:id="rId579"/>
-    <hyperlink ref="E263" r:id="rId580" display="https://www.geeksforgeeks.org/find-maximum-path-sum-in-a-binary-tree/"/>
-    <hyperlink ref="C264" r:id="rId581"/>
-    <hyperlink ref="D264" r:id="rId582" display="https://youtu.be/7oL8kDCk1OI?si=2qC45jVcOM2sCcJI"/>
-    <hyperlink ref="E264" r:id="rId583" display="https://www.geeksforgeeks.org/count-all-k-sum-paths-in-a-binary-tree/"/>
-    <hyperlink ref="C265" r:id="rId584"/>
-    <hyperlink ref="D265" r:id="rId585" display="https://youtu.be/i9ORlEy6EsI?si=Z4dWg3diarKcc3jR"/>
-    <hyperlink ref="E265" r:id="rId586" display="https://www.geeksforgeeks.org/print-nodes-distance-k-given-node-binary-tree/"/>
-    <hyperlink ref="D266" r:id="rId587" display="https://youtu.be/wIloFJzSOfE?si=qH0sMEREyVagrVK8"/>
-    <hyperlink ref="C267" r:id="rId588"/>
-    <hyperlink ref="D267" r:id="rId589" display="https://youtu.be/joxx4hTYwcw?si=wROhziCvjrJvwsi_"/>
-    <hyperlink ref="E267" r:id="rId590" display="https://www.geeksforgeeks.org/find-distance-between-two-nodes-of-a-binary-tree/"/>
-    <hyperlink ref="C268" r:id="rId591"/>
-    <hyperlink ref="D268" r:id="rId592" display="https://youtu.be/d3ceg_7NcEY?si=dh-dWju5Pqm_WG8E"/>
-    <hyperlink ref="E268" r:id="rId593" display="https://www.geeksforgeeks.org/maximum-difference-between-node-and-its-ancestor-in-binary-tree/"/>
-    <hyperlink ref="C269" r:id="rId594"/>
-    <hyperlink ref="D269" r:id="rId595" display="https://youtu.be/2r5wLmQfD6g?si=Ah-1GqZq9ZvhcISZ"/>
-    <hyperlink ref="E269" r:id="rId596" display="https://www.geeksforgeeks.org/minimum-time-to-burn-a-tree-starting-from-a-leaf-node/"/>
-    <hyperlink ref="D270" r:id="rId597" display="https://youtu.be/p7-9UvDQZ3w?si=iz_Zheaz1rsdY4bv"/>
-    <hyperlink ref="C271" r:id="rId598"/>
-    <hyperlink ref="D271" r:id="rId599" display="https://youtu.be/FiFiNvM29ps?si=7o-MgkkpMI1Aaa5W"/>
-    <hyperlink ref="C272" r:id="rId600"/>
-    <hyperlink ref="D272" r:id="rId601" display="https://youtu.be/KcNt6v_56cc?si=TxJuxG6Ps5NYvy4g"/>
-    <hyperlink ref="E272" r:id="rId602" display="https://www.geeksforgeeks.org/binary-search-tree-data-structure/"/>
-    <hyperlink ref="C273" r:id="rId603"/>
-    <hyperlink ref="E273" r:id="rId604" display="https://www.geeksforgeeks.org/find-maximum-or-minimum-in-binary-tree/"/>
-    <hyperlink ref="C274" r:id="rId605"/>
-    <hyperlink ref="D274" r:id="rId606" display="https://youtu.be/9TJYWh0adfk?si=3x4i8tP5lxtDypuG"/>
-    <hyperlink ref="E274" r:id="rId607" display="https://www.geeksforgeeks.org/find-k-th-smallest-element-in-bst-order-statistics-in-bst/"/>
-    <hyperlink ref="C275" r:id="rId608"/>
-    <hyperlink ref="D275" r:id="rId609" display="https://youtu.be/f-sj7I5oXEI?si=QAg2Uv7BMGfJKGLY"/>
-    <hyperlink ref="E275" r:id="rId610" display="https://www.geeksforgeeks.org/a-program-to-check-if-a-binary-tree-is-bst-or-not/"/>
-    <hyperlink ref="C276" r:id="rId611"/>
-    <hyperlink ref="E276" r:id="rId612" display="https://www.geeksforgeeks.org/find-closest-element-binary-search-tree/"/>
-    <hyperlink ref="C277" r:id="rId613"/>
-    <hyperlink ref="D277" r:id="rId614" display="https://youtu.be/jfk-uX_xKK4?si=2KQlXW2aA51Tz6q5"/>
-    <hyperlink ref="E277" r:id="rId615" display="https://www.geeksforgeeks.org/count-bst-nodes-that-are-in-a-given-range/"/>
-    <hyperlink ref="C278" r:id="rId616"/>
-    <hyperlink ref="D278" r:id="rId617" display="https://youtu.be/X0oXMdtUDwo?si=JBqdu2g0ktKC4DNf"/>
-    <hyperlink ref="E278" r:id="rId618" display="https://www.geeksforgeeks.org/largest-bst-binary-tree-set-2/"/>
-    <hyperlink ref="C279" r:id="rId619"/>
-    <hyperlink ref="D279" r:id="rId620" display="https://youtu.be/cX_kPV_foZc?si=vm8U3w99lvp7UPpc"/>
-    <hyperlink ref="E279" r:id="rId621" display="https://www.geeksforgeeks.org/lowest-common-ancestor-in-a-binary-search-tree/"/>
-    <hyperlink ref="C280" r:id="rId622"/>
-    <hyperlink ref="D280" r:id="rId623" display="https://youtu.be/18w8VduomfI?si=KJ0QdPfLdk6r30Sx"/>
-    <hyperlink ref="E280" r:id="rId624" display="https://www.geeksforgeeks.org/merge-two-bsts-with-limited-extra-space/"/>
-    <hyperlink ref="C281" r:id="rId625"/>
-    <hyperlink ref="D281" r:id="rId626" display="https://youtu.be/SXKAD2svfmI?si=802ib5wC0gtY44eH"/>
-    <hyperlink ref="E281" r:id="rId627" display="https://www.geeksforgeeks.org/inorder-predecessor-successor-given-key-bst/"/>
-    <hyperlink ref="C282" r:id="rId628"/>
-    <hyperlink ref="E282" r:id="rId629" display="https://www.geeksforgeeks.org/populate-inorder-successor-for-all-nodes/"/>
-    <hyperlink ref="C283" r:id="rId630"/>
-    <hyperlink ref="D283" r:id="rId631" display="https://youtu.be/7vVEJwVvAlI?si=Uwd3HoE8H_BhHFb0"/>
-    <hyperlink ref="E283" r:id="rId632" display="https://www.geeksforgeeks.org/transform-bst-sum-tree/"/>
-    <hyperlink ref="C284" r:id="rId633"/>
-    <hyperlink ref="D284" r:id="rId634" display="https://youtu.be/kouxiP_H5WE?si=wjgRijNs4nuSCHXn"/>
-    <hyperlink ref="E284" r:id="rId635" display="https://www.geeksforgeeks.org/deletion-in-binary-search-tree/"/>
-    <hyperlink ref="C286" r:id="rId636"/>
-    <hyperlink ref="D286" r:id="rId637" display="https://youtu.be/aZNaLrVebKQ?si=gAB4STDbhesQVKi0"/>
-    <hyperlink ref="E286" r:id="rId638" display="https://www.geeksforgeeks.org/construct-tree-from-given-inorder-and-preorder-traversal/"/>
-    <hyperlink ref="C287" r:id="rId639"/>
-    <hyperlink ref="D287" r:id="rId640" display="https://youtu.be/LgLRTaEMRVc?si=-Lc1FKuOxYBj4n6u"/>
-    <hyperlink ref="E287" r:id="rId641" display="https://www.geeksforgeeks.org/construct-a-binary-tree-from-postorder-and-inorder/"/>
-    <hyperlink ref="C288" r:id="rId642"/>
-    <hyperlink ref="D288" r:id="rId643" display="https://youtu.be/UmJT3j26t1I?si=tvJcbXtbATGbAUYG"/>
-    <hyperlink ref="E288" r:id="rId644" display="https://www.geeksforgeeks.org/construct-bst-from-given-preorder-traversa/"/>
-    <hyperlink ref="C289" r:id="rId645"/>
-    <hyperlink ref="E289" r:id="rId646" display="https://www.geeksforgeeks.org/construct-a-binary-tree-from-parent-array-representation/"/>
-    <hyperlink ref="C291" r:id="rId647"/>
-    <hyperlink ref="D291" r:id="rId648" display="https://youtu.be/-YbXySKJsX8?si=7GAc6pJLr12-MB1Y"/>
-    <hyperlink ref="E291" r:id="rId649" display="https://www.geeksforgeeks.org/serialize-deserialize-binary-tree/"/>
-    <hyperlink ref="C292" r:id="rId650"/>
-    <hyperlink ref="E292" r:id="rId651" display="https://www.geeksforgeeks.org/find-largest-subtree-sum-tree/"/>
-    <hyperlink ref="C293" r:id="rId652"/>
-    <hyperlink ref="D293" r:id="rId653" display="https://youtu.be/DBxCv9NpPYM?si=jX3oFEBSEGDVyDQF"/>
-    <hyperlink ref="E293" r:id="rId654" display="https://www.geeksforgeeks.org/maximum-sum-nodes-binary-tree-no-two-adjacent/"/>
-    <hyperlink ref="C294" r:id="rId655"/>
-    <hyperlink ref="D294" r:id="rId656" display="https://youtu.be/kn0Z5_qPPzY?si=5hSUj98E7uOL1JXP"/>
-    <hyperlink ref="E294" r:id="rId657" display="https://www.geeksforgeeks.org/find-duplicate-subtrees/"/>
-    <hyperlink ref="C295" r:id="rId658"/>
-    <hyperlink ref="D295" r:id="rId659" display="https://youtu.be/sWf7k1x9XR4?si=fuqHbNz-Kw01_dI1"/>
-    <hyperlink ref="E295" r:id="rId660" display="https://www.geeksforgeeks.org/flatten-a-binary-tree-into-linked-list/"/>
-    <hyperlink ref="C298" r:id="rId661"/>
-    <hyperlink ref="D298" r:id="rId662" display="https://youtu.be/YK78FU5Ffjw?si=b9cfoplt08JA0xJQ"/>
-    <hyperlink ref="E298" r:id="rId663" display="https://www.geeksforgeeks.org/write-a-c-program-to-print-all-permutations-of-a-given-string/"/>
-    <hyperlink ref="C299" r:id="rId664"/>
-    <hyperlink ref="D299" r:id="rId665" display="https://youtu.be/qhBVWf0YafA?si=2t9tPdRW_8ySW1C3"/>
-    <hyperlink ref="E299" r:id="rId666" display="https://www.geeksforgeeks.org/distinct-permutations-string-set-2/"/>
-    <hyperlink ref="C300" r:id="rId667"/>
-    <hyperlink ref="D300" r:id="rId668" display="https://youtu.be/OyZFFqQtu98?si=h4ntlYqyMU635DUw"/>
-    <hyperlink ref="E300" r:id="rId669" display="https://www.geeksforgeeks.org/combinational-sum/"/>
-    <hyperlink ref="C301" r:id="rId670"/>
-    <hyperlink ref="D301" r:id="rId671" display="https://youtu.be/G1fRTGRxXU8?si=CqK5qT_w7EcOkAEh"/>
-    <hyperlink ref="E301" r:id="rId672" display="https://www.geeksforgeeks.org/combinational-sum/"/>
-    <hyperlink ref="C302" r:id="rId673"/>
-    <hyperlink ref="E302" r:id="rId674" display="https://www.geeksforgeeks.org/all-unique-combinations-whose-sum-equals-to-k/"/>
-    <hyperlink ref="C303" r:id="rId675"/>
-    <hyperlink ref="D303" r:id="rId676" display="https://youtu.be/bLGZhJlt4y0?si=bMDZAraICwrxmTnq"/>
-    <hyperlink ref="E303" r:id="rId677" display="https://www.geeksforgeeks.org/rat-in-a-maze/"/>
-    <hyperlink ref="C304" r:id="rId678"/>
-    <hyperlink ref="D304" r:id="rId679" display="https://youtu.be/9ByWqPzfXDU?si=HVyZBiY385QXDma5"/>
-    <hyperlink ref="E304" r:id="rId680" display="https://www.geeksforgeeks.org/find-possible-words-phone-digits/"/>
-    <hyperlink ref="C305" r:id="rId681"/>
-    <hyperlink ref="D305" r:id="rId682" display="https://youtu.be/rYkfBRtMJr8?si=xdRYuVuGFT0hm2UI"/>
-    <hyperlink ref="E305" r:id="rId683" display="https://www.geeksforgeeks.org/backtracking-to-find-all-subsets/"/>
-    <hyperlink ref="C306" r:id="rId684"/>
-    <hyperlink ref="D306" r:id="rId685" display="https://youtu.be/h4zNvA4lbtc?si=uTv2-Y2ji1klfWgb"/>
-    <hyperlink ref="E306" r:id="rId686" display="https://www.geeksforgeeks.org/find-all-unique-subsets-of-a-given-set/"/>
-    <hyperlink ref="C307" r:id="rId687"/>
-    <hyperlink ref="D307" r:id="rId688" display="https://youtu.be/i05Ju7AftcM?si=rSa6wrmVJ8vvkLLz"/>
-    <hyperlink ref="E307" r:id="rId689" display="https://www.geeksforgeeks.org/n-queen-problem-backtracking-3/"/>
-    <hyperlink ref="C308" r:id="rId690"/>
-    <hyperlink ref="C309" r:id="rId691"/>
-    <hyperlink ref="D309" r:id="rId692" display="https://youtu.be/Ya_16rXu7W8?si=c6ZdSR9XKDv4D-gR"/>
-    <hyperlink ref="E309" r:id="rId693" display="https://www.geeksforgeeks.org/print-possible-strings-can-made-placing-spaces/"/>
-    <hyperlink ref="C310" r:id="rId694"/>
-    <hyperlink ref="D310" r:id="rId695" display="https://youtu.be/s9fokUqJ76A?si=zfcDWcp1AqqDy5cG"/>
-    <hyperlink ref="E310" r:id="rId696" display="https://www.geeksforgeeks.org/print-all-combinations-of-balanced-parentheses/"/>
-    <hyperlink ref="C311" r:id="rId697"/>
-    <hyperlink ref="D311" r:id="rId698" display="https://youtu.be/XU4inpwKt8A?si=lm9MpSALwsn4roQo"/>
-    <hyperlink ref="E311" r:id="rId699" display="https://www.geeksforgeeks.org/program-generate-possible-valid-ip-addresses-given-string/"/>
-    <hyperlink ref="C312" r:id="rId700"/>
-    <hyperlink ref="D312" r:id="rId701" display="https://youtu.be/FWAIf_EVUKE?si=q2DUJbZj1T6seOwb"/>
-    <hyperlink ref="E312" r:id="rId702" display="https://www.geeksforgeeks.org/sudoku-backtracking-7/"/>
-    <hyperlink ref="C313" r:id="rId703"/>
-    <hyperlink ref="D313" r:id="rId704" display="https://youtu.be/wT7gcXLYoao?si=cG3Kl4gKxBl92-1m"/>
-    <hyperlink ref="E313" r:id="rId705" display="https://www.geeksforgeeks.org/find-the-k-th-permutation-sequence-of-first-n-natural-numbers/"/>
-    <hyperlink ref="C314" r:id="rId706" display="https://www.geeksforgeeks.org/problems/word-search"/>
-    <hyperlink ref="D314" r:id="rId707" display="https://youtu.be/pfiQ_PS1g8E?si=NSwX3AHJpS6lGme4"/>
-    <hyperlink ref="E314" r:id="rId708" display="https://www.geeksforgeeks.org/search-a-word-in-a-2d-grid-of-characters/"/>
-    <hyperlink ref="C315" r:id="rId709"/>
-    <hyperlink ref="D315" r:id="rId710" display="https://youtu.be/WBgsABoClE0?si=FBXsqWuBLwm75E81"/>
-    <hyperlink ref="E315" r:id="rId711" display="https://www.geeksforgeeks.org/palindrome-partitioning-dp-17/"/>
-    <hyperlink ref="C316" r:id="rId712"/>
-    <hyperlink ref="D316" r:id="rId713" display="https://youtu.be/qB0zZpBJlh8?si=VBKh6H4NSYT6qYVO"/>
-    <hyperlink ref="E316" r:id="rId714" display="https://www.geeksforgeeks.org/decode-string-recursively-encoded-count-followed-substring/"/>
-    <hyperlink ref="C317" r:id="rId715"/>
-    <hyperlink ref="D317" r:id="rId716" display="https://youtu.be/4eOPYDOiwFo?si=VIbEA8JDKDOvwRuD"/>
-    <hyperlink ref="E317" r:id="rId717" display="https://www.geeksforgeeks.org/permute-string-changing-case/"/>
-    <hyperlink ref="C318" r:id="rId718"/>
-    <hyperlink ref="D318" r:id="rId719" display="https://youtu.be/xlPIH9216Ak?si=NpzDre5ux8rDgSdQ"/>
-    <hyperlink ref="E318" r:id="rId720" display="https://www.geeksforgeeks.org/check-given-string-sum-string/"/>
-    <hyperlink ref="C319" r:id="rId721"/>
-    <hyperlink ref="D319" r:id="rId722" display="https://youtu.be/-3rVMYGBwO0?si=w-NmOX7Or4vw8D4T"/>
-    <hyperlink ref="E319" r:id="rId723" display="https://www.geeksforgeeks.org/boggle-find-possible-words-board-characters/"/>
-    <hyperlink ref="C320" r:id="rId724"/>
-    <hyperlink ref="D320" r:id="rId725" display="https://www.youtube.com/live/GstuPf5u3lg?si=9Ymg0mpYPLzeJ38y"/>
-    <hyperlink ref="E320" r:id="rId726" display="https://www.geeksforgeeks.org/find-maximum-number-possible-by-doing-at-most-k-swaps/"/>
-    <hyperlink ref="C321" r:id="rId727"/>
-    <hyperlink ref="D321" r:id="rId728" display="https://youtu.be/mBk4I0X46oI?si=uA-5-uc7zAgLloIe"/>
-    <hyperlink ref="E321" r:id="rId729" display="https://www.geeksforgeeks.org/partition-set-k-subsets-equal-sum/"/>
-    <hyperlink ref="D323" r:id="rId730" display="https://youtu.be/M3_pLsDdeuU?si=SItRP4M088yoch07"/>
-    <hyperlink ref="C324" r:id="rId731"/>
-    <hyperlink ref="D324" r:id="rId732" display="https://youtu.be/-tgVpUgsQ5k?si=Lss9L2Zdy8Gu6BOg"/>
-    <hyperlink ref="E324" r:id="rId733" display="https://www.geeksforgeeks.org/breadth-first-search-or-bfs-for-a-graph/"/>
-    <hyperlink ref="C325" r:id="rId734"/>
-    <hyperlink ref="D325" r:id="rId735" display="https://youtu.be/Qzf1a--rhp8?si=aGYfCnBcl_NDSFad"/>
-    <hyperlink ref="E325" r:id="rId736" display="https://www.geeksforgeeks.org/depth-first-search-or-dfs-for-a-graph/"/>
-    <hyperlink ref="C326" r:id="rId737"/>
-    <hyperlink ref="D326" r:id="rId738" display="https://youtu.be/9twcmtQj4DU?si=8a8yz9stT7quiRiP"/>
-    <hyperlink ref="E326" r:id="rId739" display="https://www.geeksforgeeks.org/detect-cycle-in-a-graph/"/>
-    <hyperlink ref="C327" r:id="rId740"/>
-    <hyperlink ref="D327" r:id="rId741" display="https://youtu.be/zQ3zgFypzX4?si=oXS_VKyOM-oL_4yz"/>
-    <hyperlink ref="E327" r:id="rId742" display="https://www.geeksforgeeks.org/detect-cycle-undirected-graph/"/>
-    <hyperlink ref="C328" r:id="rId743"/>
-    <hyperlink ref="E328" r:id="rId744" display="https://www.geeksforgeeks.org/detect-negative-cycle-graph-bellman-ford/"/>
-    <hyperlink ref="C330" r:id="rId745"/>
-    <hyperlink ref="D330" r:id="rId746" display="https://youtu.be/lea-Wl_uWXY?si=g2dSfr4n7yGr1rmo"/>
-    <hyperlink ref="E330" r:id="rId747" display="https://www.geeksforgeeks.org/strongly-connected-components/"/>
-    <hyperlink ref="C331" r:id="rId748"/>
-    <hyperlink ref="D331" r:id="rId749" display="https://youtu.be/ACzkVtewUYA?si=N0HPRxovroHd2XNQ"/>
-    <hyperlink ref="E331" r:id="rId750" display="https://pnext1.geeksforgeeks.org/problems/number-of-provinces/1?page=1&amp;category%5b%5d=Backtracking&amp;sortBy=submissions"/>
-    <hyperlink ref="C332" r:id="rId751"/>
-    <hyperlink ref="D332" r:id="rId752" display="https://youtu.be/muncqlKJrH0?si=YO3SUPZz6yDpCTM8"/>
-    <hyperlink ref="E332" r:id="rId753" display="https://www.geeksforgeeks.org/find-the-number-of-islands-using-dfs/"/>
-    <hyperlink ref="C333" r:id="rId754"/>
-    <hyperlink ref="D333" r:id="rId755" display="https://youtu.be/7zmgQSJghpo?si=T3zcl9BeVooJBUAX"/>
-    <hyperlink ref="E333" r:id="rId756" display="https://www.geeksforgeeks.org/find-the-number-of-distinct-islands-in-a-2d-matrix/"/>
-    <hyperlink ref="C334" r:id="rId757"/>
-    <hyperlink ref="D334" r:id="rId758" display="https://youtu.be/X8k48xek8g8?si=UILPOo-_LidtdV_k"/>
-    <hyperlink ref="E334" r:id="rId759" display="https://www.geeksforgeeks.org/find-number-of-closed-islands-in-given-matrix/"/>
-    <hyperlink ref="C336" r:id="rId760"/>
-    <hyperlink ref="D336" r:id="rId761" display="https://youtu.be/-vu34sct1g8?si=G9gY0BZEWVQf810J"/>
-    <hyperlink ref="E336" r:id="rId762" display="https://www.geeksforgeeks.org/bipartite-graph/"/>
-    <hyperlink ref="C337" r:id="rId763"/>
-    <hyperlink ref="D337" r:id="rId764" display="https://youtu.be/wuVwUK25Rfc?si=CYcBDjL6ARNTh1FG"/>
-    <hyperlink ref="E337" r:id="rId765" display="https://www.geeksforgeeks.org/m-coloring-problem/"/>
-    <hyperlink ref="C338" r:id="rId766"/>
-    <hyperlink ref="D338" r:id="rId767" display="https://youtu.be/C4gxoTaI71U?si=k1As9n_SZUk7dYJJ"/>
-    <hyperlink ref="E338" r:id="rId768" display="https://www.geeksforgeeks.org/shortest-path-unweighted-graph/"/>
-    <hyperlink ref="C339" r:id="rId769"/>
-    <hyperlink ref="D339" r:id="rId770" display="https://youtu.be/ZUFQfFaU-8U?si=LW37HXwpS6wWWgTC"/>
-    <hyperlink ref="E339" r:id="rId771" display="https://www.geeksforgeeks.org/shortest-path-for-directed-acyclic-graphs/"/>
-    <hyperlink ref="C340" r:id="rId772"/>
-    <hyperlink ref="D340" r:id="rId773" display="https://youtu.be/V6H1qAeB-l4?si=W36zrJBLarmVkn_C"/>
-    <hyperlink ref="E340" r:id="rId774" display="https://www.geeksforgeeks.org/dijkstras-shortest-path-algorithm-greedy-algo-7/"/>
-    <hyperlink ref="C341" r:id="rId775"/>
-    <hyperlink ref="D341" r:id="rId776" display="https://www.youtube.com/live/6lgT0vEhMPo?si=pTJ2-6RIZfCDjz0X"/>
-    <hyperlink ref="E341" r:id="rId777" display="https://www.geeksforgeeks.org/minimum-steps-reach-target-knight/"/>
-    <hyperlink ref="C342" r:id="rId778"/>
-    <hyperlink ref="E342" r:id="rId779" display="https://www.geeksforgeeks.org/shortest-path-from-a-source-cell-to-a-destination-cell-of-a-binary-matrix-through-cells-consisting-only-of-1s/"/>
-    <hyperlink ref="C343" r:id="rId780"/>
-    <hyperlink ref="D343" r:id="rId781" display="https://youtu.be/Eso1Lu4mtmU?si=EqoQnXHqvPXzrtDP"/>
-    <hyperlink ref="E343" r:id="rId782" display="https://www.geeksforgeeks.org/find-if-there-is-a-path-between-two-vertices-in-an-undirected-graph/"/>
-    <hyperlink ref="C344" r:id="rId783"/>
-    <hyperlink ref="E344" r:id="rId784" display="https://www.geeksforgeeks.org/maximum-time-required-for-all-patients-to-get-infected/"/>
-    <hyperlink ref="C345" r:id="rId785"/>
-    <hyperlink ref="D345" r:id="rId786" display="https://youtu.be/t1shZ8_s6jc?si=xHiW9k7kJJ_tUTI5"/>
-    <hyperlink ref="E345" r:id="rId787" display="https://www.geeksforgeeks.org/min-cost-path-dp-6/"/>
-    <hyperlink ref="C346" r:id="rId788"/>
-    <hyperlink ref="D346" r:id="rId789" display="https://youtu.be/tRPda0rcf8E?si=qMWyd0E8oMQ7WIvy"/>
-    <hyperlink ref="E346" r:id="rId790" display="https://takeuforward.org/graph/word-ladder-i-g-29/"/>
-    <hyperlink ref="C347" r:id="rId791"/>
-    <hyperlink ref="D347" r:id="rId792" display="https://youtu.be/DREutrv2XD0?si=QfIrMBzjrv0paKAJ"/>
-    <hyperlink ref="E347" r:id="rId793" display="https://www.geeksforgeeks.org/word-ladder-length-of-shortest-chain-to-reach-a-target-word/"/>
-    <hyperlink ref="C348" r:id="rId794"/>
-    <hyperlink ref="D348" r:id="rId795" display="https://youtu.be/YbY8cVwWAvw?si=qeBBm6l3SrryejiB"/>
-    <hyperlink ref="E348" r:id="rId796" display="https://www.geeksforgeeks.org/floyd-warshall-algorithm-dp-16/"/>
-    <hyperlink ref="C349" r:id="rId797"/>
-    <hyperlink ref="D349" r:id="rId798" display="https://youtu.be/0vVofAhAYjc?si=e1hQOH4PcFbO_QUG"/>
-    <hyperlink ref="E349" r:id="rId799" display="https://www.geeksforgeeks.org/bellman-ford-algorithm-dp-23/"/>
-    <hyperlink ref="C351" r:id="rId800"/>
-    <hyperlink ref="D351" r:id="rId801" display="https://youtu.be/C-2_uSRli8o?si=z2XOpxmnekERJrxc"/>
-    <hyperlink ref="E351" r:id="rId802" display="https://www.geeksforgeeks.org/flood-fill-algorithm/"/>
-    <hyperlink ref="C352" r:id="rId803"/>
-    <hyperlink ref="E352" r:id="rId804" display="https://www.geeksforgeeks.org/given-matrix-o-x-replace-o-x-surrounded-x/"/>
-    <hyperlink ref="C353" r:id="rId805"/>
-    <hyperlink ref="E353" r:id="rId806" display="https://www.geeksforgeeks.org/find-length-largest-region-boolean-matrix/"/>
-    <hyperlink ref="C354" r:id="rId807"/>
-    <hyperlink ref="D354" r:id="rId808" display="https://youtu.be/yf3oUhkvqA0?si=l_DQbwT42fy1ThaI"/>
-    <hyperlink ref="E354" r:id="rId809" display="https://www.geeksforgeeks.org/minimum-time-required-so-that-all-oranges-become-rotten/"/>
-    <hyperlink ref="C356" r:id="rId810"/>
-    <hyperlink ref="D356" r:id="rId811" display="https://youtu.be/5lZ0iJMrUMk?si=d8Saw4jmgjKmfILx"/>
-    <hyperlink ref="E356" r:id="rId812" display="https://www.geeksforgeeks.org/topological-sorting/"/>
-    <hyperlink ref="C357" r:id="rId813"/>
-    <hyperlink ref="E357" r:id="rId814" display="https://pnext2.geeksforgeeks.org/problems/prerequisite-tasks/1?page=1&amp;company%5b%5d=Apple&amp;sortBy=submissions"/>
-    <hyperlink ref="C358" r:id="rId815"/>
-    <hyperlink ref="D358" r:id="rId816" display="https://youtu.be/WAOfKpxYHR8?si=WIg-894F_ejz1hgv"/>
-    <hyperlink ref="E358" r:id="rId817" display="https://www.geeksforgeeks.org/find-whether-it-is-possible-to-finish-all-tasks-or-not-from-given-dependencies/"/>
-    <hyperlink ref="C359" r:id="rId818"/>
-    <hyperlink ref="D359" r:id="rId819" display="https://youtu.be/WAOfKpxYHR8?si=WIg-894F_ejz1hgv"/>
-    <hyperlink ref="E359" r:id="rId820" display="https://www.geeksforgeeks.org/find-the-ordering-of-tasks-from-given-dependencies/"/>
-    <hyperlink ref="C360" r:id="rId821"/>
-    <hyperlink ref="D360" r:id="rId822" display="https://youtu.be/2gtg3VsDGyc?si=yw-aqlNDy3mCHOj5"/>
-    <hyperlink ref="E360" r:id="rId823" display="https://www.geeksforgeeks.org/eventual-safe-states/"/>
-    <hyperlink ref="C361" r:id="rId824"/>
-    <hyperlink ref="D361" r:id="rId825" display="https://youtu.be/U3N_je7tWAs?si=3QjjfX39WxlhedeU"/>
-    <hyperlink ref="E361" r:id="rId826" display="https://www.geeksforgeeks.org/given-sorted-dictionary-find-precedence-characters/"/>
-    <hyperlink ref="C363" r:id="rId827"/>
-    <hyperlink ref="D363" r:id="rId828" display="https://youtu.be/ZSPjZuZWCME?si=qz-SbjuFnphj89qo"/>
-    <hyperlink ref="E363" r:id="rId829" display="https://www.geeksforgeeks.org/kruskals-minimum-spanning-tree-algorithm-greedy-algo-2/"/>
-    <hyperlink ref="C364" r:id="rId830"/>
-    <hyperlink ref="D364" r:id="rId831" display="https://youtu.be/DMnDM_sxVig?si=_xwNmqyl69ykMMNz"/>
-    <hyperlink ref="E364" r:id="rId832" display="https://www.geeksforgeeks.org/kruskals-minimum-spanning-tree-algorithm-greedy-algo-2/"/>
-    <hyperlink ref="C365" r:id="rId833"/>
-    <hyperlink ref="E365" r:id="rId834" display="https://www.geeksforgeeks.org/minimum-cost-connect-cities/"/>
-    <hyperlink ref="C366" r:id="rId835"/>
-    <hyperlink ref="E366" r:id="rId836" display="https://www.geeksforgeeks.org/minimum-cost-required-to-connect-all-houses-in-a-city/"/>
-    <hyperlink ref="C367" r:id="rId837"/>
-    <hyperlink ref="E367" r:id="rId838" display="https://www.geeksforgeeks.org/water-connection-problem/"/>
-    <hyperlink ref="D369" r:id="rId839" display="https://youtu.be/L1T4AB8xBcw?si=aeusCwB3GXg7GprE"/>
-    <hyperlink ref="E369" r:id="rId840" display="https://www.geeksforgeeks.org/disjoint-set-data-structures/"/>
-    <hyperlink ref="D370" r:id="rId841" display="https://youtu.be/L1T4AB8xBcw?si=aeusCwB3GXg7GprE"/>
-    <hyperlink ref="E370" r:id="rId842" display="https://www.geeksforgeeks.org/union-by-rank-and-path-compression-in-union-find-algorithm/"/>
-    <hyperlink ref="C371" r:id="rId843"/>
-    <hyperlink ref="D371" r:id="rId844" display="https://youtu.be/vadly9uWMPU?si=xqtEXZf4OU7HFDru"/>
-    <hyperlink ref="E371" r:id="rId845" display="https://www.geeksforgeeks.org/minimize-count-of-connections-required-to-be-rearranged-to-make-all-the-computers-connected/"/>
-    <hyperlink ref="C372" r:id="rId846"/>
-    <hyperlink ref="D372" r:id="rId847" display="https://youtu.be/kFe_LRWuZjE?si=UUGOKxVpWXgSA3-m"/>
-    <hyperlink ref="E372" r:id="rId848" display="https://www.geeksforgeeks.org/minimum-number-swaps-required-sort-array/"/>
-    <hyperlink ref="C373" r:id="rId849"/>
-    <hyperlink ref="C374" r:id="rId850"/>
-    <hyperlink ref="E374" r:id="rId851" display="https://www.geeksforgeeks.org/find-number-pairs-xy-yx/"/>
-    <hyperlink ref="C375" r:id="rId852"/>
-    <hyperlink ref="D375" r:id="rId853" display="https://youtu.be/Rn6B-Q4SNyA?si=KaMazDJMo73etDEb"/>
-    <hyperlink ref="E375" r:id="rId854" display="https://www.geeksforgeeks.org/find-the-number-of-islands-using-disjoint-set/"/>
-    <hyperlink ref="C376" r:id="rId855" display="https://leetcode.com/problems/making-a-large-island/solutions/"/>
-    <hyperlink ref="D376" r:id="rId856" display="https://youtu.be/fi-_r0MtL5I?si=-Fyp3xqjyPhs6hwg"/>
-    <hyperlink ref="E376" r:id="rId857" display="https://www.geeksforgeeks.org/maximum-connected-group-making-a-large-island/"/>
-    <hyperlink ref="C378" r:id="rId858"/>
-    <hyperlink ref="D378" r:id="rId859" display="https://youtu.be/qrAub5z8FeA?si=X1hIai2nrqJBxs5U"/>
-    <hyperlink ref="E378" r:id="rId860" display="https://www.geeksforgeeks.org/bridge-in-a-graph/"/>
-    <hyperlink ref="C379" r:id="rId861"/>
-    <hyperlink ref="D379" r:id="rId862" display="https://youtu.be/j1QDfU21iZk?si=YzffjCCnc3tpTCAS"/>
-    <hyperlink ref="E379" r:id="rId863" display="https://www.geeksforgeeks.org/articulation-points-or-cut-vertices-in-a-graph/"/>
-    <hyperlink ref="C380" r:id="rId864"/>
-    <hyperlink ref="D380" r:id="rId865" display="https://youtu.be/HsBefuOqkd4?si=YSJZK1P5x22IDyQU"/>
-    <hyperlink ref="E380" r:id="rId866" display="https://www.geeksforgeeks.org/find-all-critical-connections-in-the-graph/"/>
-    <hyperlink ref="C381" r:id="rId867"/>
-    <hyperlink ref="D381" r:id="rId868" display="https://youtu.be/R6uoSjZ2imo?si=rKK-k7JxRlgFJNgj"/>
-    <hyperlink ref="E381" r:id="rId869" display="https://www.geeksforgeeks.org/strongly-connected-components/"/>
-    <hyperlink ref="C382" r:id="rId870"/>
-    <hyperlink ref="D382" r:id="rId871" display="https://youtu.be/UJTVaSITcYY?si=hLAyO48WqDXDDH9h"/>
-    <hyperlink ref="E382" r:id="rId872" display="https://www.geeksforgeeks.org/boggle-find-possible-words-board-characters/"/>
-    <hyperlink ref="C383" r:id="rId873"/>
-    <hyperlink ref="E383" r:id="rId874" display="https://www.geeksforgeeks.org/boggle-find-possible-words-board-characters/"/>
-    <hyperlink ref="C386" r:id="rId875"/>
-    <hyperlink ref="D386" r:id="rId876" display="https://youtu.be/_6QpiqTw_ew?si=xUX4W2QueKEKPr7S"/>
-    <hyperlink ref="E386" r:id="rId877" display="https://www.geeksforgeeks.org/minimum-number-of-jumps-to-reach-end-of-a-given-array/"/>
-    <hyperlink ref="C387" r:id="rId878"/>
-    <hyperlink ref="E387" r:id="rId879" display="https://www.geeksforgeeks.org/minimize-operations-required-to-obtain-n/"/>
-    <hyperlink ref="C388" r:id="rId880"/>
-    <hyperlink ref="E388" r:id="rId881" display="https://www.geeksforgeeks.org/minimize-sum-product-two-arrays-permutations-allowed/"/>
-    <hyperlink ref="C389" r:id="rId882"/>
-    <hyperlink ref="E389" r:id="rId883" display="https://www.geeksforgeeks.org/find-the-largest-number-with-given-number-of-digits-and-sum-of-digits/"/>
-    <hyperlink ref="C390" r:id="rId884"/>
-    <hyperlink ref="E390" r:id="rId885" display="https://www.geeksforgeeks.org/lemonade-stand-change-challenge/"/>
-    <hyperlink ref="C391" r:id="rId886"/>
-    <hyperlink ref="D391" r:id="rId887" display="https://youtu.be/jD_D-b6t_eU?si=2zgyQVT6B0-aSO06"/>
-    <hyperlink ref="E391" r:id="rId888" display="https://www.geeksforgeeks.org/activity-selection-problem-greedy-algo-1/"/>
-    <hyperlink ref="C392" r:id="rId889"/>
-    <hyperlink ref="D392" r:id="rId890" display="https://youtu.be/II6ziNnub1Q?si=nyCFIwB6nl2-LOZo"/>
-    <hyperlink ref="E392" r:id="rId891" display="https://takeuforward.org/data-structure/n-meetings-in-one-room/"/>
-    <hyperlink ref="C393" r:id="rId892"/>
-    <hyperlink ref="D393" r:id="rId893" display="https://youtu.be/dxVcMDI7vyI?si=DCFL2eWvpXNvz3dm"/>
-    <hyperlink ref="E393" r:id="rId894" display="https://www.geeksforgeeks.org/minimum-number-platforms-required-railwaybus-station/"/>
-    <hyperlink ref="C394" r:id="rId895"/>
-    <hyperlink ref="E394" r:id="rId896" display="https://www.geeksforgeeks.org/minimize-the-maximum-difference-between-the-heights/"/>
-    <hyperlink ref="C395" r:id="rId897"/>
-    <hyperlink ref="D395" r:id="rId898" display="https://youtu.be/mVg9CfJvayM?si=ZYElbpIWyYE3yEjA"/>
-    <hyperlink ref="E395" r:id="rId899" display="https://www.geeksforgeeks.org/greedy-algorithm-to-find-minimum-number-of-coins/"/>
-    <hyperlink ref="C396" r:id="rId900"/>
-    <hyperlink ref="D396" r:id="rId901" display="https://youtu.be/LjPx4wQaRIs?si=QuVNrXDBmW0nqlfy"/>
-    <hyperlink ref="E396" r:id="rId902" display="https://www.geeksforgeeks.org/job-sequencing-problem/"/>
-    <hyperlink ref="C397" r:id="rId903"/>
-    <hyperlink ref="D397" r:id="rId904" display="https://youtu.be/F_DDzYnxO14?si=Aiem1u3s1CApvD1Q"/>
-    <hyperlink ref="E397" r:id="rId905" display="https://www.geeksforgeeks.org/fractional-knapsack-problem/"/>
-    <hyperlink ref="C398" r:id="rId906"/>
-    <hyperlink ref="D398" r:id="rId907" display="https://youtu.be/Yan0cv2cLy8?si=6gEyL0RDv97Ebo_S"/>
-    <hyperlink ref="E398" r:id="rId908" display="https://www.geeksforgeeks.org/minimum-number-of-jumps-to-reach-end-of-a-given-array/"/>
-    <hyperlink ref="C399" r:id="rId909"/>
-    <hyperlink ref="D399" r:id="rId910" display="https://youtu.be/A8NUOmlwOlM?si=nSYNoRp7jNmzEZbk"/>
-    <hyperlink ref="E399" r:id="rId911" display="https://www.geeksforgeeks.org/insert-in-sorted-and-non-overlapping-interval-array/"/>
-    <hyperlink ref="C400" r:id="rId912"/>
-    <hyperlink ref="E400" r:id="rId913" display="https://www.geeksforgeeks.org/merging-intervals/"/>
-    <hyperlink ref="C401" r:id="rId914"/>
-    <hyperlink ref="D401" r:id="rId915" display="https://youtu.be/nONCGxWoUfM?si=CCH5fuaNR9Oh4SV9"/>
-    <hyperlink ref="E401" r:id="rId916" display="https://www.geeksforgeeks.org/find-non-overlapping-intervals-among-a-given-set-of-intervals/"/>
-    <hyperlink ref="C402" r:id="rId917"/>
-    <hyperlink ref="D402" r:id="rId918" display="https://youtu.be/_k_c9nqzKN0?si=8aU6CU030tv-stpm"/>
-    <hyperlink ref="E402" r:id="rId919" display="https://www.geeksforgeeks.org/connect-n-ropes-minimum-cost/"/>
-    <hyperlink ref="C403" r:id="rId920"/>
-    <hyperlink ref="E403" r:id="rId921" display="https://walkccc.me/LeetCode/problems/0763/"/>
-    <hyperlink ref="C404" r:id="rId922"/>
-    <hyperlink ref="E404" r:id="rId923" display="https://prepfortech.in/leetcode-solutions/cinema-seat-allocation/"/>
-    <hyperlink ref="C405" r:id="rId924"/>
-    <hyperlink ref="E405" r:id="rId925" display="https://www.geeksforgeeks.org/maximum-length-chain-of-pairs-dp-20/"/>
-    <hyperlink ref="C406" r:id="rId926"/>
-    <hyperlink ref="D406" r:id="rId927" display="https://youtu.be/wkDfsKijrZ8?si=M76SonbMLKKgwvoL"/>
-    <hyperlink ref="E406" r:id="rId928" display="https://www.geeksforgeeks.org/minimum-number-of-parentheses-to-be-added-to-make-it-valid/"/>
-    <hyperlink ref="C407" r:id="rId929"/>
-    <hyperlink ref="E407" r:id="rId930" display="https://www.geeksforgeeks.org/program-for-shortest-job-first-or-sjf-cpu-scheduling-set-1-non-preemptive/"/>
-    <hyperlink ref="C408" r:id="rId931"/>
-    <hyperlink ref="D408" r:id="rId932" display="https://youtu.be/xDEuM5qa0zg?si=lm-_MF96z7x2k-FC"/>
-    <hyperlink ref="E408" r:id="rId933" display="https://www.geeksforgeeks.org/lru-cache-implementation/"/>
-    <hyperlink ref="D411" r:id="rId934" display="https://youtu.be/tyB0ztf0DNY?si=g1XFqILApUcgKtJC"/>
-    <hyperlink ref="C413" r:id="rId935"/>
-    <hyperlink ref="E413" r:id="rId936" display="https://www.geeksforgeeks.org/count-number-of-ways-to-cover-a-distance/"/>
-    <hyperlink ref="C414" r:id="rId937"/>
-    <hyperlink ref="D414" r:id="rId938" display="https://youtu.be/mLfjzJsN8us?si=CtLuQbpWqlseteUe"/>
-    <hyperlink ref="E414" r:id="rId939" display="https://www.geeksforgeeks.org/count-ways-reach-nth-stair/"/>
-    <hyperlink ref="C415" r:id="rId940"/>
-    <hyperlink ref="D415" r:id="rId941" display="https://youtu.be/mLfjzJsN8us?si=CtLuQbpWqlseteUe"/>
-    <hyperlink ref="E415" r:id="rId942" display="https://www.geeksforgeeks.org/count-ways-reach-nth-stair/"/>
-    <hyperlink ref="C416" r:id="rId943"/>
-    <hyperlink ref="E416" r:id="rId944" display="https://www.geeksforgeeks.org/find-maximum-possible-stolen-value-houses/"/>
-    <hyperlink ref="C417" r:id="rId945"/>
-    <hyperlink ref="D417" r:id="rId946" display="https://youtu.be/3WaxQMELSkw?si=uGgE6spsNU-YYdHQ"/>
-    <hyperlink ref="C419" r:id="rId947"/>
-    <hyperlink ref="D419" r:id="rId948" display="https://youtu.be/sdE0A2Oxofw?si=k-DhYLU6A7eaUxPF"/>
-    <hyperlink ref="E419" r:id="rId949" display="https://www.geeksforgeeks.org/count-possible-paths-top-left-bottom-right-nxm-matrix/"/>
-    <hyperlink ref="C420" r:id="rId950"/>
-    <hyperlink ref="D420" r:id="rId951" display="https://youtu.be/TmhpgXScLyY?si=Z7i2x05K982xbodl"/>
-    <hyperlink ref="C421" r:id="rId952"/>
-    <hyperlink ref="E421" r:id="rId953" display="https://www.geeksforgeeks.org/count-possible-paths-top-left-bottom-right-nxm-matrix/"/>
-    <hyperlink ref="C422" r:id="rId954"/>
-    <hyperlink ref="D422" r:id="rId955" display="https://www.youtube.com/watch?v=_rgTlyky1uQ"/>
-    <hyperlink ref="C423" r:id="rId956"/>
-    <hyperlink ref="E423" r:id="rId957" display="https://www.geeksforgeeks.org/find-maximum-path-sum-in-a-binary-tree/"/>
-    <hyperlink ref="C424" r:id="rId958"/>
-    <hyperlink ref="D424" r:id="rId959" display="https://www.youtube.com/watch?v=SrP-PiLSYC0"/>
-    <hyperlink ref="C425" r:id="rId960"/>
-    <hyperlink ref="E425" r:id="rId961" display="https://www.geeksforgeeks.org/number-of-paths-with-exactly-k-coins/"/>
-    <hyperlink ref="C426" r:id="rId962"/>
-    <hyperlink ref="D426" r:id="rId963" display="https://youtu.be/N_aJ5qQbYA0?si=ezuW1n6Qa8XxTNEo"/>
-    <hyperlink ref="C427" r:id="rId964"/>
-    <hyperlink ref="C429" r:id="rId965"/>
-    <hyperlink ref="D429" r:id="rId966" display="https://youtu.be/fWX9xDmIzRI?si=JE2TrHBWy_MknoPu"/>
-    <hyperlink ref="C430" r:id="rId967"/>
-    <hyperlink ref="D430" r:id="rId968" display="https://youtu.be/ZHyb-A2Mte4?si=E2zp3ic9YMCmi1el"/>
-    <hyperlink ref="C431" r:id="rId969"/>
-    <hyperlink ref="D431" r:id="rId970" display="https://youtu.be/7win3dcgo3k?si=b7S5AhlT68DbwSRC"/>
-    <hyperlink ref="E431" r:id="rId971" display="https://www.geeksforgeeks.org/partition-problem-dp-18/"/>
-    <hyperlink ref="C432" r:id="rId972"/>
-    <hyperlink ref="D432" r:id="rId973" display="https://youtu.be/GS_OqZb2CWc?si=jtDc7dlrqIBDGkva"/>
-    <hyperlink ref="D433" r:id="rId974" display="https://youtu.be/zoilQD1kYSg?si=Dob0JEkW4sUmGoXn"/>
-    <hyperlink ref="C434" r:id="rId975"/>
-    <hyperlink ref="D434" r:id="rId976" display="https://youtu.be/GqOmJHQZivw?si=Z9uoyRurFlHaiwRs"/>
-    <hyperlink ref="E434" r:id="rId977" display="https://www.geeksforgeeks.org/0-1-knapsack-problem-dp-10/"/>
-    <hyperlink ref="C435" r:id="rId978"/>
-    <hyperlink ref="D435" r:id="rId979" display="https://youtu.be/GrMBfJNk_NY?si=i1ZMM-MkZu3TUA4w"/>
-    <hyperlink ref="C436" r:id="rId980"/>
-    <hyperlink ref="D436" r:id="rId981" display="https://youtu.be/HgyouUi11zk?si=lHMMApBzC27_NrBU"/>
-    <hyperlink ref="E436" r:id="rId982" display="https://www.geeksforgeeks.org/coin-change-dp-7/"/>
-    <hyperlink ref="C437" r:id="rId983"/>
-    <hyperlink ref="D437" r:id="rId984" display="https://youtu.be/myPeWb3Y68A?si=eeOZCGj3ebD3fay7"/>
-    <hyperlink ref="E437" r:id="rId985" display="https://www.geeksforgeeks.org/find-minimum-number-of-coins-that-make-a-change/"/>
-    <hyperlink ref="C438" r:id="rId986"/>
-    <hyperlink ref="D438" r:id="rId987" display="https://youtu.be/mO8XpGoJwuo?si=qNYFr6yJNxqmw4ky"/>
-    <hyperlink ref="C439" r:id="rId988"/>
-    <hyperlink ref="D439" r:id="rId989" display="https://youtu.be/b3GD8263-PQ?si=x22ue_uHcCp3vLdu"/>
-    <hyperlink ref="C440" r:id="rId990"/>
-    <hyperlink ref="C441" r:id="rId991"/>
-    <hyperlink ref="D441" r:id="rId992" display="https://youtu.be/OgvOZ6OrJoY?si=dmmo3by1GELu0E6u"/>
-    <hyperlink ref="E441" r:id="rId993" display="https://www.geeksforgeeks.org/unbounded-knapsack-repetition-items-allowed/"/>
-    <hyperlink ref="C443" r:id="rId994"/>
-    <hyperlink ref="D443" r:id="rId995" display="https://youtu.be/ekcwMsSIzVc?si=8zc9o-Q9JBpR_rLs"/>
-    <hyperlink ref="D444" r:id="rId996" display="https://youtu.be/IFfYfonAFGc?si=KQW5W74J8e_n_kXZ"/>
-    <hyperlink ref="C445" r:id="rId997"/>
-    <hyperlink ref="D445" r:id="rId998" display="https://youtu.be/y4vN0WNdrlg?si=1n-HYDfzakhkM-6W"/>
-    <hyperlink ref="E445" r:id="rId999" display="https://www.geeksforgeeks.org/longest-bitonic-subsequence-dp-15/"/>
-    <hyperlink ref="C446" r:id="rId1000"/>
-    <hyperlink ref="D446" r:id="rId1001" display="https://youtu.be/gDuZwBW9VvM?si=1E77tHD7jaVItSLZ"/>
-    <hyperlink ref="C447" r:id="rId1002"/>
-    <hyperlink ref="D447" r:id="rId1003" display="https://youtu.be/YY8iBaYcc4g?si=SVp9w9fPBfUcqhqG"/>
-    <hyperlink ref="C448" r:id="rId1004"/>
-    <hyperlink ref="D448" r:id="rId1005" display="https://youtu.be/cKVl1TFdNXg?si=N8t9as5OGiHoVzrG"/>
-    <hyperlink ref="C450" r:id="rId1006" display="https://leetcode.com/problems/longest-common-subsequence/"/>
-    <hyperlink ref="D450" r:id="rId1007" display="https://youtu.be/NPZn9jBrX8U?si=c38YFd7X1c-QcPRq"/>
-    <hyperlink ref="E450" r:id="rId1008" display="https://www.geeksforgeeks.org/longest-common-subsequence-dp-4/"/>
-    <hyperlink ref="C451" r:id="rId1009"/>
-    <hyperlink ref="D451" r:id="rId1010" display="https://youtu.be/-zI4mrF2Pb4?si=VagQXphIzNfpH9su"/>
-    <hyperlink ref="E451" r:id="rId1011" display="https://www.geeksforgeeks.org/printing-longest-common-subsequence/"/>
-    <hyperlink ref="C452" r:id="rId1012"/>
-    <hyperlink ref="D452" r:id="rId1013" display="https://youtu.be/6i_T5kkfv4A?si=7PcZQtgR9bGjBbl4"/>
-    <hyperlink ref="E452" r:id="rId1014" display="https://www.geeksforgeeks.org/longest-palindromic-subsequence-dp-12/"/>
-    <hyperlink ref="C453" r:id="rId1015"/>
-    <hyperlink ref="D453" r:id="rId1016" display="https://youtu.be/xPBLEj41rFU?si=V9kn1IUGTx3DAlSJ"/>
-    <hyperlink ref="E453" r:id="rId1017" display="https://www.geeksforgeeks.org/minimum-insertions-to-form-a-palindrome-dp-28/"/>
-    <hyperlink ref="C454" r:id="rId1018"/>
-    <hyperlink ref="D454" r:id="rId1019" display="https://youtu.be/yMnH0jrir0Q?si=wz6fbYwdh8tJgOtr"/>
-    <hyperlink ref="E454" r:id="rId1020" display="https://www.geeksforgeeks.org/minimum-number-deletions-insertions-transform-one-string-another/"/>
-    <hyperlink ref="C455" r:id="rId1021"/>
-    <hyperlink ref="D455" r:id="rId1022" display="https://youtu.be/xElxAuBcvsU?si=4dBiTvsaW1LiQ4Qm"/>
-    <hyperlink ref="E455" r:id="rId1023" display="https://www.geeksforgeeks.org/shortest-common-supersequence/"/>
-    <hyperlink ref="C456" r:id="rId1024"/>
-    <hyperlink ref="D456" r:id="rId1025" display="https://youtu.be/_wP9mWNPL5w?si=XyPQqcffZg1cYk6z"/>
-    <hyperlink ref="E456" r:id="rId1026" display="https://www.geeksforgeeks.org/longest-common-subarray-in-the-given-two-arrays/"/>
-    <hyperlink ref="C457" r:id="rId1027"/>
-    <hyperlink ref="D457" r:id="rId1028" display="https://youtu.be/UflHuQj6MVA?si=yUS26OPaaMqlvpcb"/>
-    <hyperlink ref="E457" r:id="rId1029" display="https://www.geeksforgeeks.org/longest-palindromic-substring/"/>
-    <hyperlink ref="C458" r:id="rId1030"/>
-    <hyperlink ref="D458" r:id="rId1031" display="https://youtu.be/ZqG89Z-dKpI?si=E5MPTzZgCWf45VvN"/>
-    <hyperlink ref="E458" r:id="rId1032" display="https://www.geeksforgeeks.org/longest-palindromic-substring/"/>
-    <hyperlink ref="C460" r:id="rId1033"/>
-    <hyperlink ref="D460" r:id="rId1034" display="https://youtu.be/fJaKO8FbDdo?si=SgjrMJO4gsNPV5r6"/>
-    <hyperlink ref="E460" r:id="rId1035" display="https://www.geeksforgeeks.org/edit-distance-dp-5/"/>
-    <hyperlink ref="C461" r:id="rId1036"/>
-    <hyperlink ref="D461" r:id="rId1037" display="https://youtu.be/nVG7eTiD2bY?si=FMMLyM58YqKYxEjh"/>
-    <hyperlink ref="C462" r:id="rId1038"/>
-    <hyperlink ref="D462" r:id="rId1039" display="https://youtu.be/ZmlQ3vgAOMo?si=aqw8ylH5x88-LlJs"/>
-    <hyperlink ref="E462" r:id="rId1040" display="https://www.geeksforgeeks.org/wildcard-pattern-matching/"/>
-    <hyperlink ref="C463" r:id="rId1041"/>
-    <hyperlink ref="D463" r:id="rId1042" display="https://youtu.be/Sx9NNgInc3A?si=BVL4wXtCz9BgZLrL"/>
-    <hyperlink ref="E463" r:id="rId1043" display="https://www.geeksforgeeks.org/length-of-the-longest-valid-substring/"/>
-    <hyperlink ref="C464" r:id="rId1044"/>
-    <hyperlink ref="D464" r:id="rId1045" display="https://youtu.be/Sx9NNgInc3A?si=Hmn5-egLse5GkvIx"/>
-    <hyperlink ref="E464" r:id="rId1046" display="https://www.geeksforgeeks.org/word-break-problem-dp-32/"/>
-    <hyperlink ref="C465" r:id="rId1047"/>
-    <hyperlink ref="E465" r:id="rId1048" display="https://www.geeksforgeeks.org/word-break-problem-dp-32/"/>
-    <hyperlink ref="C466" r:id="rId1049"/>
-    <hyperlink ref="D466" r:id="rId1050" display="https://youtu.be/aPdpJ_RjaXs?si=Ic_4lgafd2xh_odL"/>
-    <hyperlink ref="E466" r:id="rId1051" display="https://www.geeksforgeeks.org/word-wrap-problem-dp-19/"/>
-    <hyperlink ref="C467" r:id="rId1052"/>
-    <hyperlink ref="D467" r:id="rId1053" display="https://youtu.be/3Rw3p9LrgvE?si=WDE8R_TrpBnzAeKL"/>
-    <hyperlink ref="E467" r:id="rId1054" display="https://www.geeksforgeeks.org/find-if-a-string-is-interleaved-of-two-other-strings-dp-33/"/>
-    <hyperlink ref="C469" r:id="rId1055"/>
-    <hyperlink ref="D469" r:id="rId1056" display="https://youtu.be/excAOvwF_Wk?si=e7EyG99KPKityBdF"/>
-    <hyperlink ref="C470" r:id="rId1057"/>
-    <hyperlink ref="D470" r:id="rId1058" display="https://youtu.be/nGJmxkUJQGs?si=_mVvHG8iLKwA95lW"/>
-    <hyperlink ref="C471" r:id="rId1059"/>
-    <hyperlink ref="D471" r:id="rId1060" display="https://youtu.be/-uQGzhYj8BQ?si=FDuxAlLnMWU9e21u"/>
-    <hyperlink ref="C472" r:id="rId1061"/>
-    <hyperlink ref="D472" r:id="rId1062" display="https://youtu.be/IV1dHbk5CDc?si=TILc-BmsGoxTljr-"/>
-    <hyperlink ref="C473" r:id="rId1063"/>
-    <hyperlink ref="D473" r:id="rId1064" display="https://youtu.be/IGIe46xw3YY?si=iUqI6GSSB8BugjDm"/>
-    <hyperlink ref="C474" r:id="rId1065"/>
-    <hyperlink ref="D474" r:id="rId1066" display="https://youtu.be/k4eK-vEmnKg?si=wiaYE8Ioi-K-rSZ0"/>
-    <hyperlink ref="C476" r:id="rId1067"/>
-    <hyperlink ref="D476" r:id="rId1068" display="https://youtu.be/pDCXsbAw5Cg?si=P9UB4sQ8a6vvd2_I"/>
-    <hyperlink ref="E476" r:id="rId1069" display="https://www.geeksforgeeks.org/matrix-chain-multiplication-dp-8/"/>
-    <hyperlink ref="C477" r:id="rId1070"/>
-    <hyperlink ref="D477" r:id="rId1071" display="https://youtu.be/xwomavsC86c?si=IufdXqTfIa1F0V6I"/>
-    <hyperlink ref="E477" r:id="rId1072" display="https://takeuforward.org/data-structure/minimum-cost-to-cut-the-stick-dp-50/"/>
-    <hyperlink ref="C478" r:id="rId1073"/>
-    <hyperlink ref="D478" r:id="rId1074" display="https://youtu.be/Yz4LlDSlkns?si=d7mq5OJwAtvOBAz2"/>
-    <hyperlink ref="E478" r:id="rId1075" display="https://www.geeksforgeeks.org/burst-balloon-to-maximize-coins/"/>
-    <hyperlink ref="C479" r:id="rId1076"/>
-    <hyperlink ref="D479" r:id="rId1077" display="https://youtu.be/MM7fXopgyjw?si=qhNd2faXTK1r5x04"/>
-    <hyperlink ref="E479" r:id="rId1078" display="https://www.geeksforgeeks.org/boolean-parenthesization-problem-dp-37/"/>
-    <hyperlink ref="C480" r:id="rId1079"/>
-    <hyperlink ref="D480" r:id="rId1080" display="https://youtu.be/_H8V5hJUGd0?si=Sxlz-OqRVMjbgwgu"/>
-    <hyperlink ref="E480" r:id="rId1081" display="https://www.geeksforgeeks.org/palindrome-partitioning-dp-17/"/>
-    <hyperlink ref="C481" r:id="rId1082"/>
-    <hyperlink ref="D481" r:id="rId1083" display="https://youtu.be/PhWWJmaKfMc?si=qNDjjLCux8ibRyu-"/>
-    <hyperlink ref="E481" r:id="rId1084" display="https://www.geeksforgeeks.org/maximum-average-sum-partition-array/"/>
-    <hyperlink ref="C482" r:id="rId1085"/>
-    <hyperlink ref="D482" r:id="rId1086" display="https://youtu.be/tOylVCugy9k?si=eDTgv7YFHqvrRGMe"/>
-    <hyperlink ref="E482" r:id="rId1087" display="https://www.geeksforgeeks.org/maximum-size-rectangle-binary-sub-matrix-1s/"/>
-    <hyperlink ref="C483" r:id="rId1088"/>
-    <hyperlink ref="D483" r:id="rId1089" display="https://youtu.be/auS1fynpnjo?si=iq5LsCojilevzhM4"/>
-    <hyperlink ref="D486" r:id="rId1090" display="https://youtu.be/N0Frqx9UlrI?si=4iJkhpOo2ry9QwtQ"/>
-    <hyperlink ref="C487" r:id="rId1091" display="https://www.codingninjas.com/studio/problems/min-heap-implementation_5480527"/>
-    <hyperlink ref="D487" r:id="rId1092" display="https://youtu.be/cuL8gXCSA58?si=LkYy8KbCthuzly5l"/>
-    <hyperlink ref="E487" r:id="rId1093" display="https://www.geeksforgeeks.org/introduction-to-min-heap-data-structure/"/>
-    <hyperlink ref="C488" r:id="rId1094"/>
-    <hyperlink ref="D488" r:id="rId1095" display="https://youtu.be/cuL8gXCSA58?si=uWFN4dlnEnzdzQtq"/>
-    <hyperlink ref="E488" r:id="rId1096" display="https://www.geeksforgeeks.org/introduction-to-max-heap-data-structure/"/>
-    <hyperlink ref="C489" r:id="rId1097"/>
-    <hyperlink ref="D489" r:id="rId1098" display="https://youtu.be/cuL8gXCSA58?si=eC60B9JXzRSI_yFt"/>
-    <hyperlink ref="E489" r:id="rId1099" display="https://www.geeksforgeeks.org/convert-min-heap-to-max-heap/"/>
-    <hyperlink ref="C491" r:id="rId1100"/>
-    <hyperlink ref="D491" r:id="rId1101" display="https://youtu.be/aXJ-p3Qa4TY?si=eWjySsOqZUjCCwBP"/>
-    <hyperlink ref="E491" r:id="rId1102" display="https://www.geeksforgeeks.org/kth-smallest-largest-element-in-unsorted-array/"/>
-    <hyperlink ref="D492" r:id="rId1103" display="https://youtu.be/aXJ-p3Qa4TY?si=oPUFQfZaeFc3tOd_"/>
-    <hyperlink ref="C493" r:id="rId1104"/>
-    <hyperlink ref="D493" r:id="rId1105" display="https://youtu.be/Wh3A29psE_Y?si=X6AP6AiuXpjrM79V"/>
-    <hyperlink ref="C494" r:id="rId1106"/>
-    <hyperlink ref="D494" r:id="rId1107" display="https://youtu.be/YPTqKIgVk-k?si=HGG49q2YPTg-ke_v"/>
-    <hyperlink ref="C495" r:id="rId1108"/>
-    <hyperlink ref="D495" r:id="rId1109" display="https://youtu.be/vltY5jxqcco?si=ZHg-JUnHMX2FgvRM"/>
-    <hyperlink ref="C496" r:id="rId1110"/>
-    <hyperlink ref="D496" r:id="rId1111" display="https://youtu.be/hOjcdrqMoQ8?si=RklRakI8BwOIfYwb"/>
-    <hyperlink ref="E496" r:id="rId1112" display="https://www.geeksforgeeks.org/kth-largest-element-in-a-stream/"/>
-    <hyperlink ref="C497" r:id="rId1113"/>
-    <hyperlink ref="D497" r:id="rId1114" display="https://youtu.be/2g_b1aYTHeg?si=yHEmKdbQDc-C-Li9"/>
-    <hyperlink ref="C498" r:id="rId1115"/>
-    <hyperlink ref="D498" r:id="rId1116" display="https://www.youtube.com/live/C3YCL18cIHM?si=YPvoeHFRgzdCx35n"/>
-    <hyperlink ref="C499" r:id="rId1117"/>
-    <hyperlink ref="C500" r:id="rId1118"/>
-    <hyperlink ref="E500" r:id="rId1119" display="https://youtu.be/X5SuOsIWCoI?si=WH6z4uaMzE8B_UOK"/>
-    <hyperlink ref="C502" r:id="rId1120"/>
-    <hyperlink ref="D502" r:id="rId1121" display="https://youtu.be/kpCesr9VXDA?si=UyD8orvz_UXvSQhl"/>
-    <hyperlink ref="E502" r:id="rId1122" display="https://www.geeksforgeeks.org/merge-k-sorted-arrays/"/>
-    <hyperlink ref="C503" r:id="rId1123"/>
-    <hyperlink ref="C504" r:id="rId1124"/>
-    <hyperlink ref="C506" r:id="rId1125"/>
-    <hyperlink ref="D506" r:id="rId1126" display="https://youtu.be/itmhHWaHupI?si=kOhqNsy0u87ew1gQ"/>
-    <hyperlink ref="E506" r:id="rId1127" display="https://www.geeksforgeeks.org/median-of-stream-of-integers-running-integers/"/>
-    <hyperlink ref="C507" r:id="rId1128"/>
-    <hyperlink ref="D507" r:id="rId1129" display="https://youtu.be/DfljaUwZsOk?si=ATC7K2_3a6QPXdsS"/>
-    <hyperlink ref="C508" r:id="rId1130"/>
-    <hyperlink ref="C510" r:id="rId1131"/>
-    <hyperlink ref="D510" r:id="rId1132" display="https://youtu.be/f7JOBJIC-NA?si=qACVSM1NauAdTfmG"/>
-    <hyperlink ref="E510" r:id="rId1133" display="https://www.geeksforgeeks.org/connect-n-ropes-minimum-cost/"/>
-    <hyperlink ref="C511" r:id="rId1134"/>
-    <hyperlink ref="D511" r:id="rId1135" display="https://youtu.be/FdzJmTCVyJU?si=I_7q86O10M1_5nTy"/>
-    <hyperlink ref="E511" r:id="rId1136" display="https://www.geeksforgeeks.org/find-maximum-meetings-in-one-room/"/>
-    <hyperlink ref="C512" r:id="rId1137"/>
-    <hyperlink ref="D512" r:id="rId1138" display="https://youtu.be/IbhQ3U5NHLI?si=PSp_XzWTzv4wQ57W"/>
-    <hyperlink ref="E512" r:id="rId1139" display="https://www.geeksforgeeks.org/minimum-cost-to-complete-given-tasks-if-cost-of-1-7-and-30-days-are-given/"/>
-    <hyperlink ref="C513" r:id="rId1140"/>
-    <hyperlink ref="E513" r:id="rId1141" display="https://www.geeksforgeeks.org/minimum-cost-to-process-m-tasks-where-switching-costs/"/>
-    <hyperlink ref="C514" r:id="rId1142"/>
-    <hyperlink ref="D514" r:id="rId1143" display="https://youtu.be/sKjKLN5JswQ?si=kF07TsHuwP_jmuzh"/>
-    <hyperlink ref="E514" r:id="rId1144" display="https://www.geeksforgeeks.org/minimize-refills-to-reach-end-of-path/"/>
-    <hyperlink ref="C517" r:id="rId1145"/>
-    <hyperlink ref="D517" r:id="rId1146" display="https://youtu.be/oobqoCJlHA0?si=HTMe5ROchxy4KAaU"/>
-    <hyperlink ref="E517" r:id="rId1147" display="https://www.geeksforgeeks.org/trie-insert-and-search/"/>
-    <hyperlink ref="C518" r:id="rId1148" display="https://www.geeksforgeeks.org/problems/word-break-trie--141631/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D518" r:id="rId1149" display="https://youtu.be/th4OnoGasMU?si=r6--sa8rf-0P2Hc0"/>
-    <hyperlink ref="E518" r:id="rId1150" display="https://www.geeksforgeeks.org/word-break-problem-trie-solution/"/>
-    <hyperlink ref="C519" r:id="rId1151"/>
-    <hyperlink ref="D519" r:id="rId1152" display="https://youtu.be/fhyIORFDD0k?si=llRsS8TY44gkz9s6"/>
-    <hyperlink ref="E519" r:id="rId1153" display="https://www.geeksforgeeks.org/longest-common-prefix-using-sorting/"/>
-    <hyperlink ref="C520" r:id="rId1154" display="https://www.geeksforgeeks.org/problems/maximum-xor-of-two-numbers-in-an-array/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D520" r:id="rId1155" display="https://youtu.be/jCuZCbXnpLo?si=bjswCkTxSANJnuQj"/>
-    <hyperlink ref="E520" r:id="rId1156" display="https://www.geeksforgeeks.org/maximum-xor-of-two-numbers-in-an-array/"/>
-    <hyperlink ref="C521" r:id="rId1157" display="https://www.geeksforgeeks.org/problems/unique-rows-in-boolean-matrix/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D521" r:id="rId1158" display="https://youtu.be/GixyVinjtFk?si=7THXd_L892zgFeIw"/>
-    <hyperlink ref="E521" r:id="rId1159" display="https://www.geeksforgeeks.org/print-unique-rows/"/>
-    <hyperlink ref="C522" r:id="rId1160"/>
-    <hyperlink ref="D522" r:id="rId1161" display="https://www.youtube.com/live/bs4MqQ_0ZS0?si=Xgos1T5uEzHu__1a"/>
-    <hyperlink ref="E522" r:id="rId1162" display="https://www.geeksforgeeks.org/count-of-strings-whose-prefix-match-with-the-given-string-to-a-given-length-k/"/>
-    <hyperlink ref="C525" r:id="rId1163"/>
-    <hyperlink ref="D525" r:id="rId1164" display="https://youtu.be/2I9XO8jwZCA?si=ldC-gp4Wv4Gra1z7"/>
-    <hyperlink ref="E525" r:id="rId1165" display="https://www.geeksforgeeks.org/write-your-own-atoi/"/>
-    <hyperlink ref="C526" r:id="rId1166"/>
-    <hyperlink ref="E526" r:id="rId1167" display="https://www.geeksforgeeks.org/look-and-say-sequence/"/>
-    <hyperlink ref="C527" r:id="rId1168" display="https://www.geeksforgeeks.org/problems/count-the-reversals0401/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D527" r:id="rId1169" display="https://youtu.be/8q1sma-qMsA?si=22qpLT56elmIfBgl"/>
-    <hyperlink ref="E527" r:id="rId1170" display="https://www.geeksforgeeks.org/minimum-number-of-bracket-reversals-needed-to-make-an-expression-balanced/"/>
-    <hyperlink ref="C528" r:id="rId1171"/>
-    <hyperlink ref="D528" r:id="rId1172" display="https://youtu.be/oxd_Z1osgCk?si=kxhwCfdV3t6M0IHB"/>
-    <hyperlink ref="E528" r:id="rId1173" display="https://www.geeksforgeeks.org/rabin-karp-algorithm-for-pattern-searching/"/>
-    <hyperlink ref="C529" r:id="rId1174"/>
-    <hyperlink ref="E529" r:id="rId1175" display="https://www.geeksforgeeks.org/boyer-moore-algorithm-for-pattern-searching/"/>
-    <hyperlink ref="C530" r:id="rId1176"/>
-    <hyperlink ref="D530" r:id="rId1177" display="https://youtu.be/ziteu2FpYsA?si=iLKlrPrn4Qn1Pl3G"/>
-    <hyperlink ref="E530" r:id="rId1178" display="https://www.geeksforgeeks.org/longest-prefix-also-suffix/"/>
-    <hyperlink ref="C531" r:id="rId1179"/>
-    <hyperlink ref="E531" r:id="rId1180" display="https://www.geeksforgeeks.org/longest-prefix-also-suffix/"/>
-    <hyperlink ref="C532" r:id="rId1181"/>
-    <hyperlink ref="D532" r:id="rId1182" display="https://youtu.be/w6LcypDgC4w?si=q2BwgPUVgXvVBs5K"/>
-    <hyperlink ref="E532" r:id="rId1183" display="https://www.geeksforgeeks.org/recursively-remove-adjacent-duplicates-given-string/"/>
-    <hyperlink ref="C533" r:id="rId1184"/>
-    <hyperlink ref="D533" r:id="rId1185" display="https://youtu.be/KEs5UyBJ39g?si=9hG4JdZkDb_a1sju"/>
-    <hyperlink ref="E533" r:id="rId1186" display="https://www.geeksforgeeks.org/string-hashing-using-polynomial-rolling-hash-function/"/>
-    <hyperlink ref="C534" r:id="rId1187"/>
-    <hyperlink ref="D534" r:id="rId1188" display="https://youtu.be/vzdNOK2oB2E?si=jgGJngudIz4L_4oP"/>
-    <hyperlink ref="E534" r:id="rId1189" display="https://www.geeksforgeeks.org/given-a-sequence-of-words-print-all-anagrams-together/"/>
-    <hyperlink ref="C535" r:id="rId1190"/>
-    <hyperlink ref="D535" r:id="rId1191" display="https://www.youtube.com/live/-1qq3hekxBw?si=zOa8LDear3iIsWRl"/>
-    <hyperlink ref="E535" r:id="rId1192" display="https://www.geeksforgeeks.org/z-algorithm-linear-time-pattern-searching-algorithm/"/>
-    <hyperlink ref="C536" r:id="rId1193" display="https://leetcode.com/problems/shortest-palindrome/"/>
-    <hyperlink ref="D536" r:id="rId1194" display="https://youtu.be/xPBLEj41rFU?si=04dcB7ymKkMft7VE"/>
-    <hyperlink ref="E536" r:id="rId1195" display="https://www.geeksforgeeks.org/minimum-insertions-to-form-shortest-palindrome/"/>
-    <hyperlink ref="C537" r:id="rId1196"/>
-    <hyperlink ref="D537" r:id="rId1197" display="https://youtu.be/DBcbRXAlE0U?si=Nm16p-kL_VVEuAAY"/>
-    <hyperlink ref="E537" r:id="rId1198" display="https://www.geeksforgeeks.org/given-array-strings-find-strings-can-chained-form-circle/"/>
-    <hyperlink ref="C538" r:id="rId1199" display="https://www.geeksforgeeks.org/problems/roman-number-to-integer3201/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
-    <hyperlink ref="D538" r:id="rId1200" display="https://youtu.be/dlATMslQ6Uc?si=ImmwMRmjbHD-umKR"/>
-    <hyperlink ref="E538" r:id="rId1201" display="https://www.geeksforgeeks.org/converting-roman-numerals-decimal-lying-1-3999/"/>
-    <hyperlink ref="B544" r:id="rId1202"/>
-    <hyperlink ref="B545" r:id="rId1203"/>
-    <hyperlink ref="B546" r:id="rId1204" display="https://www.overleaf.com/articles/ravi-kukretis-resume/cxprrkxbccgb"/>
+    <hyperlink ref="D34" r:id="rId41" display="https://youtu.be/37E9ckMDdTk?si=0TR032zkFFRqHymE"/>
+    <hyperlink ref="E34" r:id="rId42" display="https://www.geeksforgeeks.org/maximum-and-minimum-in-an-array/"/>
+    <hyperlink ref="C35" r:id="rId43"/>
+    <hyperlink ref="D35" r:id="rId44" display="https://youtu.be/37E9ckMDdTk?si=0TR032zkFFRqHymE"/>
+    <hyperlink ref="E35" r:id="rId45" display="https://www.geeksforgeeks.org/third-largest-element-array-distinct-elements/"/>
+    <hyperlink ref="C36" r:id="rId46"/>
+    <hyperlink ref="D36" r:id="rId47" display="https://youtu.be/wvcQg43_V8U?si=duJ5xqerLGj0IR7R"/>
+    <hyperlink ref="E36" r:id="rId48" display="https://www.geeksforgeeks.org/c-program-to-traverse-an-array/"/>
+    <hyperlink ref="C37" r:id="rId49"/>
+    <hyperlink ref="D37" r:id="rId50" display="https://youtu.be/2D0D8HE6uak?si=HL1gv_qVc7mUaHoJ"/>
+    <hyperlink ref="E37" r:id="rId51" display="https://www.geeksforgeeks.org/find-the-missing-number/"/>
+    <hyperlink ref="D38" r:id="rId52" display="https://youtu.be/2D0D8HE6uak?si=HL1gv_qVc7mUaHoJ"/>
+    <hyperlink ref="C39" r:id="rId53" display="https://www.geeksforgeeks.org/problems/sort-an-array-of-0s-1s-and-2s4231/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D39" r:id="rId54" display="https://youtu.be/tp8JIuCXBaU?si=8iicmWUzbNMzAapK"/>
+    <hyperlink ref="E39" r:id="rId55" display="https://www.geeksforgeeks.org/sort-an-array-of-0s-1s-and-2s/"/>
+    <hyperlink ref="C40" r:id="rId56" display="https://www.geeksforgeeks.org/problems/check-if-two-arrays-are-equal-or-not3847/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="E40" r:id="rId57" display="https://www.geeksforgeeks.org/check-if-two-arrays-are-equal-or-not/"/>
+    <hyperlink ref="C41" r:id="rId58" display="https://www.geeksforgeeks.org/problems/cyclically-rotate-an-array-by-one2614/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D41" r:id="rId59" display="https://youtu.be/BHr381Guz3Y?si=LxSVwsQemuIvjvdu"/>
+    <hyperlink ref="E41" r:id="rId60" display="https://www.geeksforgeeks.org/c-program-cyclically-rotate-array-one/"/>
+    <hyperlink ref="C42" r:id="rId61"/>
+    <hyperlink ref="D42" r:id="rId62" display="https://youtu.be/wvcQg43_V8U?si=sd6dy_KO9X1yvwQY"/>
+    <hyperlink ref="E42" r:id="rId63" display="https://www.geeksforgeeks.org/print-array-after-it-is-right-rotated-k-times/"/>
+    <hyperlink ref="C43" r:id="rId64"/>
+    <hyperlink ref="E43" r:id="rId65" display="https://www.geeksforgeeks.org/find-whether-an-array-is-subset-of-another-array-set-1/"/>
+    <hyperlink ref="D44" r:id="rId66" display="https://youtu.be/KEs5UyBJ39g?si=RVR7_pJUEOH4dlUZ"/>
+    <hyperlink ref="E44" r:id="rId67" display="https://www.geeksforgeeks.org/introduction-to-map-data-structure-and-algorithm-tutorials/"/>
+    <hyperlink ref="C45" r:id="rId68"/>
+    <hyperlink ref="E45" r:id="rId69" display="https://www.geeksforgeeks.org/counting-frequencies-of-array-elements/"/>
+    <hyperlink ref="C47" r:id="rId70" display="https://www.geeksforgeeks.org/problems/key-pair5616/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D47" r:id="rId71" display="https://youtu.be/UXDSeD9mN-k?si=0OalQrKPSoSeO6io"/>
+    <hyperlink ref="E47" r:id="rId72" display="https://www.geeksforgeeks.org/check-if-pair-with-given-sum-exists-in-array/"/>
+    <hyperlink ref="C48" r:id="rId73" display="https://www.geeksforgeeks.org/problems/triplet-sum-in-array-1587115621/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D48" r:id="rId74" display="https://youtu.be/DhFh8Kw7ymk?si=Fwh27YWXIuwurZjz"/>
+    <hyperlink ref="E48" r:id="rId75" display="https://www.geeksforgeeks.org/find-a-triplet-that-sum-to-a-given-value/"/>
+    <hyperlink ref="C49" r:id="rId76"/>
+    <hyperlink ref="D49" r:id="rId77" display="https://youtu.be/eD95WRfh81c?si=01Uliqaf14HWboWE"/>
+    <hyperlink ref="E49" r:id="rId78" display="https://www.geeksforgeeks.org/find-four-elements-that-sum-to-a-given-value-set-2/"/>
+    <hyperlink ref="C50" r:id="rId79"/>
+    <hyperlink ref="D50" r:id="rId80" display="https://youtu.be/cJlJwroDw6o?si=UzoMg7WQXEX_-nQL"/>
+    <hyperlink ref="E50" r:id="rId81" display="https://www.geeksforgeeks.org/find-triplets-array-whose-sum-equal-zero/"/>
+    <hyperlink ref="C51" r:id="rId82" display="https://practice.geeksforgeeks.org/problems/count-the-triplets4615/1"/>
+    <hyperlink ref="D51" r:id="rId83" display="https://youtu.be/jqI7kKIJVF8?si=tN1E706NtO33ZE29"/>
+    <hyperlink ref="E51" r:id="rId84" display="https://www.geeksforgeeks.org/count-triplets-such-that-one-of-the-numbers-can-be-written-as-sum-of-the-other-two/"/>
+    <hyperlink ref="C52" r:id="rId85"/>
+    <hyperlink ref="D52" r:id="rId86" display="https://youtu.be/wvcQg43_V8U?si=sd6dy_KO9X1yvwQY"/>
+    <hyperlink ref="E52" r:id="rId87" display="https://www.geeksforgeeks.org/find-union-and-intersection-of-two-unsorted-arrays/"/>
+    <hyperlink ref="C53" r:id="rId88" display="https://www.geeksforgeeks.org/problems/intersection-of-two-arrays2404/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D53" r:id="rId89" display="https://youtu.be/wvcQg43_V8U?si=sd6dy_KO9X1yvwQY"/>
+    <hyperlink ref="E53" r:id="rId90" display="https://www.geeksforgeeks.org/find-union-and-intersection-of-two-unsorted-arrays/"/>
+    <hyperlink ref="C54" r:id="rId91" display="https://www.geeksforgeeks.org/problems/remove-duplicate-elements-from-sorted-array/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D54" r:id="rId92" display="https://youtu.be/37E9ckMDdTk?si=sgQG1IPqP4_lMLI7"/>
+    <hyperlink ref="E54" r:id="rId93" display="https://www.geeksforgeeks.org/remove-duplicates-sorted-array/"/>
+    <hyperlink ref="C55" r:id="rId94" display="https://www.geeksforgeeks.org/problems/k-th-element-of-two-sorted-array1317/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="E55" r:id="rId95" display="https://www.geeksforgeeks.org/k-th-element-two-sorted-arrays/"/>
+    <hyperlink ref="C56" r:id="rId96"/>
+    <hyperlink ref="D56" r:id="rId97" display="https://youtu.be/frf7qxiN2qU?si=JPQuhDD95ggmdzkh"/>
+    <hyperlink ref="E56" r:id="rId98" display="https://www.geeksforgeeks.org/length-of-longest-subarray-with-increasing-contiguous-elements/"/>
+    <hyperlink ref="C57" r:id="rId99" display="https://www.geeksforgeeks.org/problems/trapping-rain-water-1587115621/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D57" r:id="rId100" display="https://youtu.be/m18Hntz4go8?si=ciSWVbyZK9fRqwlD"/>
+    <hyperlink ref="E57" r:id="rId101" display="https://www.geeksforgeeks.org/trapping-rain-water/"/>
+    <hyperlink ref="C59" r:id="rId102"/>
+    <hyperlink ref="D59" r:id="rId103" display="https://youtu.be/nP_ns3uSh80?si=7StWyumzZ4xALf_n"/>
+    <hyperlink ref="E59" r:id="rId104" display="https://www.geeksforgeeks.org/majority-element/"/>
+    <hyperlink ref="C60" r:id="rId105"/>
+    <hyperlink ref="D60" r:id="rId106" display="https://youtu.be/AHZpyENo7k4?si=Gedgrb5NcCsKTvpr"/>
+    <hyperlink ref="E60" r:id="rId107" display="https://www.geeksforgeeks.org/largest-sum-contiguous-subarray/"/>
+    <hyperlink ref="C61" r:id="rId108"/>
+    <hyperlink ref="D61" r:id="rId109" display="https://youtu.be/AseUmwVNaoY?si=ryexsr9Pkd2oEqLb"/>
+    <hyperlink ref="E61" r:id="rId110" display="https://www.geeksforgeeks.org/inversion-count-in-array-using-merge-sort/"/>
+    <hyperlink ref="C62" r:id="rId111"/>
+    <hyperlink ref="D62" r:id="rId112" display="https://youtu.be/IexN60k62jo?si=fTYDjb_XUvQNSMQK"/>
+    <hyperlink ref="E62" r:id="rId113" display="https://www.geeksforgeeks.org/merging-intervals/"/>
+    <hyperlink ref="C63" r:id="rId114"/>
+    <hyperlink ref="D63" r:id="rId115" display="https://youtu.be/hnswaLJvr6g?si=dsjYUnsya81zUUoU"/>
+    <hyperlink ref="E63" r:id="rId116" display="https://www.geeksforgeeks.org/maximum-product-subarray/"/>
+    <hyperlink ref="C64" r:id="rId117"/>
+    <hyperlink ref="D64" r:id="rId118" display="https://youtu.be/JDOXKqF60RQ?si=N0kQyEkb3HU3cAFN"/>
+    <hyperlink ref="E64" r:id="rId119" display="https://www.geeksforgeeks.org/next-permutation/"/>
+    <hyperlink ref="C65" r:id="rId120"/>
+    <hyperlink ref="D65" r:id="rId121" display="https://youtu.be/QDFM7Mjk2mc?si=N-KRLLlVPFDbP7ig"/>
+    <hyperlink ref="E65" r:id="rId122" display="https://www.geeksforgeeks.org/sieve-of-eratosthenes/"/>
+    <hyperlink ref="B66" r:id="rId123" display="https://youtu.be/FPu9Uld7W-E?si=s_d6cjdb6UtlVg16"/>
+    <hyperlink ref="D69" r:id="rId124" display="https://youtu.be/J1aQ9JN4vZY?si=Zyvvj50RIqnHS_dI"/>
+    <hyperlink ref="E69" r:id="rId125" display="https://www.geeksforgeeks.org/multidimensional-arrays-in-c/"/>
+    <hyperlink ref="C70" r:id="rId126"/>
+    <hyperlink ref="D70" r:id="rId127" display="https://youtu.be/JXU4Akft7yk?si=ftzaCZifMOyqSHYd"/>
+    <hyperlink ref="E70" r:id="rId128" display="https://www.geeksforgeeks.org/search-element-sorted-matrix/"/>
+    <hyperlink ref="C71" r:id="rId129"/>
+    <hyperlink ref="D71" r:id="rId130" display="https://youtu.be/Z0R2u6gd3GU?si=09YatNJUpyE7ZCjg"/>
+    <hyperlink ref="E71" r:id="rId131" display="https://www.geeksforgeeks.org/rotate-a-matrix-by-90-degree-in-clockwise-direction-without-using-any-extra-space/"/>
+    <hyperlink ref="C72" r:id="rId132" display="https://www.geeksforgeeks.org/problems/row-with-minimum-number-of-1s5430/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D72" r:id="rId133" display="https://youtu.be/SCz-1TtYxDI?si=XeAz7btJ6r2MbZuh"/>
+    <hyperlink ref="E72" r:id="rId134" display="https://www.geeksforgeeks.org/find-the-row-with-maximum-number-1s/"/>
+    <hyperlink ref="C73" r:id="rId135"/>
+    <hyperlink ref="D73" r:id="rId136" display="https://youtu.be/Z0R2u6gd3GU?si=7sxqBk_sUWTCigqc"/>
+    <hyperlink ref="E73" r:id="rId137" display="https://www.geeksforgeeks.org/rotate-matrix-right-k-times/"/>
+    <hyperlink ref="C74" r:id="rId138" display="https://www.geeksforgeeks.org/problems/print-matrix-in-diagonal-pattern/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="E74" r:id="rId139" display="https://www.geeksforgeeks.org/print-matrix-diagonal-pattern/"/>
+    <hyperlink ref="C75" r:id="rId140"/>
+    <hyperlink ref="D75" r:id="rId141" display="https://youtu.be/N0MgLvceX7M?si=jJ_jUtmeE5mb0LB0"/>
+    <hyperlink ref="E75" r:id="rId142" display="https://takeuforward.org/data-structure/set-matrix-zero/"/>
+    <hyperlink ref="D77" r:id="rId143" display="https://youtu.be/yVdKa8dnKiE?si=SRrnZral-975-l3T"/>
+    <hyperlink ref="E77" r:id="rId144" display="https://www.geeksforgeeks.org/how-to-solve-time-complexity-recurrence-relations-using-recursion-tree-method/"/>
+    <hyperlink ref="C78" r:id="rId145"/>
+    <hyperlink ref="D78" r:id="rId146" display="https://youtu.be/un6PLygfXrA?si=lTiOfyUrTigDKJuT"/>
+    <hyperlink ref="E78" r:id="rId147" display="https://takeuforward.org/data-structure/print-n-to-1-and-1-to-n-using-recursion/"/>
+    <hyperlink ref="C79" r:id="rId148"/>
+    <hyperlink ref="D79" r:id="rId149" display="https://youtu.be/69ZCDFy-OUo?si=ZSOqIZK0c4L27ad2"/>
+    <hyperlink ref="E79" r:id="rId150" display="https://www.geeksforgeeks.org/program-for-factorial-of-a-number/"/>
+    <hyperlink ref="C80" r:id="rId151" display="https://www.geeksforgeeks.org/problems/nth-fibonacci-number1335/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D80" r:id="rId152" display="https://youtu.be/kvRjNm4rVBE?si=HoIm_q77BpGtePSF"/>
+    <hyperlink ref="E80" r:id="rId153" display="https://www.geeksforgeeks.org/program-for-nth-fibonacci-number/"/>
+    <hyperlink ref="C81" r:id="rId154" display="https://www.geeksforgeeks.org/problems/power-of-numbers-1587115620/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D81" r:id="rId155" display="https://youtu.be/l0YC3876qxg?si=gpooiy_1Voz_M2b6"/>
+    <hyperlink ref="E81" r:id="rId156" display="https://www.geeksforgeeks.org/write-a-c-program-to-calculate-powxn/"/>
+    <hyperlink ref="C82" r:id="rId157"/>
+    <hyperlink ref="D82" r:id="rId158" display="https://youtu.be/tNm_NNSB3_w?si=qRueLOLTmrBAtTTC"/>
+    <hyperlink ref="E82" r:id="rId159" display="https://www.geeksforgeeks.org/c-programs-print-interesting-patterns/"/>
+    <hyperlink ref="C83" r:id="rId160" display="https://practice.geeksforgeeks.org/problems/implement-atoi/1?utm_source=geeksforgeeks&amp;utm_medium=ml_article_practice_tab&amp;utm_campaign=article_practice_tab"/>
+    <hyperlink ref="D83" r:id="rId161" display="https://youtu.be/cXf7NKgT13s?si=7CiE2Yq4IRTwI3vh"/>
+    <hyperlink ref="E83" r:id="rId162" display="https://www.geeksforgeeks.org/recursive-implementation-of-atoi/"/>
+    <hyperlink ref="C84" r:id="rId163"/>
+    <hyperlink ref="D84" r:id="rId164" display="https://youtu.be/bR7mQgwQ_o8?si=sqnpPOV603FTpnTr"/>
+    <hyperlink ref="E84" r:id="rId165" display="https://www.geeksforgeeks.org/pascal-triangle/"/>
+    <hyperlink ref="C87" r:id="rId166"/>
+    <hyperlink ref="D87" r:id="rId167" display="https://youtu.be/MHf6awe89xw?si=SZFA7hgK2TgcOc0p"/>
+    <hyperlink ref="E87" r:id="rId168" display="https://www.geeksforgeeks.org/search-an-element-in-a-sorted-and-pivoted-array/"/>
+    <hyperlink ref="C88" r:id="rId169"/>
+    <hyperlink ref="D88" r:id="rId170" display="https://youtu.be/6zhGS79oQ4k?si=HTYRycV3VAbAV7wJ"/>
+    <hyperlink ref="E88" r:id="rId171" display="https://takeuforward.org/arrays/floor-and-ceil-in-sorted-array/"/>
+    <hyperlink ref="C89" r:id="rId172"/>
+    <hyperlink ref="D89" r:id="rId173" display="https://youtu.be/hjR1IYVx9lY?si=LvMcs8L77aY4RPsP"/>
+    <hyperlink ref="E89" r:id="rId174" display="https://www.geeksforgeeks.org/search-an-element-in-a-sorted-and-pivoted-array/"/>
+    <hyperlink ref="C90" r:id="rId175"/>
+    <hyperlink ref="D90" r:id="rId176" display="https://youtu.be/2D0D8HE6uak?si=lL-NPH7ot2zCdWFk"/>
+    <hyperlink ref="E90" r:id="rId177" display="https://www.geeksforgeeks.org/find-the-missing-number/"/>
+    <hyperlink ref="C91" r:id="rId178" display="https://www.geeksforgeeks.org/problems/square-root/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D91" r:id="rId179" display="https://youtu.be/Bsv3FPUX_BA?si=pkOV3citxe_BydNv"/>
+    <hyperlink ref="E91" r:id="rId180" display="https://www.geeksforgeeks.org/square-root-of-an-integer/"/>
+    <hyperlink ref="C92" r:id="rId181"/>
+    <hyperlink ref="D92" r:id="rId182" display="https://youtu.be/W9QJ8HaRvJQ?si=7qkUdUy7sHugcc-4"/>
+    <hyperlink ref="E92" r:id="rId183" display="https://takeuforward.org/data-structure/search-in-an-infinite-sorted-array/"/>
+    <hyperlink ref="C94" r:id="rId184"/>
+    <hyperlink ref="D94" r:id="rId185" display="https://youtu.be/5qGrJbHhqFs?si=BQOhDElObCoMlfNF"/>
+    <hyperlink ref="E94" r:id="rId186" display="https://www.geeksforgeeks.org/search-an-element-in-a-sorted-and-rotated-array-with-duplicates/"/>
+    <hyperlink ref="C95" r:id="rId187"/>
+    <hyperlink ref="D95" r:id="rId188" display="https://youtu.be/nhEMDKMB44g?si=oulPpoG2QvlG0YgL"/>
+    <hyperlink ref="E95" r:id="rId189" display="https://www.geeksforgeeks.org/find-minimum-element-in-a-sorted-and-rotated-array/"/>
+    <hyperlink ref="C96" r:id="rId190" display="https://www.geeksforgeeks.org/problems/rotation4723/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D96" r:id="rId191" display="https://youtu.be/jtSiWTPLwd0?si=-rI5dZ-3sY3qDsS6"/>
+    <hyperlink ref="E96" r:id="rId192" display="https://www.geeksforgeeks.org/find-rotation-count-rotated-sorted-array/"/>
+    <hyperlink ref="E97" r:id="rId193" display="https://www.geeksforgeeks.org/maximum-element-in-a-sorted-and-rotated-array/"/>
+    <hyperlink ref="C99" r:id="rId194"/>
+    <hyperlink ref="D99" r:id="rId195" display="https://youtu.be/cXxmbemS6XM?si=uuZ5GDVRhz1DuRpp"/>
+    <hyperlink ref="E99" r:id="rId196" display="https://www.geeksforgeeks.org/find-a-peak-in-a-given-array/"/>
+    <hyperlink ref="C100" r:id="rId197"/>
+    <hyperlink ref="D100" r:id="rId198" display="https://youtu.be/W9QJ8HaRvJQ?si=7qkUdUy7sHugcc-4"/>
+    <hyperlink ref="E100" r:id="rId199" display="https://www.geeksforgeeks.org/find-element-bitonic-array/"/>
+    <hyperlink ref="C102" r:id="rId200"/>
+    <hyperlink ref="D102" r:id="rId201" display="https://youtu.be/SCz-1TtYxDI?si=U_jEDIFYaa8QGnxo"/>
+    <hyperlink ref="E102" r:id="rId202" display="https://www.geeksforgeeks.org/find-the-row-with-maximum-number-1s/"/>
+    <hyperlink ref="C103" r:id="rId203" display="https://www.geeksforgeeks.org/problems/search-in-a-matrix-1587115621/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D103" r:id="rId204" display="https://youtu.be/JXU4Akft7yk?si=oY5y29BNgKveTd7q"/>
+    <hyperlink ref="E103" r:id="rId205" display="https://www.geeksforgeeks.org/search-in-row-wise-and-column-wise-sorted-matrix/"/>
+    <hyperlink ref="C104" r:id="rId206"/>
+    <hyperlink ref="D104" r:id="rId207" display="https://youtu.be/9ZbB397jU4k?si=LYzHu6tpjUc5D73I"/>
+    <hyperlink ref="E104" r:id="rId208" display="https://www.geeksforgeeks.org/search-in-a-sorted-2d-matrix-stored-in-row-major-order/"/>
+    <hyperlink ref="C105" r:id="rId209"/>
+    <hyperlink ref="D105" r:id="rId210" display="https://youtu.be/9ZbB397jU4k?si=wSh6BEJiQjJRFuhD"/>
+    <hyperlink ref="E105" r:id="rId211" display="https://www.geeksforgeeks.org/find-peak-element-2d-array/"/>
+    <hyperlink ref="C107" r:id="rId212"/>
+    <hyperlink ref="D107" r:id="rId213" display="https://youtu.be/R_Mfw4ew-Vo?si=5YexrvejL-U8Lp9e"/>
+    <hyperlink ref="E107" r:id="rId214" display="https://www.geeksforgeeks.org/assign-stalls-to-k-cows-to-maximize-the-minimum-distance-between-them/"/>
+    <hyperlink ref="C108" r:id="rId215" display="https://www.geeksforgeeks.org/problems/allocate-minimum-number-of-pages0937/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D108" r:id="rId216" display="https://youtu.be/Z0hwjftStI4?si=md6pnkK1gK2OydeX"/>
+    <hyperlink ref="E108" r:id="rId217" display="https://www.geeksforgeeks.org/allocate-minimum-number-pages/"/>
+    <hyperlink ref="C109" r:id="rId218"/>
+    <hyperlink ref="D109" r:id="rId219" display="https://youtu.be/thUd_WJn6wk?si=83_t-BSmFO1JPtFX"/>
+    <hyperlink ref="E109" r:id="rId220" display="https://www.geeksforgeeks.org/painters-partition-problem/"/>
+    <hyperlink ref="C110" r:id="rId221"/>
+    <hyperlink ref="D110" r:id="rId222" display="https://youtu.be/thUd_WJn6wk?si=83_t-BSmFO1JPtFX"/>
+    <hyperlink ref="E110" r:id="rId223" display="https://www.geeksforgeeks.org/split-the-given-array-into-k-sub-arrays-such-that-maximum-sum-of-all-sub-arrays-is-minimum/"/>
+    <hyperlink ref="C111" r:id="rId224"/>
+    <hyperlink ref="D111" r:id="rId225" display="https://youtu.be/TXAuxeYBTdg?si=am2Vhrx6NzRn666i"/>
+    <hyperlink ref="E111" r:id="rId226" display="https://takeuforward.org/arrays/minimum-days-to-make-m-bouquets/"/>
+    <hyperlink ref="C112" r:id="rId227"/>
+    <hyperlink ref="D112" r:id="rId228" display="https://youtu.be/MG-Ac4TAvTY?si=AZ1NbXoBg0WpOIVu"/>
+    <hyperlink ref="E112" r:id="rId229" display="https://www.geeksforgeeks.org/capacity-to-ship-packages-within-d-days/"/>
+    <hyperlink ref="C113" r:id="rId230"/>
+    <hyperlink ref="D113" r:id="rId231" display="https://youtu.be/qyfekrNni90?si=jMI1EAu9QbNoPwdL"/>
+    <hyperlink ref="E113" r:id="rId232" display="https://www.geeksforgeeks.org/koko-eating-bananas/"/>
+    <hyperlink ref="C114" r:id="rId233"/>
+    <hyperlink ref="D114" r:id="rId234" display="https://youtu.be/N-7biZf7a0I?si=CfkbhxMALJCEo69w"/>
+    <hyperlink ref="E114" r:id="rId235" display="https://www.geeksforgeeks.org/kth-smallest-number-in-multiplication-table/"/>
+    <hyperlink ref="C115" r:id="rId236"/>
+    <hyperlink ref="D115" r:id="rId237" display="https://youtu.be/veu_Q-da6ZY?si=T0MVODyANtV8Q8jE"/>
+    <hyperlink ref="E115" r:id="rId238" display="https://www.geeksforgeeks.org/k-th-smallest-absolute-difference-two-elements-array/"/>
+    <hyperlink ref="C116" r:id="rId239"/>
+    <hyperlink ref="D116" r:id="rId240" display="https://youtu.be/X5SuOsIWCoI?si=EQTTz3FlzY37wihS"/>
+    <hyperlink ref="E116" r:id="rId241" display="https://www.geeksforgeeks.org/ugly-numbers/"/>
+    <hyperlink ref="C117" r:id="rId242" display="https://www.geeksforgeeks.org/problems/median-of-2-sorted-arrays-of-different-sizes/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D117" r:id="rId243" display="https://youtu.be/F9c7LpRZWVQ?si=UBBKqg6vDwaEPBla"/>
+    <hyperlink ref="E117" r:id="rId244" display="https://www.geeksforgeeks.org/median-of-two-sorted-arrays-of-different-sizes/"/>
+    <hyperlink ref="C118" r:id="rId245" display="https://leetcode.com/problems/find-the-smallest-divisor-given-a-threshold/"/>
+    <hyperlink ref="D118" r:id="rId246" display="https://youtu.be/UvBKTVaG6U8?si=U-dfjanJFfqbEEOE"/>
+    <hyperlink ref="E118" r:id="rId247" display="https://takeuforward.org/arrays/find-the-smallest-divisor-given-a-threshold/"/>
+    <hyperlink ref="C120" r:id="rId248" display="https://www.geeksforgeeks.org/problems/bubble-sort/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D120" r:id="rId249" display="https://youtu.be/HGk_ypEuS24?si=7Y4nO0hu37rPwmjB"/>
+    <hyperlink ref="E120" r:id="rId250" display="https://www.geeksforgeeks.org/bubble-sort/"/>
+    <hyperlink ref="C121" r:id="rId251" display="https://www.geeksforgeeks.org/problems/selection-sort/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D121" r:id="rId252" display="https://youtu.be/HGk_ypEuS24?si=7Y4nO0hu37rPwmjB"/>
+    <hyperlink ref="E121" r:id="rId253" display="https://www.geeksforgeeks.org/selection-sort/"/>
+    <hyperlink ref="C122" r:id="rId254" display="https://www.geeksforgeeks.org/problems/insertion-sort/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D122" r:id="rId255" display="https://youtu.be/HGk_ypEuS24?si=7Y4nO0hu37rPwmjB"/>
+    <hyperlink ref="E122" r:id="rId256" display="https://www.geeksforgeeks.org/insertion-sort/"/>
+    <hyperlink ref="C123" r:id="rId257" display="https://www.geeksforgeeks.org/problems/merge-sort/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D123" r:id="rId258" display="https://youtu.be/ogjf7ORKfd8?si=nHB5zJMfQf-fmOim"/>
+    <hyperlink ref="E123" r:id="rId259" display="https://www.geeksforgeeks.org/merge-sort/"/>
+    <hyperlink ref="C124" r:id="rId260" display="https://www.geeksforgeeks.org/problems/quick-sort/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D124" r:id="rId261" display="https://youtu.be/WIrA4YexLRQ?si=IBwwb6xHsi3YGOSN"/>
+    <hyperlink ref="E124" r:id="rId262" display="https://www.geeksforgeeks.org/quick-sort/"/>
+    <hyperlink ref="D126" r:id="rId263" display="https://youtu.be/Nq7ok-OyEpg?si=ryFFMk9gQcXMephl"/>
+    <hyperlink ref="E126" r:id="rId264" display="https://www.geeksforgeeks.org/what-is-linked-list/"/>
+    <hyperlink ref="D127" r:id="rId265" display="https://youtu.be/VaECK03Dz-g?si=-81fgfc9CAs2P-yg"/>
+    <hyperlink ref="E127" r:id="rId266" display="https://www.programiz.com/dsa/linked-list-operations"/>
+    <hyperlink ref="C128" r:id="rId267"/>
+    <hyperlink ref="D128" r:id="rId268" display="https://youtu.be/Nq7ok-OyEpg?si=oiwMXSQZwVteQp7t"/>
+    <hyperlink ref="E128" r:id="rId269" display="https://www.geeksforgeeks.org/search-an-element-in-a-linked-list-iterative-and-recursive/"/>
+    <hyperlink ref="C129" r:id="rId270"/>
+    <hyperlink ref="D129" r:id="rId271" display="https://youtu.be/D2vI2DNJGd8?si=vljGaBvoeAzu2yjH"/>
+    <hyperlink ref="E129" r:id="rId272" display="https://www.geeksforgeeks.org/reverse-a-linked-list/"/>
+    <hyperlink ref="C130" r:id="rId273"/>
+    <hyperlink ref="D130" r:id="rId274" display="https://youtu.be/lRY_G-u_8jk?si=NpNIWRnrnLxtwvHc"/>
+    <hyperlink ref="E130" r:id="rId275" display="https://www.geeksforgeeks.org/function-to-check-if-a-singly-linked-list-is-palindrome/"/>
+    <hyperlink ref="C131" r:id="rId276"/>
+    <hyperlink ref="D131" r:id="rId277" display="https://youtu.be/7LjQ57RqgEc?si=7TB3YSJldSkveCM6"/>
+    <hyperlink ref="E131" r:id="rId278" display="https://www.geeksforgeeks.org/insert-node-middle-linked-list/"/>
+    <hyperlink ref="C132" r:id="rId279"/>
+    <hyperlink ref="D132" r:id="rId280" display="https://youtu.be/0DYoPz2Tpt4?si=kwaZaI8b848cqh7q"/>
+    <hyperlink ref="E132" r:id="rId281" display="https://www.geeksforgeeks.org/write-a-function-to-get-the-intersection-point-of-two-linked-lists/"/>
+    <hyperlink ref="C133" r:id="rId282" display="https://www.geeksforgeeks.org/problems/union-of-two-linked-list/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D133" r:id="rId283" display="https://youtu.be/wvcQg43_V8U?si=hnKPSWEqSjHN9dNn"/>
+    <hyperlink ref="E133" r:id="rId284" display="https://www.geeksforgeeks.org/union-and-intersection-of-two-linked-lists/"/>
+    <hyperlink ref="C134" r:id="rId285"/>
+    <hyperlink ref="D134" r:id="rId286" display="https://youtu.be/icnp4FJdZ_c?si=NZr1bzvtR_ARASzF"/>
+    <hyperlink ref="E134" r:id="rId287" display="https://www.geeksforgeeks.org/delete-a-node-from-linked-list-without-head-pointer/"/>
+    <hyperlink ref="C135" r:id="rId288"/>
+    <hyperlink ref="E135" r:id="rId289" display="https://www.geeksforgeeks.org/count-pairs-two-linked-lists-whose-sum-equal-given-value/"/>
+    <hyperlink ref="C136" r:id="rId290"/>
+    <hyperlink ref="D136" r:id="rId291" display="https://youtu.be/lIar1skcQYI?si=maRDPjLBH_7lm7XJ"/>
+    <hyperlink ref="E136" r:id="rId292" display="https://www.geeksforgeeks.org/reverse-a-linked-list-in-groups-of-given-size/"/>
+    <hyperlink ref="C138" r:id="rId293"/>
+    <hyperlink ref="D138" r:id="rId294" display="https://youtu.be/wiOo4DC5GGA?si=8SqmTgLyYwgXw95f"/>
+    <hyperlink ref="E138" r:id="rId295" display="https://www.geeksforgeeks.org/detect-loop-in-a-linked-list/"/>
+    <hyperlink ref="C139" r:id="rId296"/>
+    <hyperlink ref="D139" r:id="rId297" display="https://youtu.be/I4g1qbkTPus?si=YqFJkeqopml7lRkN"/>
+    <hyperlink ref="E139" r:id="rId298" display="https://www.geeksforgeeks.org/find-length-of-loop-in-linked-list/"/>
+    <hyperlink ref="C140" r:id="rId299"/>
+    <hyperlink ref="D140" r:id="rId300" display="https://youtu.be/2Kd0KKmmHFc?si=G-cVazaPJN8XjgfB"/>
+    <hyperlink ref="E140" r:id="rId301" display="https://www.geeksforgeeks.org/find-first-node-of-loop-in-a-linked-list/"/>
+    <hyperlink ref="C141" r:id="rId302"/>
+    <hyperlink ref="D141" r:id="rId303" display="https://youtu.be/_BG9rjkAXj8?si=egrP9V6ROMAip9jT"/>
+    <hyperlink ref="E141" r:id="rId304" display="https://www.geeksforgeeks.org/detect-and-remove-loop-in-a-linked-list/"/>
+    <hyperlink ref="C143" r:id="rId305"/>
+    <hyperlink ref="D143" r:id="rId306" display="https://youtu.be/gRII7LhdJWc?si=q-xNQeYvdXPR8WWj"/>
+    <hyperlink ref="E143" r:id="rId307" display="https://www.geeksforgeeks.org/sort-a-linked-list-of-0s-1s-or-2s/"/>
+    <hyperlink ref="C144" r:id="rId308"/>
+    <hyperlink ref="D144" r:id="rId309" display="https://youtu.be/bN8nk4ZXzK0?si=iA2AjojAqKG9d_WU"/>
+    <hyperlink ref="E144" r:id="rId310" display="https://www.geeksforgeeks.org/pairwise-swap-elements-of-a-given-linked-list/"/>
+    <hyperlink ref="C145" r:id="rId311"/>
+    <hyperlink ref="D145" r:id="rId312" display="https://youtu.be/q5a5OiGbT6Q?si=IMmJI7RvGvEP59_C"/>
+    <hyperlink ref="E145" r:id="rId313" display="https://www.geeksforgeeks.org/merge-two-sorted-linked-lists/"/>
+    <hyperlink ref="C146" r:id="rId314"/>
+    <hyperlink ref="D146" r:id="rId315" display="https://youtu.be/ogjf7ORKfd8?si=rzOnEXKe2To-rSdw"/>
+    <hyperlink ref="E146" r:id="rId316" display="https://www.geeksforgeeks.org/merge-sort-for-linked-list/"/>
+    <hyperlink ref="C147" r:id="rId317" display="https://www.geeksforgeeks.org/problems/quick-sort-on-linked-list/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D147" r:id="rId318" display="https://youtu.be/WIrA4YexLRQ?si=-NZqIbzEpb-6OARV"/>
+    <hyperlink ref="E147" r:id="rId319" display="https://www.geeksforgeeks.org/quicksort-on-singly-linked-list/"/>
+    <hyperlink ref="D148" r:id="rId320" display="https://youtu.be/YJKVTnOJXSY?si=v8RSH10efQJUvW0C"/>
+    <hyperlink ref="E148" r:id="rId321" display="https://www.geeksforgeeks.org/remove-duplicates-from-a-sorted-linked-list/"/>
+    <hyperlink ref="C149" r:id="rId322"/>
+    <hyperlink ref="D149" r:id="rId323" display="https://www.youtube.com/live/JfWROTUQcn8?si=o9X1KOCltap_orbJ"/>
+    <hyperlink ref="E149" r:id="rId324" display="https://www.geeksforgeeks.org/segregate-even-and-odd-elements-in-a-linked-list/"/>
+    <hyperlink ref="C151" r:id="rId325"/>
+    <hyperlink ref="D151" r:id="rId326" display="https://youtu.be/aXQWhbvT3w0?si=YWdIiQXsrfQHnrYn"/>
+    <hyperlink ref="E151" r:id="rId327" display="https://www.geeksforgeeks.org/add-1-number-represented-linked-list/"/>
+    <hyperlink ref="C152" r:id="rId328"/>
+    <hyperlink ref="D152" r:id="rId329" display="https://youtu.be/LBVsXSMOIk4?si=iIQRk_sF9zAtwknT"/>
+    <hyperlink ref="E152" r:id="rId330" display="https://www.geeksforgeeks.org/add-two-numbers-represented-by-linked-list/"/>
+    <hyperlink ref="C153" r:id="rId331"/>
+    <hyperlink ref="E153" r:id="rId332" display="https://www.geeksforgeeks.org/subtract-two-numbers-represented-as-linked-lists/"/>
+    <hyperlink ref="C155" r:id="rId333"/>
+    <hyperlink ref="D155" r:id="rId334" display="https://youtu.be/uT7YI7XbTY8?si=ueKdt7ev8rjshlGW"/>
+    <hyperlink ref="E155" r:id="rId335" display="https://www.geeksforgeeks.org/rearrange-a-given-linked-list-in-place/"/>
+    <hyperlink ref="C156" r:id="rId336"/>
+    <hyperlink ref="D156" r:id="rId337" display="https://youtu.be/ysytSSXpAI0?si=K3PCYAXGifgKqL1p"/>
+    <hyperlink ref="E156" r:id="rId338" display="https://www.geeksforgeeks.org/flattening-a-linked-list/"/>
+    <hyperlink ref="C157" r:id="rId339"/>
+    <hyperlink ref="D157" r:id="rId340" display="https://youtu.be/jDPrM5XIqzM?si=w0IEUl9Y2qmXSdtC"/>
+    <hyperlink ref="E157" r:id="rId341" display="https://www.geeksforgeeks.org/delete-nodes-which-have-a-greater-value-on-right-side/"/>
+    <hyperlink ref="C158" r:id="rId342"/>
+    <hyperlink ref="D158" r:id="rId343" display="https://youtu.be/icnp4FJdZ_c?si=a2BJWMCc9ETeevAO"/>
+    <hyperlink ref="E158" r:id="rId344" display="https://www.geeksforgeeks.org/delete-n-nodes-after-m-nodes-of-a-linked-list/"/>
+    <hyperlink ref="D159" r:id="rId345" display="https://youtu.be/Mh0NH_SD92k?si=_jaOPDZKpnHohet2"/>
+    <hyperlink ref="C160" r:id="rId346"/>
+    <hyperlink ref="D160" r:id="rId347" display="https://youtu.be/VNf6VynfpdM?si=e1slTowpTqIc---M"/>
+    <hyperlink ref="E160" r:id="rId348" display="https://www.geeksforgeeks.org/a-linked-list-with-next-and-arbit-pointer/"/>
+    <hyperlink ref="C161" r:id="rId349"/>
+    <hyperlink ref="D161" r:id="rId350" display="https://youtu.be/6i_T5kkfv4A?si=L6rVlrvdYuSXGiWa"/>
+    <hyperlink ref="E161" r:id="rId351" display="https://www.geeksforgeeks.org/length-longest-palindrome-list-linked-list-using-o1-extra-space/"/>
+    <hyperlink ref="E162" r:id="rId352" display="https://www.geeksforgeeks.org/circular-linked-list/"/>
+    <hyperlink ref="D164" r:id="rId353" display="https://youtu.be/Nq7ok-OyEpg?si=dDrqbUkV_lKFkLSV"/>
+    <hyperlink ref="E164" r:id="rId354" display="https://www.geeksforgeeks.org/what-is-linked-list/"/>
+    <hyperlink ref="C165" r:id="rId355"/>
+    <hyperlink ref="D165" r:id="rId356" display="https://youtu.be/u3WUW2qe6ww?si=hAazIXgy1oPd1_KJ"/>
+    <hyperlink ref="E165" r:id="rId357" display="https://www.geeksforgeeks.org/reverse-a-doubly-linked-list/"/>
+    <hyperlink ref="C166" r:id="rId358"/>
+    <hyperlink ref="D166" r:id="rId359" display="https://youtu.be/YitR4dQsddE?si=mrZaT1w0xdI_VKYJ"/>
+    <hyperlink ref="E166" r:id="rId360" display="https://www.geeksforgeeks.org/find-pairs-given-sum-doubly-linked-list/"/>
+    <hyperlink ref="C169" r:id="rId361"/>
+    <hyperlink ref="E169" r:id="rId362" display="https://www.geeksforgeeks.org/introduction-to-stack-data-structure-and-algorithm-tutorials/"/>
+    <hyperlink ref="C170" r:id="rId363"/>
+    <hyperlink ref="D170" r:id="rId364" display="https://youtu.be/GYptUgnIM_I?si=YEr87UrxZw1xaMk3"/>
+    <hyperlink ref="E170" r:id="rId365" display="https://www.geeksforgeeks.org/implement-two-stacks-in-an-array/"/>
+    <hyperlink ref="C171" r:id="rId366"/>
+    <hyperlink ref="D171" r:id="rId367" display="https://youtu.be/wkDfsKijrZ8?si=xmSeeK82cI-4hsWZ"/>
+    <hyperlink ref="E171" r:id="rId368" display="https://www.geeksforgeeks.org/check-if-given-parentheses-expression-is-balanced-or-not/"/>
+    <hyperlink ref="C172" r:id="rId369"/>
+    <hyperlink ref="E172" r:id="rId370" display="https://www.geeksforgeeks.org/design-a-stack-that-supports-getmin-in-o1-time-and-o1-extra-space/"/>
+    <hyperlink ref="C174" r:id="rId371"/>
+    <hyperlink ref="D174" r:id="rId372" display="https://youtu.be/Du881K7Jtk8?si=1KDoD1_Ke3mzxlL1"/>
+    <hyperlink ref="E174" r:id="rId373" display="https://www.geeksforgeeks.org/next-greater-element/"/>
+    <hyperlink ref="C175" r:id="rId374"/>
+    <hyperlink ref="E175" r:id="rId375" display="https://www.geeksforgeeks.org/find-the-next-greater-element-in-a-circular-array/"/>
+    <hyperlink ref="C177" r:id="rId376"/>
+    <hyperlink ref="D177" r:id="rId377" display="https://youtu.be/_RtghJnM1Qo?si=4qrv3aDDwijeRm_o"/>
+    <hyperlink ref="E177" r:id="rId378" display="https://www.geeksforgeeks.org/find-the-nearest-smaller-numbers-on-left-side-in-an-array/"/>
+    <hyperlink ref="C178" r:id="rId379"/>
+    <hyperlink ref="D178" r:id="rId380" display="https://youtu.be/_RtghJnM1Qo?si=4qrv3aDDwijeRm_o"/>
+    <hyperlink ref="E178" r:id="rId381" display="https://www.procoding.org/nearest-smaller-to-right"/>
+    <hyperlink ref="C179" r:id="rId382"/>
+    <hyperlink ref="D179" r:id="rId383" display="https://youtu.be/slYh0ZNEqSw?si=Bb04H9MqRP1wTDDl"/>
+    <hyperlink ref="E179" r:id="rId384" display="https://www.geeksforgeeks.org/the-stock-span-problem/"/>
+    <hyperlink ref="C180" r:id="rId385" display="https://www.geeksforgeeks.org/problems/trapping-rain-water-1587115621/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D180" r:id="rId386" display="https://youtu.be/m18Hntz4go8?si=7qLelcwMU1zX_f8T"/>
+    <hyperlink ref="E180" r:id="rId387" display="https://www.geeksforgeeks.org/trapping-rain-water/"/>
+    <hyperlink ref="C181" r:id="rId388"/>
+    <hyperlink ref="D181" r:id="rId389" display="https://youtu.be/X0X6G-eWgQ8?si=MRIKghS-DLv_7Pi2"/>
+    <hyperlink ref="E181" r:id="rId390" display="https://www.geeksforgeeks.org/largest-rectangular-area-in-a-histogram-using-stack/"/>
+    <hyperlink ref="C182" r:id="rId391"/>
+    <hyperlink ref="D182" r:id="rId392" display="https://youtu.be/tOylVCugy9k?si=5qpEF2oU_iQyv1yp"/>
+    <hyperlink ref="E182" r:id="rId393" display="https://www.geeksforgeeks.org/maximum-size-rectangle-binary-sub-matrix-1s/"/>
+    <hyperlink ref="C184" r:id="rId394"/>
+    <hyperlink ref="D184" r:id="rId395" display="https://youtu.be/PAceaOSnxQs?si=LFGbZRMkHTMthAqQ"/>
+    <hyperlink ref="E184" r:id="rId396" display="https://www.geeksforgeeks.org/convert-infix-expression-to-postfix-expression/"/>
+    <hyperlink ref="C185" r:id="rId397"/>
+    <hyperlink ref="D185" r:id="rId398" display="https://youtu.be/u3paQa8KXu0?si=v-QZxZvRK7yRTdnm"/>
+    <hyperlink ref="E185" r:id="rId399" display="https://www.geeksforgeeks.org/evaluation-of-postfix-expression/"/>
+    <hyperlink ref="C186" r:id="rId400"/>
+    <hyperlink ref="D186" r:id="rId401" display="https://youtu.be/RY4GkLahbCI?si=PxZ0CNQSmPe5Iri2"/>
+    <hyperlink ref="E186" r:id="rId402" display="https://www.geeksforgeeks.org/prefix-postfix-conversion/"/>
+    <hyperlink ref="C187" r:id="rId403"/>
+    <hyperlink ref="E187" r:id="rId404" display="https://www.geeksforgeeks.org/arithmetic-expression-evalution/"/>
+    <hyperlink ref="C189" r:id="rId405"/>
+    <hyperlink ref="D189" r:id="rId406" display="https://youtu.be/BmZnJehDzyU?si=bZejmkHrQhG9nc-D"/>
+    <hyperlink ref="E189" r:id="rId407" display="https://www.geeksforgeeks.org/program-to-insert-an-element-at-the-bottom-of-a-stack/"/>
+    <hyperlink ref="C190" r:id="rId408"/>
+    <hyperlink ref="D190" r:id="rId409" display="https://youtu.be/SW14tOda_kI?si=8j5-licSNQkxX7GW"/>
+    <hyperlink ref="E190" r:id="rId410" display="https://www.geeksforgeeks.org/reverse-a-stack-using-recursion/"/>
+    <hyperlink ref="C191" r:id="rId411"/>
+    <hyperlink ref="D191" r:id="rId412" display="https://youtu.be/SjDq1xYxC44?si=Y3th_GK9E5TE4LQt"/>
+    <hyperlink ref="E191" r:id="rId413" display="https://www.geeksforgeeks.org/sort-a-stack-using-recursion/"/>
+    <hyperlink ref="C193" r:id="rId414"/>
+    <hyperlink ref="D193" r:id="rId415" display="https://youtu.be/9u2BJfmWNEg?si=6KkJHm8rjX6xTOsm"/>
+    <hyperlink ref="E193" r:id="rId416" display="https://www.geeksforgeeks.org/the-celebrity-problem/"/>
+    <hyperlink ref="C194" r:id="rId417"/>
+    <hyperlink ref="D194" r:id="rId418" display="https://youtu.be/fIdNHd5nEqI?si=AX5qTxIvmvKKlyRf"/>
+    <hyperlink ref="E194" r:id="rId419" display="https://www.geeksforgeeks.org/reduce-the-string-by-removing-k-consecutive-identical-characters/"/>
+    <hyperlink ref="C195" r:id="rId420"/>
+    <hyperlink ref="D195" r:id="rId421" display="https://www.youtube.com/live/Bg0Y9__J8UE?si=bR4Jmm1QtbwHocbQ"/>
+    <hyperlink ref="E195" r:id="rId422" display="https://www.geeksforgeeks.org/minimum-number-of-bracket-reversals-needed-to-make-an-expression-balanced/"/>
+    <hyperlink ref="C198" r:id="rId423"/>
+    <hyperlink ref="D198" r:id="rId424" display="https://youtu.be/M6GnoUDpqEE?si=_dqoKIYUU275Hcmv"/>
+    <hyperlink ref="E198" r:id="rId425" display="https://www.geeksforgeeks.org/array-implementation-of-queue-simple/"/>
+    <hyperlink ref="C199" r:id="rId426"/>
+    <hyperlink ref="E199" r:id="rId427" display="https://www.geeksforgeeks.org/queue-linked-list-implementation/"/>
+    <hyperlink ref="C200" r:id="rId428"/>
+    <hyperlink ref="D200" r:id="rId429" display="https://youtu.be/3Et9MrMc02A?si=voYSp9_jK2S7pkFr"/>
+    <hyperlink ref="E200" r:id="rId430" display="https://www.geeksforgeeks.org/implement-stack-using-queue/"/>
+    <hyperlink ref="C201" r:id="rId431"/>
+    <hyperlink ref="D201" r:id="rId432" display="https://youtu.be/jDZQKzEtbYQ?si=-3eKyh6SDVQXJPIv"/>
+    <hyperlink ref="E201" r:id="rId433" display="https://www.geeksforgeeks.org/implement-stack-using-queue/"/>
+    <hyperlink ref="C202" r:id="rId434"/>
+    <hyperlink ref="E202" r:id="rId435" display="https://www.geeksforgeeks.org/reversing-a-queue/"/>
+    <hyperlink ref="C204" r:id="rId436"/>
+    <hyperlink ref="D204" r:id="rId437" display="https://youtu.be/_gJ3to4RyeQ?si=qK6-vjLpG1O_jjW3"/>
+    <hyperlink ref="E204" r:id="rId438" display="https://www.geeksforgeeks.org/find-a-tour-that-visits-all-stations/"/>
+    <hyperlink ref="C205" r:id="rId439"/>
+    <hyperlink ref="D205" r:id="rId440" display="https://youtu.be/_gJ3to4RyeQ?si=qK6-vjLpG1O_jjW3"/>
+    <hyperlink ref="E205" r:id="rId441" display="https://www.geeksforgeeks.org/find-first-non-repeating-character-stream-characters/"/>
+    <hyperlink ref="C206" r:id="rId442"/>
+    <hyperlink ref="D206" r:id="rId443" display="https://www.youtube.com/watch?v=_gJ3to4RyeQ&amp;t=4244s"/>
+    <hyperlink ref="E206" r:id="rId444" display="https://www.geeksforgeeks.org/reversing-first-k-elements-queue/"/>
+    <hyperlink ref="C207" r:id="rId445"/>
+    <hyperlink ref="D207" r:id="rId446" display="https://youtu.be/xDEuM5qa0zg?si=1I7GJk3ep77i7dN3"/>
+    <hyperlink ref="E207" r:id="rId447" display="https://www.geeksforgeeks.org/lru-cache-implementation/"/>
+    <hyperlink ref="C208" r:id="rId448"/>
+    <hyperlink ref="E208" r:id="rId449" display="https://www.geeksforgeeks.org/connect-n-ropes-minimum-cost/"/>
+    <hyperlink ref="C209" r:id="rId450"/>
+    <hyperlink ref="E209" r:id="rId451" display="https://www.geeksforgeeks.org/nearly-sorted-algorithm/"/>
+    <hyperlink ref="C212" r:id="rId452" display="https://www.geeksforgeeks.org/problems/max-sum-subarray-of-size-k5313/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D212" r:id="rId453" display="https://youtu.be/TCHSXAu5pls?si=ZP_jrOEraTJAophE"/>
+    <hyperlink ref="E212" r:id="rId454" display="https://www.geeksforgeeks.org/find-maximum-minimum-sum-subarray-size-k/"/>
+    <hyperlink ref="C213" r:id="rId455"/>
+    <hyperlink ref="D213" r:id="rId456" display="https://www.youtube.com/live/3QSvHEmJAkc?si=O76LO8eM72LpKL4s"/>
+    <hyperlink ref="E213" r:id="rId457" display="https://www.geeksforgeeks.org/count-distinct-elements-in-every-window-of-size-k/"/>
+    <hyperlink ref="C214" r:id="rId458"/>
+    <hyperlink ref="D214" r:id="rId459" display="https://www.youtube.com/live/QIDV7m1JrnA?si=Lmr9b8Zi6H06MCTS"/>
+    <hyperlink ref="E214" r:id="rId460" display="https://www.geeksforgeeks.org/first-negative-integer-every-window-size-k/"/>
+    <hyperlink ref="C215" r:id="rId461"/>
+    <hyperlink ref="D215" r:id="rId462" display="https://youtu.be/CZQGRp93K4k?si=7zprdiDcdlnC9vmM"/>
+    <hyperlink ref="E215" r:id="rId463" display="https://www.geeksforgeeks.org/sliding-window-maximum-maximum-of-all-subarrays-of-size-k/"/>
+    <hyperlink ref="C216" r:id="rId464"/>
+    <hyperlink ref="D216" r:id="rId465" display="https://youtu.be/WIkO_t1Kam8?si=u2P3Mo1qvBqxwfRv"/>
+    <hyperlink ref="E216" r:id="rId466" display="https://www.geeksforgeeks.org/count-of-substrings-of-length-k-with-exactly-k-distinct-characters/"/>
+    <hyperlink ref="C217" r:id="rId467"/>
+    <hyperlink ref="D217" r:id="rId468" display="https://www.youtube.com/live/CK8PIAF-m2E?si=t61U2qRD6k7jeFwn"/>
+    <hyperlink ref="E217" r:id="rId469" display="https://www.geeksforgeeks.org/find-the-maximum-of-minimums-for-every-window-size-in-a-given-array/"/>
+    <hyperlink ref="C219" r:id="rId470"/>
+    <hyperlink ref="D219" r:id="rId471" display="https://youtu.be/Ofl4KgFhLsM?si=68FBAztFdbHbV_CF"/>
+    <hyperlink ref="E219" r:id="rId472" display="https://www.geeksforgeeks.org/find-subarray-with-given-sum/"/>
+    <hyperlink ref="C220" r:id="rId473"/>
+    <hyperlink ref="D220" r:id="rId474" display="https://youtu.be/frf7qxiN2qU?si=3VDd0PuUXyWxTFTr"/>
+    <hyperlink ref="E220" r:id="rId475" display="https://www.geeksforgeeks.org/longest-sub-array-sum-k/"/>
+    <hyperlink ref="C221" r:id="rId476"/>
+    <hyperlink ref="D221" r:id="rId477" display="https://youtu.be/xmguZ6GbatA?si=Zxs8fEIzorVIa5_X"/>
+    <hyperlink ref="E221" r:id="rId478" display="https://www.geeksforgeeks.org/find-if-there-is-a-subarray-with-0-sum/"/>
+    <hyperlink ref="C222" r:id="rId479"/>
+    <hyperlink ref="D222" r:id="rId480" display="https://youtu.be/zm50uGBsSz4?si=hGS8FZK2mWMPg-vX"/>
+    <hyperlink ref="E222" r:id="rId481" display="https://www.geeksforgeeks.org/smallest-window-contains-characters-string/"/>
+    <hyperlink ref="C223" r:id="rId482"/>
+    <hyperlink ref="D223" r:id="rId483" display="https://www.youtube.com/live/FMxJQqWaD28?si=py1VR3QKmYSdtQWy"/>
+    <hyperlink ref="E223" r:id="rId484" display="https://www.geeksforgeeks.org/smallest-window-containing-0-1-and-2/"/>
+    <hyperlink ref="C224" r:id="rId485"/>
+    <hyperlink ref="D224" r:id="rId486" display="https://youtu.be/jSto0O4AJbM?si=y-lWXYWB4yZZ9cVQ"/>
+    <hyperlink ref="E224" r:id="rId487" display="https://www.geeksforgeeks.org/find-the-smallest-window-in-a-string-containing-all-characters-of-another-string/"/>
+    <hyperlink ref="C225" r:id="rId488"/>
+    <hyperlink ref="D225" r:id="rId489" display="https://youtu.be/qtVh-XEpsJo?si=DdoYedxtXw0DDrNf"/>
+    <hyperlink ref="E225" r:id="rId490" display="https://www.geeksforgeeks.org/length-of-the-longest-substring-without-repeating-characters/"/>
+    <hyperlink ref="C226" r:id="rId491"/>
+    <hyperlink ref="D226" r:id="rId492" display="https://youtu.be/xmguZ6GbatA?si=x29mj29byvR_FBBd"/>
+    <hyperlink ref="E226" r:id="rId493" display="https://www.geeksforgeeks.org/largest-subarray-with-equal-number-of-0s-and-1s/"/>
+    <hyperlink ref="C227" r:id="rId494"/>
+    <hyperlink ref="D227" r:id="rId495" display="https://youtu.be/fYgU6Bi2fRg?si=q45yqwde54whHlR2"/>
+    <hyperlink ref="E227" r:id="rId496" display="https://www.geeksforgeeks.org/count-occurrences-of-anagrams/"/>
+    <hyperlink ref="C228" r:id="rId497"/>
+    <hyperlink ref="D228" r:id="rId498" display="https://youtu.be/Mo33MjjMlyA?si=01XiyS0oBtaaFenb"/>
+    <hyperlink ref="E228" r:id="rId499" display="https://www.geeksforgeeks.org/maximum-consecutive-ones-formed-by-deleting-at-most-k-0s/"/>
+    <hyperlink ref="C229" r:id="rId500"/>
+    <hyperlink ref="C230" r:id="rId501"/>
+    <hyperlink ref="D230" r:id="rId502" display="https://youtu.be/gqXU1UyA8pk?si=ytPr4mkVqLJfD7v4"/>
+    <hyperlink ref="C231" r:id="rId503"/>
+    <hyperlink ref="D231" r:id="rId504" display="https://youtu.be/gqXU1UyA8pk?si=rMwzYE99DsiO2Gj-"/>
+    <hyperlink ref="C232" r:id="rId505"/>
+    <hyperlink ref="D232" r:id="rId506" display="https://youtu.be/jSto0O4AJbM?si=-ls0q5Dhw9uqf-cF"/>
+    <hyperlink ref="C233" r:id="rId507"/>
+    <hyperlink ref="D233" r:id="rId508" display="https://youtu.be/jSto0O4AJbM?si=-ls0q5Dhw9uqf-cF"/>
+    <hyperlink ref="C234" r:id="rId509"/>
+    <hyperlink ref="D234" r:id="rId510" display="https://youtu.be/akwRFY2eyXs?si=AKnbBikPvDJtF2lA"/>
+    <hyperlink ref="D236" r:id="rId511" display="https://youtu.be/_ANrF3FJm7I?si=U4__gOBVdaEBZwJ9"/>
+    <hyperlink ref="C237" r:id="rId512"/>
+    <hyperlink ref="D237" r:id="rId513" display="https://youtu.be/RlUu72JrOCQ?si=Vfh9JTBxwgVQGeIk"/>
+    <hyperlink ref="E237" r:id="rId514" display="https://www.geeksforgeeks.org/preorder-traversal-of-binary-tree/"/>
+    <hyperlink ref="C238" r:id="rId515"/>
+    <hyperlink ref="D238" r:id="rId516" display="https://youtu.be/Z_NEgBgbRVI?si=Ji2rLUtTb7-6OylN"/>
+    <hyperlink ref="E238" r:id="rId517" display="https://www.geeksforgeeks.org/inorder-traversal-of-binary-tree/"/>
+    <hyperlink ref="C239" r:id="rId518"/>
+    <hyperlink ref="D239" r:id="rId519" display="https://youtu.be/COQOU6klsBg?si=0yuM-upS3qmX2kWF"/>
+    <hyperlink ref="E239" r:id="rId520" display="https://www.geeksforgeeks.org/postorder-traversal-of-binary-tree/"/>
+    <hyperlink ref="C240" r:id="rId521"/>
+    <hyperlink ref="D240" r:id="rId522" display="https://youtu.be/EoAsWbO7sqg?si=1NSXTiOBM6LObxiN"/>
+    <hyperlink ref="E240" r:id="rId523" display="https://www.geeksforgeeks.org/level-order-tree-traversal/"/>
+    <hyperlink ref="C241" r:id="rId524"/>
+    <hyperlink ref="D241" r:id="rId525" display="https://youtu.be/0ca1nvR0be4?si=53I0bM9ppRbgnF0x"/>
+    <hyperlink ref="E241" r:id="rId526" display="https://www.geeksforgeeks.org/boundary-traversal-of-binary-tree/"/>
+    <hyperlink ref="C242" r:id="rId527"/>
+    <hyperlink ref="D242" r:id="rId528" display="https://youtu.be/q_a6lpbKJdw?si=uewd5ll1X-h-GTzT"/>
+    <hyperlink ref="E242" r:id="rId529" display="https://www.geeksforgeeks.org/vertical-order-traversal-of-binary-tree-using-map/"/>
+    <hyperlink ref="C243" r:id="rId530"/>
+    <hyperlink ref="D243" r:id="rId531" display="https://youtu.be/Et9OCDNvJ78?si=oeOojp-R7oWt1IVF"/>
+    <hyperlink ref="E243" r:id="rId532" display="https://www.geeksforgeeks.org/print-nodes-top-view-binary-tree/"/>
+    <hyperlink ref="C244" r:id="rId533"/>
+    <hyperlink ref="D244" r:id="rId534" display="https://youtu.be/0FtVY6I4pB8?si=hfNz5XIojTt16c5K"/>
+    <hyperlink ref="E244" r:id="rId535" display="http://v/"/>
+    <hyperlink ref="C245" r:id="rId536"/>
+    <hyperlink ref="D245" r:id="rId537" display="https://youtu.be/KV4mRzTjlAk?si=_fgLNgJSstGTAq5h"/>
+    <hyperlink ref="E245" r:id="rId538" display="https://www.geeksforgeeks.org/print-left-view-binary-tree/"/>
+    <hyperlink ref="C246" r:id="rId539"/>
+    <hyperlink ref="D246" r:id="rId540" display="https://youtu.be/KV4mRzTjlAk?si=_fgLNgJSstGTAq5h"/>
+    <hyperlink ref="E246" r:id="rId541" display="https://www.geeksforgeeks.org/print-right-view-binary-tree-2/"/>
+    <hyperlink ref="C247" r:id="rId542"/>
+    <hyperlink ref="E247" r:id="rId543" display="https://www.geeksforgeeks.org/diagonal-traversal-of-binary-tree/"/>
+    <hyperlink ref="E249" r:id="rId544" display="https://www.geeksforgeeks.org/insertion-in-binary-search-tree/"/>
+    <hyperlink ref="C250" r:id="rId545"/>
+    <hyperlink ref="D250" r:id="rId546" display="https://youtu.be/eD3tmO66aBA?si=USzVxf8j_Bh8cF9s"/>
+    <hyperlink ref="E250" r:id="rId547" display="https://www.geeksforgeeks.org/find-the-maximum-depth-or-height-of-a-tree/"/>
+    <hyperlink ref="C251" r:id="rId548"/>
+    <hyperlink ref="D251" r:id="rId549" display="https://youtu.be/Rezetez59Nk?si=1PPe8FweQ_aY4r5R"/>
+    <hyperlink ref="E251" r:id="rId550" display="https://www.geeksforgeeks.org/diameter-of-a-binary-tree/"/>
+    <hyperlink ref="C252" r:id="rId551"/>
+    <hyperlink ref="D252" r:id="rId552" display="https://youtu.be/BhuvF_-PWS0?si=jkA1zhLsZjSM3As8"/>
+    <hyperlink ref="E252" r:id="rId553" display="https://www.geeksforgeeks.org/write-c-code-to-determine-if-two-trees-are-identical/"/>
+    <hyperlink ref="C253" r:id="rId554"/>
+    <hyperlink ref="D253" r:id="rId555" display="https://youtu.be/E36O5SWp-LE?si=cIhKUJ-T11II1wJx"/>
+    <hyperlink ref="E253" r:id="rId556" display="https://www.geeksforgeeks.org/check-if-a-binary-tree-is-subtree-of-another-binary-tree/"/>
+    <hyperlink ref="C254" r:id="rId557"/>
+    <hyperlink ref="D254" r:id="rId558" display="https://youtu.be/Yt50Jfbd8Po?si=W4TpdW3XaW-S4cFc"/>
+    <hyperlink ref="E254" r:id="rId559" display="https://www.geeksforgeeks.org/how-to-determine-if-a-binary-tree-is-balanced/"/>
+    <hyperlink ref="C255" r:id="rId560"/>
+    <hyperlink ref="D255" r:id="rId561" display="https://youtu.be/_-QHfMDde90?si=HJ5h-9Tm18BT0ezj"/>
+    <hyperlink ref="E255" r:id="rId562" display="https://www.geeksforgeeks.org/lowest-common-ancestor-binary-tree-set-1/"/>
+    <hyperlink ref="C256" r:id="rId563"/>
+    <hyperlink ref="E256" r:id="rId564" display="https://www.geeksforgeeks.org/check-if-a-given-binary-tree-is-sumtree/"/>
+    <hyperlink ref="C257" r:id="rId565"/>
+    <hyperlink ref="D257" r:id="rId566" display="https://youtu.be/nKggNAiEpBE?si=dUY7QGWwUBs3XxYs"/>
+    <hyperlink ref="E257" r:id="rId567" display="https://www.geeksforgeeks.org/symmetric-tree-tree-which-is-mirror-image-of-itself/"/>
+    <hyperlink ref="C258" r:id="rId568"/>
+    <hyperlink ref="D258" r:id="rId569" display="https://youtu.be/FtdyIHBaKjc?si=pf4peCzMbF56N5UF"/>
+    <hyperlink ref="E258" r:id="rId570" display="https://www.geeksforgeeks.org/write-an-efficient-c-function-to-convert-a-tree-into-its-mirror-tree/"/>
+    <hyperlink ref="C259" r:id="rId571"/>
+    <hyperlink ref="D259" r:id="rId572" display="https://youtu.be/Q9Np3-FX91U?si=ioypQwgjldt1tCGQ"/>
+    <hyperlink ref="C261" r:id="rId573"/>
+    <hyperlink ref="D261" r:id="rId574" display="https://youtu.be/fmflMqVOC7k?si=iSdK8HdoNEeKJARf"/>
+    <hyperlink ref="E261" r:id="rId575" display="https://www.geeksforgeeks.org/given-a-binary-tree-print-all-root-to-leaf-paths/"/>
+    <hyperlink ref="C262" r:id="rId576"/>
+    <hyperlink ref="E262" r:id="rId577" display="https://www.geeksforgeeks.org/root-to-leaf-path-sum-equal-to-a-given-number/"/>
+    <hyperlink ref="C263" r:id="rId578"/>
+    <hyperlink ref="E263" r:id="rId579" display="https://www.geeksforgeeks.org/find-maximum-path-sum-in-a-binary-tree/"/>
+    <hyperlink ref="C264" r:id="rId580"/>
+    <hyperlink ref="D264" r:id="rId581" display="https://youtu.be/7oL8kDCk1OI?si=2qC45jVcOM2sCcJI"/>
+    <hyperlink ref="E264" r:id="rId582" display="https://www.geeksforgeeks.org/count-all-k-sum-paths-in-a-binary-tree/"/>
+    <hyperlink ref="C265" r:id="rId583"/>
+    <hyperlink ref="D265" r:id="rId584" display="https://youtu.be/i9ORlEy6EsI?si=Z4dWg3diarKcc3jR"/>
+    <hyperlink ref="E265" r:id="rId585" display="https://www.geeksforgeeks.org/print-nodes-distance-k-given-node-binary-tree/"/>
+    <hyperlink ref="D266" r:id="rId586" display="https://youtu.be/wIloFJzSOfE?si=qH0sMEREyVagrVK8"/>
+    <hyperlink ref="C267" r:id="rId587"/>
+    <hyperlink ref="D267" r:id="rId588" display="https://youtu.be/joxx4hTYwcw?si=wROhziCvjrJvwsi_"/>
+    <hyperlink ref="E267" r:id="rId589" display="https://www.geeksforgeeks.org/find-distance-between-two-nodes-of-a-binary-tree/"/>
+    <hyperlink ref="C268" r:id="rId590"/>
+    <hyperlink ref="D268" r:id="rId591" display="https://youtu.be/d3ceg_7NcEY?si=dh-dWju5Pqm_WG8E"/>
+    <hyperlink ref="E268" r:id="rId592" display="https://www.geeksforgeeks.org/maximum-difference-between-node-and-its-ancestor-in-binary-tree/"/>
+    <hyperlink ref="C269" r:id="rId593"/>
+    <hyperlink ref="D269" r:id="rId594" display="https://youtu.be/2r5wLmQfD6g?si=Ah-1GqZq9ZvhcISZ"/>
+    <hyperlink ref="E269" r:id="rId595" display="https://www.geeksforgeeks.org/minimum-time-to-burn-a-tree-starting-from-a-leaf-node/"/>
+    <hyperlink ref="D270" r:id="rId596" display="https://youtu.be/p7-9UvDQZ3w?si=iz_Zheaz1rsdY4bv"/>
+    <hyperlink ref="C271" r:id="rId597"/>
+    <hyperlink ref="D271" r:id="rId598" display="https://youtu.be/FiFiNvM29ps?si=7o-MgkkpMI1Aaa5W"/>
+    <hyperlink ref="C272" r:id="rId599"/>
+    <hyperlink ref="D272" r:id="rId600" display="https://youtu.be/KcNt6v_56cc?si=TxJuxG6Ps5NYvy4g"/>
+    <hyperlink ref="E272" r:id="rId601" display="https://www.geeksforgeeks.org/binary-search-tree-data-structure/"/>
+    <hyperlink ref="C273" r:id="rId602"/>
+    <hyperlink ref="E273" r:id="rId603" display="https://www.geeksforgeeks.org/find-maximum-or-minimum-in-binary-tree/"/>
+    <hyperlink ref="C274" r:id="rId604"/>
+    <hyperlink ref="D274" r:id="rId605" display="https://youtu.be/9TJYWh0adfk?si=3x4i8tP5lxtDypuG"/>
+    <hyperlink ref="E274" r:id="rId606" display="https://www.geeksforgeeks.org/find-k-th-smallest-element-in-bst-order-statistics-in-bst/"/>
+    <hyperlink ref="C275" r:id="rId607"/>
+    <hyperlink ref="D275" r:id="rId608" display="https://youtu.be/f-sj7I5oXEI?si=QAg2Uv7BMGfJKGLY"/>
+    <hyperlink ref="E275" r:id="rId609" display="https://www.geeksforgeeks.org/a-program-to-check-if-a-binary-tree-is-bst-or-not/"/>
+    <hyperlink ref="C276" r:id="rId610"/>
+    <hyperlink ref="E276" r:id="rId611" display="https://www.geeksforgeeks.org/find-closest-element-binary-search-tree/"/>
+    <hyperlink ref="C277" r:id="rId612"/>
+    <hyperlink ref="D277" r:id="rId613" display="https://youtu.be/jfk-uX_xKK4?si=2KQlXW2aA51Tz6q5"/>
+    <hyperlink ref="E277" r:id="rId614" display="https://www.geeksforgeeks.org/count-bst-nodes-that-are-in-a-given-range/"/>
+    <hyperlink ref="C278" r:id="rId615"/>
+    <hyperlink ref="D278" r:id="rId616" display="https://youtu.be/X0oXMdtUDwo?si=JBqdu2g0ktKC4DNf"/>
+    <hyperlink ref="E278" r:id="rId617" display="https://www.geeksforgeeks.org/largest-bst-binary-tree-set-2/"/>
+    <hyperlink ref="C279" r:id="rId618"/>
+    <hyperlink ref="D279" r:id="rId619" display="https://youtu.be/cX_kPV_foZc?si=vm8U3w99lvp7UPpc"/>
+    <hyperlink ref="E279" r:id="rId620" display="https://www.geeksforgeeks.org/lowest-common-ancestor-in-a-binary-search-tree/"/>
+    <hyperlink ref="C280" r:id="rId621"/>
+    <hyperlink ref="D280" r:id="rId622" display="https://youtu.be/18w8VduomfI?si=KJ0QdPfLdk6r30Sx"/>
+    <hyperlink ref="E280" r:id="rId623" display="https://www.geeksforgeeks.org/merge-two-bsts-with-limited-extra-space/"/>
+    <hyperlink ref="C281" r:id="rId624"/>
+    <hyperlink ref="D281" r:id="rId625" display="https://youtu.be/SXKAD2svfmI?si=802ib5wC0gtY44eH"/>
+    <hyperlink ref="E281" r:id="rId626" display="https://www.geeksforgeeks.org/inorder-predecessor-successor-given-key-bst/"/>
+    <hyperlink ref="C282" r:id="rId627"/>
+    <hyperlink ref="E282" r:id="rId628" display="https://www.geeksforgeeks.org/populate-inorder-successor-for-all-nodes/"/>
+    <hyperlink ref="C283" r:id="rId629"/>
+    <hyperlink ref="D283" r:id="rId630" display="https://youtu.be/7vVEJwVvAlI?si=Uwd3HoE8H_BhHFb0"/>
+    <hyperlink ref="E283" r:id="rId631" display="https://www.geeksforgeeks.org/transform-bst-sum-tree/"/>
+    <hyperlink ref="C284" r:id="rId632"/>
+    <hyperlink ref="D284" r:id="rId633" display="https://youtu.be/kouxiP_H5WE?si=wjgRijNs4nuSCHXn"/>
+    <hyperlink ref="E284" r:id="rId634" display="https://www.geeksforgeeks.org/deletion-in-binary-search-tree/"/>
+    <hyperlink ref="C286" r:id="rId635"/>
+    <hyperlink ref="D286" r:id="rId636" display="https://youtu.be/aZNaLrVebKQ?si=gAB4STDbhesQVKi0"/>
+    <hyperlink ref="E286" r:id="rId637" display="https://www.geeksforgeeks.org/construct-tree-from-given-inorder-and-preorder-traversal/"/>
+    <hyperlink ref="C287" r:id="rId638"/>
+    <hyperlink ref="D287" r:id="rId639" display="https://youtu.be/LgLRTaEMRVc?si=-Lc1FKuOxYBj4n6u"/>
+    <hyperlink ref="E287" r:id="rId640" display="https://www.geeksforgeeks.org/construct-a-binary-tree-from-postorder-and-inorder/"/>
+    <hyperlink ref="C288" r:id="rId641"/>
+    <hyperlink ref="D288" r:id="rId642" display="https://youtu.be/UmJT3j26t1I?si=tvJcbXtbATGbAUYG"/>
+    <hyperlink ref="E288" r:id="rId643" display="https://www.geeksforgeeks.org/construct-bst-from-given-preorder-traversa/"/>
+    <hyperlink ref="C289" r:id="rId644"/>
+    <hyperlink ref="E289" r:id="rId645" display="https://www.geeksforgeeks.org/construct-a-binary-tree-from-parent-array-representation/"/>
+    <hyperlink ref="C291" r:id="rId646"/>
+    <hyperlink ref="D291" r:id="rId647" display="https://youtu.be/-YbXySKJsX8?si=7GAc6pJLr12-MB1Y"/>
+    <hyperlink ref="E291" r:id="rId648" display="https://www.geeksforgeeks.org/serialize-deserialize-binary-tree/"/>
+    <hyperlink ref="C292" r:id="rId649"/>
+    <hyperlink ref="E292" r:id="rId650" display="https://www.geeksforgeeks.org/find-largest-subtree-sum-tree/"/>
+    <hyperlink ref="C293" r:id="rId651"/>
+    <hyperlink ref="D293" r:id="rId652" display="https://youtu.be/DBxCv9NpPYM?si=jX3oFEBSEGDVyDQF"/>
+    <hyperlink ref="E293" r:id="rId653" display="https://www.geeksforgeeks.org/maximum-sum-nodes-binary-tree-no-two-adjacent/"/>
+    <hyperlink ref="C294" r:id="rId654"/>
+    <hyperlink ref="D294" r:id="rId655" display="https://youtu.be/kn0Z5_qPPzY?si=5hSUj98E7uOL1JXP"/>
+    <hyperlink ref="E294" r:id="rId656" display="https://www.geeksforgeeks.org/find-duplicate-subtrees/"/>
+    <hyperlink ref="C295" r:id="rId657"/>
+    <hyperlink ref="D295" r:id="rId658" display="https://youtu.be/sWf7k1x9XR4?si=fuqHbNz-Kw01_dI1"/>
+    <hyperlink ref="E295" r:id="rId659" display="https://www.geeksforgeeks.org/flatten-a-binary-tree-into-linked-list/"/>
+    <hyperlink ref="C298" r:id="rId660"/>
+    <hyperlink ref="D298" r:id="rId661" display="https://youtu.be/YK78FU5Ffjw?si=b9cfoplt08JA0xJQ"/>
+    <hyperlink ref="E298" r:id="rId662" display="https://www.geeksforgeeks.org/write-a-c-program-to-print-all-permutations-of-a-given-string/"/>
+    <hyperlink ref="C299" r:id="rId663"/>
+    <hyperlink ref="D299" r:id="rId664" display="https://youtu.be/qhBVWf0YafA?si=2t9tPdRW_8ySW1C3"/>
+    <hyperlink ref="E299" r:id="rId665" display="https://www.geeksforgeeks.org/distinct-permutations-string-set-2/"/>
+    <hyperlink ref="C300" r:id="rId666"/>
+    <hyperlink ref="D300" r:id="rId667" display="https://youtu.be/OyZFFqQtu98?si=h4ntlYqyMU635DUw"/>
+    <hyperlink ref="E300" r:id="rId668" display="https://www.geeksforgeeks.org/combinational-sum/"/>
+    <hyperlink ref="C301" r:id="rId669"/>
+    <hyperlink ref="D301" r:id="rId670" display="https://youtu.be/G1fRTGRxXU8?si=CqK5qT_w7EcOkAEh"/>
+    <hyperlink ref="E301" r:id="rId671" display="https://www.geeksforgeeks.org/combinational-sum/"/>
+    <hyperlink ref="C302" r:id="rId672"/>
+    <hyperlink ref="E302" r:id="rId673" display="https://www.geeksforgeeks.org/all-unique-combinations-whose-sum-equals-to-k/"/>
+    <hyperlink ref="C303" r:id="rId674"/>
+    <hyperlink ref="D303" r:id="rId675" display="https://youtu.be/bLGZhJlt4y0?si=bMDZAraICwrxmTnq"/>
+    <hyperlink ref="E303" r:id="rId676" display="https://www.geeksforgeeks.org/rat-in-a-maze/"/>
+    <hyperlink ref="C304" r:id="rId677"/>
+    <hyperlink ref="D304" r:id="rId678" display="https://youtu.be/9ByWqPzfXDU?si=HVyZBiY385QXDma5"/>
+    <hyperlink ref="E304" r:id="rId679" display="https://www.geeksforgeeks.org/find-possible-words-phone-digits/"/>
+    <hyperlink ref="C305" r:id="rId680"/>
+    <hyperlink ref="D305" r:id="rId681" display="https://youtu.be/rYkfBRtMJr8?si=xdRYuVuGFT0hm2UI"/>
+    <hyperlink ref="E305" r:id="rId682" display="https://www.geeksforgeeks.org/backtracking-to-find-all-subsets/"/>
+    <hyperlink ref="C306" r:id="rId683"/>
+    <hyperlink ref="D306" r:id="rId684" display="https://youtu.be/h4zNvA4lbtc?si=uTv2-Y2ji1klfWgb"/>
+    <hyperlink ref="E306" r:id="rId685" display="https://www.geeksforgeeks.org/find-all-unique-subsets-of-a-given-set/"/>
+    <hyperlink ref="C307" r:id="rId686"/>
+    <hyperlink ref="D307" r:id="rId687" display="https://youtu.be/i05Ju7AftcM?si=rSa6wrmVJ8vvkLLz"/>
+    <hyperlink ref="E307" r:id="rId688" display="https://www.geeksforgeeks.org/n-queen-problem-backtracking-3/"/>
+    <hyperlink ref="C308" r:id="rId689"/>
+    <hyperlink ref="C309" r:id="rId690"/>
+    <hyperlink ref="D309" r:id="rId691" display="https://youtu.be/Ya_16rXu7W8?si=c6ZdSR9XKDv4D-gR"/>
+    <hyperlink ref="E309" r:id="rId692" display="https://www.geeksforgeeks.org/print-possible-strings-can-made-placing-spaces/"/>
+    <hyperlink ref="C310" r:id="rId693"/>
+    <hyperlink ref="D310" r:id="rId694" display="https://youtu.be/s9fokUqJ76A?si=zfcDWcp1AqqDy5cG"/>
+    <hyperlink ref="E310" r:id="rId695" display="https://www.geeksforgeeks.org/print-all-combinations-of-balanced-parentheses/"/>
+    <hyperlink ref="C311" r:id="rId696"/>
+    <hyperlink ref="D311" r:id="rId697" display="https://youtu.be/XU4inpwKt8A?si=lm9MpSALwsn4roQo"/>
+    <hyperlink ref="E311" r:id="rId698" display="https://www.geeksforgeeks.org/program-generate-possible-valid-ip-addresses-given-string/"/>
+    <hyperlink ref="C312" r:id="rId699"/>
+    <hyperlink ref="D312" r:id="rId700" display="https://youtu.be/FWAIf_EVUKE?si=q2DUJbZj1T6seOwb"/>
+    <hyperlink ref="E312" r:id="rId701" display="https://www.geeksforgeeks.org/sudoku-backtracking-7/"/>
+    <hyperlink ref="C313" r:id="rId702"/>
+    <hyperlink ref="D313" r:id="rId703" display="https://youtu.be/wT7gcXLYoao?si=cG3Kl4gKxBl92-1m"/>
+    <hyperlink ref="E313" r:id="rId704" display="https://www.geeksforgeeks.org/find-the-k-th-permutation-sequence-of-first-n-natural-numbers/"/>
+    <hyperlink ref="C314" r:id="rId705" display="https://www.geeksforgeeks.org/problems/word-search"/>
+    <hyperlink ref="D314" r:id="rId706" display="https://youtu.be/pfiQ_PS1g8E?si=NSwX3AHJpS6lGme4"/>
+    <hyperlink ref="E314" r:id="rId707" display="https://www.geeksforgeeks.org/search-a-word-in-a-2d-grid-of-characters/"/>
+    <hyperlink ref="C315" r:id="rId708"/>
+    <hyperlink ref="D315" r:id="rId709" display="https://youtu.be/WBgsABoClE0?si=FBXsqWuBLwm75E81"/>
+    <hyperlink ref="E315" r:id="rId710" display="https://www.geeksforgeeks.org/palindrome-partitioning-dp-17/"/>
+    <hyperlink ref="C316" r:id="rId711"/>
+    <hyperlink ref="D316" r:id="rId712" display="https://youtu.be/qB0zZpBJlh8?si=VBKh6H4NSYT6qYVO"/>
+    <hyperlink ref="E316" r:id="rId713" display="https://www.geeksforgeeks.org/decode-string-recursively-encoded-count-followed-substring/"/>
+    <hyperlink ref="C317" r:id="rId714"/>
+    <hyperlink ref="D317" r:id="rId715" display="https://youtu.be/4eOPYDOiwFo?si=VIbEA8JDKDOvwRuD"/>
+    <hyperlink ref="E317" r:id="rId716" display="https://www.geeksforgeeks.org/permute-string-changing-case/"/>
+    <hyperlink ref="C318" r:id="rId717"/>
+    <hyperlink ref="D318" r:id="rId718" display="https://youtu.be/xlPIH9216Ak?si=NpzDre5ux8rDgSdQ"/>
+    <hyperlink ref="E318" r:id="rId719" display="https://www.geeksforgeeks.org/check-given-string-sum-string/"/>
+    <hyperlink ref="C319" r:id="rId720"/>
+    <hyperlink ref="D319" r:id="rId721" display="https://youtu.be/-3rVMYGBwO0?si=w-NmOX7Or4vw8D4T"/>
+    <hyperlink ref="E319" r:id="rId722" display="https://www.geeksforgeeks.org/boggle-find-possible-words-board-characters/"/>
+    <hyperlink ref="C320" r:id="rId723"/>
+    <hyperlink ref="D320" r:id="rId724" display="https://www.youtube.com/live/GstuPf5u3lg?si=9Ymg0mpYPLzeJ38y"/>
+    <hyperlink ref="E320" r:id="rId725" display="https://www.geeksforgeeks.org/find-maximum-number-possible-by-doing-at-most-k-swaps/"/>
+    <hyperlink ref="C321" r:id="rId726"/>
+    <hyperlink ref="D321" r:id="rId727" display="https://youtu.be/mBk4I0X46oI?si=uA-5-uc7zAgLloIe"/>
+    <hyperlink ref="E321" r:id="rId728" display="https://www.geeksforgeeks.org/partition-set-k-subsets-equal-sum/"/>
+    <hyperlink ref="D323" r:id="rId729" display="https://youtu.be/M3_pLsDdeuU?si=SItRP4M088yoch07"/>
+    <hyperlink ref="C324" r:id="rId730"/>
+    <hyperlink ref="D324" r:id="rId731" display="https://youtu.be/-tgVpUgsQ5k?si=Lss9L2Zdy8Gu6BOg"/>
+    <hyperlink ref="E324" r:id="rId732" display="https://www.geeksforgeeks.org/breadth-first-search-or-bfs-for-a-graph/"/>
+    <hyperlink ref="C325" r:id="rId733"/>
+    <hyperlink ref="D325" r:id="rId734" display="https://youtu.be/Qzf1a--rhp8?si=aGYfCnBcl_NDSFad"/>
+    <hyperlink ref="E325" r:id="rId735" display="https://www.geeksforgeeks.org/depth-first-search-or-dfs-for-a-graph/"/>
+    <hyperlink ref="C326" r:id="rId736"/>
+    <hyperlink ref="D326" r:id="rId737" display="https://youtu.be/9twcmtQj4DU?si=8a8yz9stT7quiRiP"/>
+    <hyperlink ref="E326" r:id="rId738" display="https://www.geeksforgeeks.org/detect-cycle-in-a-graph/"/>
+    <hyperlink ref="C327" r:id="rId739"/>
+    <hyperlink ref="D327" r:id="rId740" display="https://youtu.be/zQ3zgFypzX4?si=oXS_VKyOM-oL_4yz"/>
+    <hyperlink ref="E327" r:id="rId741" display="https://www.geeksforgeeks.org/detect-cycle-undirected-graph/"/>
+    <hyperlink ref="C328" r:id="rId742"/>
+    <hyperlink ref="E328" r:id="rId743" display="https://www.geeksforgeeks.org/detect-negative-cycle-graph-bellman-ford/"/>
+    <hyperlink ref="C330" r:id="rId744"/>
+    <hyperlink ref="D330" r:id="rId745" display="https://youtu.be/lea-Wl_uWXY?si=g2dSfr4n7yGr1rmo"/>
+    <hyperlink ref="E330" r:id="rId746" display="https://www.geeksforgeeks.org/strongly-connected-components/"/>
+    <hyperlink ref="C331" r:id="rId747"/>
+    <hyperlink ref="D331" r:id="rId748" display="https://youtu.be/ACzkVtewUYA?si=N0HPRxovroHd2XNQ"/>
+    <hyperlink ref="E331" r:id="rId749" display="https://pnext1.geeksforgeeks.org/problems/number-of-provinces/1?page=1&amp;category%5b%5d=Backtracking&amp;sortBy=submissions"/>
+    <hyperlink ref="C332" r:id="rId750"/>
+    <hyperlink ref="D332" r:id="rId751" display="https://youtu.be/muncqlKJrH0?si=YO3SUPZz6yDpCTM8"/>
+    <hyperlink ref="E332" r:id="rId752" display="https://www.geeksforgeeks.org/find-the-number-of-islands-using-dfs/"/>
+    <hyperlink ref="C333" r:id="rId753"/>
+    <hyperlink ref="D333" r:id="rId754" display="https://youtu.be/7zmgQSJghpo?si=T3zcl9BeVooJBUAX"/>
+    <hyperlink ref="E333" r:id="rId755" display="https://www.geeksforgeeks.org/find-the-number-of-distinct-islands-in-a-2d-matrix/"/>
+    <hyperlink ref="C334" r:id="rId756"/>
+    <hyperlink ref="D334" r:id="rId757" display="https://youtu.be/X8k48xek8g8?si=UILPOo-_LidtdV_k"/>
+    <hyperlink ref="E334" r:id="rId758" display="https://www.geeksforgeeks.org/find-number-of-closed-islands-in-given-matrix/"/>
+    <hyperlink ref="C336" r:id="rId759"/>
+    <hyperlink ref="D336" r:id="rId760" display="https://youtu.be/-vu34sct1g8?si=G9gY0BZEWVQf810J"/>
+    <hyperlink ref="E336" r:id="rId761" display="https://www.geeksforgeeks.org/bipartite-graph/"/>
+    <hyperlink ref="C337" r:id="rId762"/>
+    <hyperlink ref="D337" r:id="rId763" display="https://youtu.be/wuVwUK25Rfc?si=CYcBDjL6ARNTh1FG"/>
+    <hyperlink ref="E337" r:id="rId764" display="https://www.geeksforgeeks.org/m-coloring-problem/"/>
+    <hyperlink ref="C338" r:id="rId765"/>
+    <hyperlink ref="D338" r:id="rId766" display="https://youtu.be/C4gxoTaI71U?si=k1As9n_SZUk7dYJJ"/>
+    <hyperlink ref="E338" r:id="rId767" display="https://www.geeksforgeeks.org/shortest-path-unweighted-graph/"/>
+    <hyperlink ref="C339" r:id="rId768"/>
+    <hyperlink ref="D339" r:id="rId769" display="https://youtu.be/ZUFQfFaU-8U?si=LW37HXwpS6wWWgTC"/>
+    <hyperlink ref="E339" r:id="rId770" display="https://www.geeksforgeeks.org/shortest-path-for-directed-acyclic-graphs/"/>
+    <hyperlink ref="C340" r:id="rId771"/>
+    <hyperlink ref="D340" r:id="rId772" display="https://youtu.be/V6H1qAeB-l4?si=W36zrJBLarmVkn_C"/>
+    <hyperlink ref="E340" r:id="rId773" display="https://www.geeksforgeeks.org/dijkstras-shortest-path-algorithm-greedy-algo-7/"/>
+    <hyperlink ref="C341" r:id="rId774"/>
+    <hyperlink ref="D341" r:id="rId775" display="https://www.youtube.com/live/6lgT0vEhMPo?si=pTJ2-6RIZfCDjz0X"/>
+    <hyperlink ref="E341" r:id="rId776" display="https://www.geeksforgeeks.org/minimum-steps-reach-target-knight/"/>
+    <hyperlink ref="C342" r:id="rId777"/>
+    <hyperlink ref="E342" r:id="rId778" display="https://www.geeksforgeeks.org/shortest-path-from-a-source-cell-to-a-destination-cell-of-a-binary-matrix-through-cells-consisting-only-of-1s/"/>
+    <hyperlink ref="C343" r:id="rId779"/>
+    <hyperlink ref="D343" r:id="rId780" display="https://youtu.be/Eso1Lu4mtmU?si=EqoQnXHqvPXzrtDP"/>
+    <hyperlink ref="E343" r:id="rId781" display="https://www.geeksforgeeks.org/find-if-there-is-a-path-between-two-vertices-in-an-undirected-graph/"/>
+    <hyperlink ref="C344" r:id="rId782"/>
+    <hyperlink ref="E344" r:id="rId783" display="https://www.geeksforgeeks.org/maximum-time-required-for-all-patients-to-get-infected/"/>
+    <hyperlink ref="C345" r:id="rId784"/>
+    <hyperlink ref="D345" r:id="rId785" display="https://youtu.be/t1shZ8_s6jc?si=xHiW9k7kJJ_tUTI5"/>
+    <hyperlink ref="E345" r:id="rId786" display="https://www.geeksforgeeks.org/min-cost-path-dp-6/"/>
+    <hyperlink ref="C346" r:id="rId787"/>
+    <hyperlink ref="D346" r:id="rId788" display="https://youtu.be/tRPda0rcf8E?si=qMWyd0E8oMQ7WIvy"/>
+    <hyperlink ref="E346" r:id="rId789" display="https://takeuforward.org/graph/word-ladder-i-g-29/"/>
+    <hyperlink ref="C347" r:id="rId790"/>
+    <hyperlink ref="D347" r:id="rId791" display="https://youtu.be/DREutrv2XD0?si=QfIrMBzjrv0paKAJ"/>
+    <hyperlink ref="E347" r:id="rId792" display="https://www.geeksforgeeks.org/word-ladder-length-of-shortest-chain-to-reach-a-target-word/"/>
+    <hyperlink ref="C348" r:id="rId793"/>
+    <hyperlink ref="D348" r:id="rId794" display="https://youtu.be/YbY8cVwWAvw?si=qeBBm6l3SrryejiB"/>
+    <hyperlink ref="E348" r:id="rId795" display="https://www.geeksforgeeks.org/floyd-warshall-algorithm-dp-16/"/>
+    <hyperlink ref="C349" r:id="rId796"/>
+    <hyperlink ref="D349" r:id="rId797" display="https://youtu.be/0vVofAhAYjc?si=e1hQOH4PcFbO_QUG"/>
+    <hyperlink ref="E349" r:id="rId798" display="https://www.geeksforgeeks.org/bellman-ford-algorithm-dp-23/"/>
+    <hyperlink ref="C351" r:id="rId799"/>
+    <hyperlink ref="D351" r:id="rId800" display="https://youtu.be/C-2_uSRli8o?si=z2XOpxmnekERJrxc"/>
+    <hyperlink ref="E351" r:id="rId801" display="https://www.geeksforgeeks.org/flood-fill-algorithm/"/>
+    <hyperlink ref="C352" r:id="rId802"/>
+    <hyperlink ref="E352" r:id="rId803" display="https://www.geeksforgeeks.org/given-matrix-o-x-replace-o-x-surrounded-x/"/>
+    <hyperlink ref="C353" r:id="rId804"/>
+    <hyperlink ref="E353" r:id="rId805" display="https://www.geeksforgeeks.org/find-length-largest-region-boolean-matrix/"/>
+    <hyperlink ref="C354" r:id="rId806"/>
+    <hyperlink ref="D354" r:id="rId807" display="https://youtu.be/yf3oUhkvqA0?si=l_DQbwT42fy1ThaI"/>
+    <hyperlink ref="E354" r:id="rId808" display="https://www.geeksforgeeks.org/minimum-time-required-so-that-all-oranges-become-rotten/"/>
+    <hyperlink ref="C356" r:id="rId809"/>
+    <hyperlink ref="D356" r:id="rId810" display="https://youtu.be/5lZ0iJMrUMk?si=d8Saw4jmgjKmfILx"/>
+    <hyperlink ref="E356" r:id="rId811" display="https://www.geeksforgeeks.org/topological-sorting/"/>
+    <hyperlink ref="C357" r:id="rId812"/>
+    <hyperlink ref="E357" r:id="rId813" display="https://pnext2.geeksforgeeks.org/problems/prerequisite-tasks/1?page=1&amp;company%5b%5d=Apple&amp;sortBy=submissions"/>
+    <hyperlink ref="C358" r:id="rId814"/>
+    <hyperlink ref="D358" r:id="rId815" display="https://youtu.be/WAOfKpxYHR8?si=WIg-894F_ejz1hgv"/>
+    <hyperlink ref="E358" r:id="rId816" display="https://www.geeksforgeeks.org/find-whether-it-is-possible-to-finish-all-tasks-or-not-from-given-dependencies/"/>
+    <hyperlink ref="C359" r:id="rId817"/>
+    <hyperlink ref="D359" r:id="rId818" display="https://youtu.be/WAOfKpxYHR8?si=WIg-894F_ejz1hgv"/>
+    <hyperlink ref="E359" r:id="rId819" display="https://www.geeksforgeeks.org/find-the-ordering-of-tasks-from-given-dependencies/"/>
+    <hyperlink ref="C360" r:id="rId820"/>
+    <hyperlink ref="D360" r:id="rId821" display="https://youtu.be/2gtg3VsDGyc?si=yw-aqlNDy3mCHOj5"/>
+    <hyperlink ref="E360" r:id="rId822" display="https://www.geeksforgeeks.org/eventual-safe-states/"/>
+    <hyperlink ref="C361" r:id="rId823"/>
+    <hyperlink ref="D361" r:id="rId824" display="https://youtu.be/U3N_je7tWAs?si=3QjjfX39WxlhedeU"/>
+    <hyperlink ref="E361" r:id="rId825" display="https://www.geeksforgeeks.org/given-sorted-dictionary-find-precedence-characters/"/>
+    <hyperlink ref="C363" r:id="rId826"/>
+    <hyperlink ref="D363" r:id="rId827" display="https://youtu.be/ZSPjZuZWCME?si=qz-SbjuFnphj89qo"/>
+    <hyperlink ref="E363" r:id="rId828" display="https://www.geeksforgeeks.org/kruskals-minimum-spanning-tree-algorithm-greedy-algo-2/"/>
+    <hyperlink ref="C364" r:id="rId829"/>
+    <hyperlink ref="D364" r:id="rId830" display="https://youtu.be/DMnDM_sxVig?si=_xwNmqyl69ykMMNz"/>
+    <hyperlink ref="E364" r:id="rId831" display="https://www.geeksforgeeks.org/kruskals-minimum-spanning-tree-algorithm-greedy-algo-2/"/>
+    <hyperlink ref="C365" r:id="rId832"/>
+    <hyperlink ref="E365" r:id="rId833" display="https://www.geeksforgeeks.org/minimum-cost-connect-cities/"/>
+    <hyperlink ref="C366" r:id="rId834"/>
+    <hyperlink ref="E366" r:id="rId835" display="https://www.geeksforgeeks.org/minimum-cost-required-to-connect-all-houses-in-a-city/"/>
+    <hyperlink ref="C367" r:id="rId836"/>
+    <hyperlink ref="E367" r:id="rId837" display="https://www.geeksforgeeks.org/water-connection-problem/"/>
+    <hyperlink ref="D369" r:id="rId838" display="https://youtu.be/L1T4AB8xBcw?si=aeusCwB3GXg7GprE"/>
+    <hyperlink ref="E369" r:id="rId839" display="https://www.geeksforgeeks.org/disjoint-set-data-structures/"/>
+    <hyperlink ref="D370" r:id="rId840" display="https://youtu.be/L1T4AB8xBcw?si=aeusCwB3GXg7GprE"/>
+    <hyperlink ref="E370" r:id="rId841" display="https://www.geeksforgeeks.org/union-by-rank-and-path-compression-in-union-find-algorithm/"/>
+    <hyperlink ref="C371" r:id="rId842"/>
+    <hyperlink ref="D371" r:id="rId843" display="https://youtu.be/vadly9uWMPU?si=xqtEXZf4OU7HFDru"/>
+    <hyperlink ref="E371" r:id="rId844" display="https://www.geeksforgeeks.org/minimize-count-of-connections-required-to-be-rearranged-to-make-all-the-computers-connected/"/>
+    <hyperlink ref="C372" r:id="rId845"/>
+    <hyperlink ref="D372" r:id="rId846" display="https://youtu.be/kFe_LRWuZjE?si=UUGOKxVpWXgSA3-m"/>
+    <hyperlink ref="E372" r:id="rId847" display="https://www.geeksforgeeks.org/minimum-number-swaps-required-sort-array/"/>
+    <hyperlink ref="C373" r:id="rId848"/>
+    <hyperlink ref="C374" r:id="rId849"/>
+    <hyperlink ref="E374" r:id="rId850" display="https://www.geeksforgeeks.org/find-number-pairs-xy-yx/"/>
+    <hyperlink ref="C375" r:id="rId851"/>
+    <hyperlink ref="D375" r:id="rId852" display="https://youtu.be/Rn6B-Q4SNyA?si=KaMazDJMo73etDEb"/>
+    <hyperlink ref="E375" r:id="rId853" display="https://www.geeksforgeeks.org/find-the-number-of-islands-using-disjoint-set/"/>
+    <hyperlink ref="C376" r:id="rId854" display="https://leetcode.com/problems/making-a-large-island/solutions/"/>
+    <hyperlink ref="D376" r:id="rId855" display="https://youtu.be/fi-_r0MtL5I?si=-Fyp3xqjyPhs6hwg"/>
+    <hyperlink ref="E376" r:id="rId856" display="https://www.geeksforgeeks.org/maximum-connected-group-making-a-large-island/"/>
+    <hyperlink ref="C378" r:id="rId857"/>
+    <hyperlink ref="D378" r:id="rId858" display="https://youtu.be/qrAub5z8FeA?si=X1hIai2nrqJBxs5U"/>
+    <hyperlink ref="E378" r:id="rId859" display="https://www.geeksforgeeks.org/bridge-in-a-graph/"/>
+    <hyperlink ref="C379" r:id="rId860"/>
+    <hyperlink ref="D379" r:id="rId861" display="https://youtu.be/j1QDfU21iZk?si=YzffjCCnc3tpTCAS"/>
+    <hyperlink ref="E379" r:id="rId862" display="https://www.geeksforgeeks.org/articulation-points-or-cut-vertices-in-a-graph/"/>
+    <hyperlink ref="C380" r:id="rId863"/>
+    <hyperlink ref="D380" r:id="rId864" display="https://youtu.be/HsBefuOqkd4?si=YSJZK1P5x22IDyQU"/>
+    <hyperlink ref="E380" r:id="rId865" display="https://www.geeksforgeeks.org/find-all-critical-connections-in-the-graph/"/>
+    <hyperlink ref="C381" r:id="rId866"/>
+    <hyperlink ref="D381" r:id="rId867" display="https://youtu.be/R6uoSjZ2imo?si=rKK-k7JxRlgFJNgj"/>
+    <hyperlink ref="E381" r:id="rId868" display="https://www.geeksforgeeks.org/strongly-connected-components/"/>
+    <hyperlink ref="C382" r:id="rId869"/>
+    <hyperlink ref="D382" r:id="rId870" display="https://youtu.be/UJTVaSITcYY?si=hLAyO48WqDXDDH9h"/>
+    <hyperlink ref="E382" r:id="rId871" display="https://www.geeksforgeeks.org/boggle-find-possible-words-board-characters/"/>
+    <hyperlink ref="C383" r:id="rId872"/>
+    <hyperlink ref="E383" r:id="rId873" display="https://www.geeksforgeeks.org/boggle-find-possible-words-board-characters/"/>
+    <hyperlink ref="C386" r:id="rId874"/>
+    <hyperlink ref="D386" r:id="rId875" display="https://youtu.be/_6QpiqTw_ew?si=xUX4W2QueKEKPr7S"/>
+    <hyperlink ref="E386" r:id="rId876" display="https://www.geeksforgeeks.org/minimum-number-of-jumps-to-reach-end-of-a-given-array/"/>
+    <hyperlink ref="C387" r:id="rId877"/>
+    <hyperlink ref="E387" r:id="rId878" display="https://www.geeksforgeeks.org/minimize-operations-required-to-obtain-n/"/>
+    <hyperlink ref="C388" r:id="rId879"/>
+    <hyperlink ref="E388" r:id="rId880" display="https://www.geeksforgeeks.org/minimize-sum-product-two-arrays-permutations-allowed/"/>
+    <hyperlink ref="C389" r:id="rId881"/>
+    <hyperlink ref="E389" r:id="rId882" display="https://www.geeksforgeeks.org/find-the-largest-number-with-given-number-of-digits-and-sum-of-digits/"/>
+    <hyperlink ref="C390" r:id="rId883"/>
+    <hyperlink ref="E390" r:id="rId884" display="https://www.geeksforgeeks.org/lemonade-stand-change-challenge/"/>
+    <hyperlink ref="C391" r:id="rId885"/>
+    <hyperlink ref="D391" r:id="rId886" display="https://youtu.be/jD_D-b6t_eU?si=2zgyQVT6B0-aSO06"/>
+    <hyperlink ref="E391" r:id="rId887" display="https://www.geeksforgeeks.org/activity-selection-problem-greedy-algo-1/"/>
+    <hyperlink ref="C392" r:id="rId888"/>
+    <hyperlink ref="D392" r:id="rId889" display="https://youtu.be/II6ziNnub1Q?si=nyCFIwB6nl2-LOZo"/>
+    <hyperlink ref="E392" r:id="rId890" display="https://takeuforward.org/data-structure/n-meetings-in-one-room/"/>
+    <hyperlink ref="C393" r:id="rId891"/>
+    <hyperlink ref="D393" r:id="rId892" display="https://youtu.be/dxVcMDI7vyI?si=DCFL2eWvpXNvz3dm"/>
+    <hyperlink ref="E393" r:id="rId893" display="https://www.geeksforgeeks.org/minimum-number-platforms-required-railwaybus-station/"/>
+    <hyperlink ref="C394" r:id="rId894"/>
+    <hyperlink ref="E394" r:id="rId895" display="https://www.geeksforgeeks.org/minimize-the-maximum-difference-between-the-heights/"/>
+    <hyperlink ref="C395" r:id="rId896"/>
+    <hyperlink ref="D395" r:id="rId897" display="https://youtu.be/mVg9CfJvayM?si=ZYElbpIWyYE3yEjA"/>
+    <hyperlink ref="E395" r:id="rId898" display="https://www.geeksforgeeks.org/greedy-algorithm-to-find-minimum-number-of-coins/"/>
+    <hyperlink ref="C396" r:id="rId899"/>
+    <hyperlink ref="D396" r:id="rId900" display="https://youtu.be/LjPx4wQaRIs?si=QuVNrXDBmW0nqlfy"/>
+    <hyperlink ref="E396" r:id="rId901" display="https://www.geeksforgeeks.org/job-sequencing-problem/"/>
+    <hyperlink ref="C397" r:id="rId902"/>
+    <hyperlink ref="D397" r:id="rId903" display="https://youtu.be/F_DDzYnxO14?si=Aiem1u3s1CApvD1Q"/>
+    <hyperlink ref="E397" r:id="rId904" display="https://www.geeksforgeeks.org/fractional-knapsack-problem/"/>
+    <hyperlink ref="C398" r:id="rId905"/>
+    <hyperlink ref="D398" r:id="rId906" display="https://youtu.be/Yan0cv2cLy8?si=6gEyL0RDv97Ebo_S"/>
+    <hyperlink ref="E398" r:id="rId907" display="https://www.geeksforgeeks.org/minimum-number-of-jumps-to-reach-end-of-a-given-array/"/>
+    <hyperlink ref="C399" r:id="rId908"/>
+    <hyperlink ref="D399" r:id="rId909" display="https://youtu.be/A8NUOmlwOlM?si=nSYNoRp7jNmzEZbk"/>
+    <hyperlink ref="E399" r:id="rId910" display="https://www.geeksforgeeks.org/insert-in-sorted-and-non-overlapping-interval-array/"/>
+    <hyperlink ref="C400" r:id="rId911"/>
+    <hyperlink ref="E400" r:id="rId912" display="https://www.geeksforgeeks.org/merging-intervals/"/>
+    <hyperlink ref="C401" r:id="rId913"/>
+    <hyperlink ref="D401" r:id="rId914" display="https://youtu.be/nONCGxWoUfM?si=CCH5fuaNR9Oh4SV9"/>
+    <hyperlink ref="E401" r:id="rId915" display="https://www.geeksforgeeks.org/find-non-overlapping-intervals-among-a-given-set-of-intervals/"/>
+    <hyperlink ref="C402" r:id="rId916"/>
+    <hyperlink ref="D402" r:id="rId917" display="https://youtu.be/_k_c9nqzKN0?si=8aU6CU030tv-stpm"/>
+    <hyperlink ref="E402" r:id="rId918" display="https://www.geeksforgeeks.org/connect-n-ropes-minimum-cost/"/>
+    <hyperlink ref="C403" r:id="rId919"/>
+    <hyperlink ref="E403" r:id="rId920" display="https://walkccc.me/LeetCode/problems/0763/"/>
+    <hyperlink ref="C404" r:id="rId921"/>
+    <hyperlink ref="E404" r:id="rId922" display="https://prepfortech.in/leetcode-solutions/cinema-seat-allocation/"/>
+    <hyperlink ref="C405" r:id="rId923"/>
+    <hyperlink ref="E405" r:id="rId924" display="https://www.geeksforgeeks.org/maximum-length-chain-of-pairs-dp-20/"/>
+    <hyperlink ref="C406" r:id="rId925"/>
+    <hyperlink ref="D406" r:id="rId926" display="https://youtu.be/wkDfsKijrZ8?si=M76SonbMLKKgwvoL"/>
+    <hyperlink ref="E406" r:id="rId927" display="https://www.geeksforgeeks.org/minimum-number-of-parentheses-to-be-added-to-make-it-valid/"/>
+    <hyperlink ref="C407" r:id="rId928"/>
+    <hyperlink ref="E407" r:id="rId929" display="https://www.geeksforgeeks.org/program-for-shortest-job-first-or-sjf-cpu-scheduling-set-1-non-preemptive/"/>
+    <hyperlink ref="C408" r:id="rId930"/>
+    <hyperlink ref="D408" r:id="rId931" display="https://youtu.be/xDEuM5qa0zg?si=lm-_MF96z7x2k-FC"/>
+    <hyperlink ref="E408" r:id="rId932" display="https://www.geeksforgeeks.org/lru-cache-implementation/"/>
+    <hyperlink ref="D411" r:id="rId933" display="https://youtu.be/tyB0ztf0DNY?si=g1XFqILApUcgKtJC"/>
+    <hyperlink ref="C413" r:id="rId934"/>
+    <hyperlink ref="E413" r:id="rId935" display="https://www.geeksforgeeks.org/count-number-of-ways-to-cover-a-distance/"/>
+    <hyperlink ref="C414" r:id="rId936"/>
+    <hyperlink ref="D414" r:id="rId937" display="https://youtu.be/mLfjzJsN8us?si=CtLuQbpWqlseteUe"/>
+    <hyperlink ref="E414" r:id="rId938" display="https://www.geeksforgeeks.org/count-ways-reach-nth-stair/"/>
+    <hyperlink ref="C415" r:id="rId939"/>
+    <hyperlink ref="D415" r:id="rId940" display="https://youtu.be/mLfjzJsN8us?si=CtLuQbpWqlseteUe"/>
+    <hyperlink ref="E415" r:id="rId941" display="https://www.geeksforgeeks.org/count-ways-reach-nth-stair/"/>
+    <hyperlink ref="C416" r:id="rId942"/>
+    <hyperlink ref="E416" r:id="rId943" display="https://www.geeksforgeeks.org/find-maximum-possible-stolen-value-houses/"/>
+    <hyperlink ref="C417" r:id="rId944"/>
+    <hyperlink ref="D417" r:id="rId945" display="https://youtu.be/3WaxQMELSkw?si=uGgE6spsNU-YYdHQ"/>
+    <hyperlink ref="C419" r:id="rId946"/>
+    <hyperlink ref="D419" r:id="rId947" display="https://youtu.be/sdE0A2Oxofw?si=k-DhYLU6A7eaUxPF"/>
+    <hyperlink ref="E419" r:id="rId948" display="https://www.geeksforgeeks.org/count-possible-paths-top-left-bottom-right-nxm-matrix/"/>
+    <hyperlink ref="C420" r:id="rId949"/>
+    <hyperlink ref="D420" r:id="rId950" display="https://youtu.be/TmhpgXScLyY?si=Z7i2x05K982xbodl"/>
+    <hyperlink ref="C421" r:id="rId951"/>
+    <hyperlink ref="E421" r:id="rId952" display="https://www.geeksforgeeks.org/count-possible-paths-top-left-bottom-right-nxm-matrix/"/>
+    <hyperlink ref="C422" r:id="rId953"/>
+    <hyperlink ref="D422" r:id="rId954" display="https://www.youtube.com/watch?v=_rgTlyky1uQ"/>
+    <hyperlink ref="C423" r:id="rId955"/>
+    <hyperlink ref="E423" r:id="rId956" display="https://www.geeksforgeeks.org/find-maximum-path-sum-in-a-binary-tree/"/>
+    <hyperlink ref="C424" r:id="rId957"/>
+    <hyperlink ref="D424" r:id="rId958" display="https://www.youtube.com/watch?v=SrP-PiLSYC0"/>
+    <hyperlink ref="C425" r:id="rId959"/>
+    <hyperlink ref="E425" r:id="rId960" display="https://www.geeksforgeeks.org/number-of-paths-with-exactly-k-coins/"/>
+    <hyperlink ref="C426" r:id="rId961"/>
+    <hyperlink ref="D426" r:id="rId962" display="https://youtu.be/N_aJ5qQbYA0?si=ezuW1n6Qa8XxTNEo"/>
+    <hyperlink ref="C427" r:id="rId963"/>
+    <hyperlink ref="C429" r:id="rId964"/>
+    <hyperlink ref="D429" r:id="rId965" display="https://youtu.be/fWX9xDmIzRI?si=JE2TrHBWy_MknoPu"/>
+    <hyperlink ref="C430" r:id="rId966"/>
+    <hyperlink ref="D430" r:id="rId967" display="https://youtu.be/ZHyb-A2Mte4?si=E2zp3ic9YMCmi1el"/>
+    <hyperlink ref="C431" r:id="rId968"/>
+    <hyperlink ref="D431" r:id="rId969" display="https://youtu.be/7win3dcgo3k?si=b7S5AhlT68DbwSRC"/>
+    <hyperlink ref="E431" r:id="rId970" display="https://www.geeksforgeeks.org/partition-problem-dp-18/"/>
+    <hyperlink ref="C432" r:id="rId971"/>
+    <hyperlink ref="D432" r:id="rId972" display="https://youtu.be/GS_OqZb2CWc?si=jtDc7dlrqIBDGkva"/>
+    <hyperlink ref="D433" r:id="rId973" display="https://youtu.be/zoilQD1kYSg?si=Dob0JEkW4sUmGoXn"/>
+    <hyperlink ref="C434" r:id="rId974"/>
+    <hyperlink ref="D434" r:id="rId975" display="https://youtu.be/GqOmJHQZivw?si=Z9uoyRurFlHaiwRs"/>
+    <hyperlink ref="E434" r:id="rId976" display="https://www.geeksforgeeks.org/0-1-knapsack-problem-dp-10/"/>
+    <hyperlink ref="C435" r:id="rId977"/>
+    <hyperlink ref="D435" r:id="rId978" display="https://youtu.be/GrMBfJNk_NY?si=i1ZMM-MkZu3TUA4w"/>
+    <hyperlink ref="C436" r:id="rId979"/>
+    <hyperlink ref="D436" r:id="rId980" display="https://youtu.be/HgyouUi11zk?si=lHMMApBzC27_NrBU"/>
+    <hyperlink ref="E436" r:id="rId981" display="https://www.geeksforgeeks.org/coin-change-dp-7/"/>
+    <hyperlink ref="C437" r:id="rId982"/>
+    <hyperlink ref="D437" r:id="rId983" display="https://youtu.be/myPeWb3Y68A?si=eeOZCGj3ebD3fay7"/>
+    <hyperlink ref="E437" r:id="rId984" display="https://www.geeksforgeeks.org/find-minimum-number-of-coins-that-make-a-change/"/>
+    <hyperlink ref="C438" r:id="rId985"/>
+    <hyperlink ref="D438" r:id="rId986" display="https://youtu.be/mO8XpGoJwuo?si=qNYFr6yJNxqmw4ky"/>
+    <hyperlink ref="C439" r:id="rId987"/>
+    <hyperlink ref="D439" r:id="rId988" display="https://youtu.be/b3GD8263-PQ?si=x22ue_uHcCp3vLdu"/>
+    <hyperlink ref="C440" r:id="rId989"/>
+    <hyperlink ref="C441" r:id="rId990"/>
+    <hyperlink ref="D441" r:id="rId991" display="https://youtu.be/OgvOZ6OrJoY?si=dmmo3by1GELu0E6u"/>
+    <hyperlink ref="E441" r:id="rId992" display="https://www.geeksforgeeks.org/unbounded-knapsack-repetition-items-allowed/"/>
+    <hyperlink ref="C443" r:id="rId993"/>
+    <hyperlink ref="D443" r:id="rId994" display="https://youtu.be/ekcwMsSIzVc?si=8zc9o-Q9JBpR_rLs"/>
+    <hyperlink ref="D444" r:id="rId995" display="https://youtu.be/IFfYfonAFGc?si=KQW5W74J8e_n_kXZ"/>
+    <hyperlink ref="C445" r:id="rId996"/>
+    <hyperlink ref="D445" r:id="rId997" display="https://youtu.be/y4vN0WNdrlg?si=1n-HYDfzakhkM-6W"/>
+    <hyperlink ref="E445" r:id="rId998" display="https://www.geeksforgeeks.org/longest-bitonic-subsequence-dp-15/"/>
+    <hyperlink ref="C446" r:id="rId999"/>
+    <hyperlink ref="D446" r:id="rId1000" display="https://youtu.be/gDuZwBW9VvM?si=1E77tHD7jaVItSLZ"/>
+    <hyperlink ref="C447" r:id="rId1001"/>
+    <hyperlink ref="D447" r:id="rId1002" display="https://youtu.be/YY8iBaYcc4g?si=SVp9w9fPBfUcqhqG"/>
+    <hyperlink ref="C448" r:id="rId1003"/>
+    <hyperlink ref="D448" r:id="rId1004" display="https://youtu.be/cKVl1TFdNXg?si=N8t9as5OGiHoVzrG"/>
+    <hyperlink ref="C450" r:id="rId1005" display="https://leetcode.com/problems/longest-common-subsequence/"/>
+    <hyperlink ref="D450" r:id="rId1006" display="https://youtu.be/NPZn9jBrX8U?si=c38YFd7X1c-QcPRq"/>
+    <hyperlink ref="E450" r:id="rId1007" display="https://www.geeksforgeeks.org/longest-common-subsequence-dp-4/"/>
+    <hyperlink ref="C451" r:id="rId1008"/>
+    <hyperlink ref="D451" r:id="rId1009" display="https://youtu.be/-zI4mrF2Pb4?si=VagQXphIzNfpH9su"/>
+    <hyperlink ref="E451" r:id="rId1010" display="https://www.geeksforgeeks.org/printing-longest-common-subsequence/"/>
+    <hyperlink ref="C452" r:id="rId1011"/>
+    <hyperlink ref="D452" r:id="rId1012" display="https://youtu.be/6i_T5kkfv4A?si=7PcZQtgR9bGjBbl4"/>
+    <hyperlink ref="E452" r:id="rId1013" display="https://www.geeksforgeeks.org/longest-palindromic-subsequence-dp-12/"/>
+    <hyperlink ref="C453" r:id="rId1014"/>
+    <hyperlink ref="D453" r:id="rId1015" display="https://youtu.be/xPBLEj41rFU?si=V9kn1IUGTx3DAlSJ"/>
+    <hyperlink ref="E453" r:id="rId1016" display="https://www.geeksforgeeks.org/minimum-insertions-to-form-a-palindrome-dp-28/"/>
+    <hyperlink ref="C454" r:id="rId1017"/>
+    <hyperlink ref="D454" r:id="rId1018" display="https://youtu.be/yMnH0jrir0Q?si=wz6fbYwdh8tJgOtr"/>
+    <hyperlink ref="E454" r:id="rId1019" display="https://www.geeksforgeeks.org/minimum-number-deletions-insertions-transform-one-string-another/"/>
+    <hyperlink ref="C455" r:id="rId1020"/>
+    <hyperlink ref="D455" r:id="rId1021" display="https://youtu.be/xElxAuBcvsU?si=4dBiTvsaW1LiQ4Qm"/>
+    <hyperlink ref="E455" r:id="rId1022" display="https://www.geeksforgeeks.org/shortest-common-supersequence/"/>
+    <hyperlink ref="C456" r:id="rId1023"/>
+    <hyperlink ref="D456" r:id="rId1024" display="https://youtu.be/_wP9mWNPL5w?si=XyPQqcffZg1cYk6z"/>
+    <hyperlink ref="E456" r:id="rId1025" display="https://www.geeksforgeeks.org/longest-common-subarray-in-the-given-two-arrays/"/>
+    <hyperlink ref="C457" r:id="rId1026"/>
+    <hyperlink ref="D457" r:id="rId1027" display="https://youtu.be/UflHuQj6MVA?si=yUS26OPaaMqlvpcb"/>
+    <hyperlink ref="E457" r:id="rId1028" display="https://www.geeksforgeeks.org/longest-palindromic-substring/"/>
+    <hyperlink ref="C458" r:id="rId1029"/>
+    <hyperlink ref="D458" r:id="rId1030" display="https://youtu.be/ZqG89Z-dKpI?si=E5MPTzZgCWf45VvN"/>
+    <hyperlink ref="E458" r:id="rId1031" display="https://www.geeksforgeeks.org/longest-palindromic-substring/"/>
+    <hyperlink ref="C460" r:id="rId1032"/>
+    <hyperlink ref="D460" r:id="rId1033" display="https://youtu.be/fJaKO8FbDdo?si=SgjrMJO4gsNPV5r6"/>
+    <hyperlink ref="E460" r:id="rId1034" display="https://www.geeksforgeeks.org/edit-distance-dp-5/"/>
+    <hyperlink ref="C461" r:id="rId1035"/>
+    <hyperlink ref="D461" r:id="rId1036" display="https://youtu.be/nVG7eTiD2bY?si=FMMLyM58YqKYxEjh"/>
+    <hyperlink ref="C462" r:id="rId1037"/>
+    <hyperlink ref="D462" r:id="rId1038" display="https://youtu.be/ZmlQ3vgAOMo?si=aqw8ylH5x88-LlJs"/>
+    <hyperlink ref="E462" r:id="rId1039" display="https://www.geeksforgeeks.org/wildcard-pattern-matching/"/>
+    <hyperlink ref="C463" r:id="rId1040"/>
+    <hyperlink ref="D463" r:id="rId1041" display="https://youtu.be/Sx9NNgInc3A?si=BVL4wXtCz9BgZLrL"/>
+    <hyperlink ref="E463" r:id="rId1042" display="https://www.geeksforgeeks.org/length-of-the-longest-valid-substring/"/>
+    <hyperlink ref="C464" r:id="rId1043"/>
+    <hyperlink ref="D464" r:id="rId1044" display="https://youtu.be/Sx9NNgInc3A?si=Hmn5-egLse5GkvIx"/>
+    <hyperlink ref="E464" r:id="rId1045" display="https://www.geeksforgeeks.org/word-break-problem-dp-32/"/>
+    <hyperlink ref="C465" r:id="rId1046"/>
+    <hyperlink ref="E465" r:id="rId1047" display="https://www.geeksforgeeks.org/word-break-problem-dp-32/"/>
+    <hyperlink ref="C466" r:id="rId1048"/>
+    <hyperlink ref="D466" r:id="rId1049" display="https://youtu.be/aPdpJ_RjaXs?si=Ic_4lgafd2xh_odL"/>
+    <hyperlink ref="E466" r:id="rId1050" display="https://www.geeksforgeeks.org/word-wrap-problem-dp-19/"/>
+    <hyperlink ref="C467" r:id="rId1051"/>
+    <hyperlink ref="D467" r:id="rId1052" display="https://youtu.be/3Rw3p9LrgvE?si=WDE8R_TrpBnzAeKL"/>
+    <hyperlink ref="E467" r:id="rId1053" display="https://www.geeksforgeeks.org/find-if-a-string-is-interleaved-of-two-other-strings-dp-33/"/>
+    <hyperlink ref="C469" r:id="rId1054"/>
+    <hyperlink ref="D469" r:id="rId1055" display="https://youtu.be/excAOvwF_Wk?si=e7EyG99KPKityBdF"/>
+    <hyperlink ref="C470" r:id="rId1056"/>
+    <hyperlink ref="D470" r:id="rId1057" display="https://youtu.be/nGJmxkUJQGs?si=_mVvHG8iLKwA95lW"/>
+    <hyperlink ref="C471" r:id="rId1058"/>
+    <hyperlink ref="D471" r:id="rId1059" display="https://youtu.be/-uQGzhYj8BQ?si=FDuxAlLnMWU9e21u"/>
+    <hyperlink ref="C472" r:id="rId1060"/>
+    <hyperlink ref="D472" r:id="rId1061" display="https://youtu.be/IV1dHbk5CDc?si=TILc-BmsGoxTljr-"/>
+    <hyperlink ref="C473" r:id="rId1062"/>
+    <hyperlink ref="D473" r:id="rId1063" display="https://youtu.be/IGIe46xw3YY?si=iUqI6GSSB8BugjDm"/>
+    <hyperlink ref="C474" r:id="rId1064"/>
+    <hyperlink ref="D474" r:id="rId1065" display="https://youtu.be/k4eK-vEmnKg?si=wiaYE8Ioi-K-rSZ0"/>
+    <hyperlink ref="C476" r:id="rId1066"/>
+    <hyperlink ref="D476" r:id="rId1067" display="https://youtu.be/pDCXsbAw5Cg?si=P9UB4sQ8a6vvd2_I"/>
+    <hyperlink ref="E476" r:id="rId1068" display="https://www.geeksforgeeks.org/matrix-chain-multiplication-dp-8/"/>
+    <hyperlink ref="C477" r:id="rId1069"/>
+    <hyperlink ref="D477" r:id="rId1070" display="https://youtu.be/xwomavsC86c?si=IufdXqTfIa1F0V6I"/>
+    <hyperlink ref="E477" r:id="rId1071" display="https://takeuforward.org/data-structure/minimum-cost-to-cut-the-stick-dp-50/"/>
+    <hyperlink ref="C478" r:id="rId1072"/>
+    <hyperlink ref="D478" r:id="rId1073" display="https://youtu.be/Yz4LlDSlkns?si=d7mq5OJwAtvOBAz2"/>
+    <hyperlink ref="E478" r:id="rId1074" display="https://www.geeksforgeeks.org/burst-balloon-to-maximize-coins/"/>
+    <hyperlink ref="C479" r:id="rId1075"/>
+    <hyperlink ref="D479" r:id="rId1076" display="https://youtu.be/MM7fXopgyjw?si=qhNd2faXTK1r5x04"/>
+    <hyperlink ref="E479" r:id="rId1077" display="https://www.geeksforgeeks.org/boolean-parenthesization-problem-dp-37/"/>
+    <hyperlink ref="C480" r:id="rId1078"/>
+    <hyperlink ref="D480" r:id="rId1079" display="https://youtu.be/_H8V5hJUGd0?si=Sxlz-OqRVMjbgwgu"/>
+    <hyperlink ref="E480" r:id="rId1080" display="https://www.geeksforgeeks.org/palindrome-partitioning-dp-17/"/>
+    <hyperlink ref="C481" r:id="rId1081"/>
+    <hyperlink ref="D481" r:id="rId1082" display="https://youtu.be/PhWWJmaKfMc?si=qNDjjLCux8ibRyu-"/>
+    <hyperlink ref="E481" r:id="rId1083" display="https://www.geeksforgeeks.org/maximum-average-sum-partition-array/"/>
+    <hyperlink ref="C482" r:id="rId1084"/>
+    <hyperlink ref="D482" r:id="rId1085" display="https://youtu.be/tOylVCugy9k?si=eDTgv7YFHqvrRGMe"/>
+    <hyperlink ref="E482" r:id="rId1086" display="https://www.geeksforgeeks.org/maximum-size-rectangle-binary-sub-matrix-1s/"/>
+    <hyperlink ref="C483" r:id="rId1087"/>
+    <hyperlink ref="D483" r:id="rId1088" display="https://youtu.be/auS1fynpnjo?si=iq5LsCojilevzhM4"/>
+    <hyperlink ref="D486" r:id="rId1089" display="https://youtu.be/N0Frqx9UlrI?si=4iJkhpOo2ry9QwtQ"/>
+    <hyperlink ref="C487" r:id="rId1090" display="https://www.codingninjas.com/studio/problems/min-heap-implementation_5480527"/>
+    <hyperlink ref="D487" r:id="rId1091" display="https://youtu.be/cuL8gXCSA58?si=LkYy8KbCthuzly5l"/>
+    <hyperlink ref="E487" r:id="rId1092" display="https://www.geeksforgeeks.org/introduction-to-min-heap-data-structure/"/>
+    <hyperlink ref="C488" r:id="rId1093"/>
+    <hyperlink ref="D488" r:id="rId1094" display="https://youtu.be/cuL8gXCSA58?si=uWFN4dlnEnzdzQtq"/>
+    <hyperlink ref="E488" r:id="rId1095" display="https://www.geeksforgeeks.org/introduction-to-max-heap-data-structure/"/>
+    <hyperlink ref="C489" r:id="rId1096"/>
+    <hyperlink ref="D489" r:id="rId1097" display="https://youtu.be/cuL8gXCSA58?si=eC60B9JXzRSI_yFt"/>
+    <hyperlink ref="E489" r:id="rId1098" display="https://www.geeksforgeeks.org/convert-min-heap-to-max-heap/"/>
+    <hyperlink ref="C491" r:id="rId1099"/>
+    <hyperlink ref="D491" r:id="rId1100" display="https://youtu.be/aXJ-p3Qa4TY?si=eWjySsOqZUjCCwBP"/>
+    <hyperlink ref="E491" r:id="rId1101" display="https://www.geeksforgeeks.org/kth-smallest-largest-element-in-unsorted-array/"/>
+    <hyperlink ref="D492" r:id="rId1102" display="https://youtu.be/aXJ-p3Qa4TY?si=oPUFQfZaeFc3tOd_"/>
+    <hyperlink ref="C493" r:id="rId1103"/>
+    <hyperlink ref="D493" r:id="rId1104" display="https://youtu.be/Wh3A29psE_Y?si=X6AP6AiuXpjrM79V"/>
+    <hyperlink ref="C494" r:id="rId1105"/>
+    <hyperlink ref="D494" r:id="rId1106" display="https://youtu.be/YPTqKIgVk-k?si=HGG49q2YPTg-ke_v"/>
+    <hyperlink ref="C495" r:id="rId1107"/>
+    <hyperlink ref="D495" r:id="rId1108" display="https://youtu.be/vltY5jxqcco?si=ZHg-JUnHMX2FgvRM"/>
+    <hyperlink ref="C496" r:id="rId1109"/>
+    <hyperlink ref="D496" r:id="rId1110" display="https://youtu.be/hOjcdrqMoQ8?si=RklRakI8BwOIfYwb"/>
+    <hyperlink ref="E496" r:id="rId1111" display="https://www.geeksforgeeks.org/kth-largest-element-in-a-stream/"/>
+    <hyperlink ref="C497" r:id="rId1112"/>
+    <hyperlink ref="D497" r:id="rId1113" display="https://youtu.be/2g_b1aYTHeg?si=yHEmKdbQDc-C-Li9"/>
+    <hyperlink ref="C498" r:id="rId1114"/>
+    <hyperlink ref="D498" r:id="rId1115" display="https://www.youtube.com/live/C3YCL18cIHM?si=YPvoeHFRgzdCx35n"/>
+    <hyperlink ref="C499" r:id="rId1116"/>
+    <hyperlink ref="C500" r:id="rId1117"/>
+    <hyperlink ref="E500" r:id="rId1118" display="https://youtu.be/X5SuOsIWCoI?si=WH6z4uaMzE8B_UOK"/>
+    <hyperlink ref="C502" r:id="rId1119"/>
+    <hyperlink ref="D502" r:id="rId1120" display="https://youtu.be/kpCesr9VXDA?si=UyD8orvz_UXvSQhl"/>
+    <hyperlink ref="E502" r:id="rId1121" display="https://www.geeksforgeeks.org/merge-k-sorted-arrays/"/>
+    <hyperlink ref="C503" r:id="rId1122"/>
+    <hyperlink ref="C504" r:id="rId1123"/>
+    <hyperlink ref="C506" r:id="rId1124"/>
+    <hyperlink ref="D506" r:id="rId1125" display="https://youtu.be/itmhHWaHupI?si=kOhqNsy0u87ew1gQ"/>
+    <hyperlink ref="E506" r:id="rId1126" display="https://www.geeksforgeeks.org/median-of-stream-of-integers-running-integers/"/>
+    <hyperlink ref="C507" r:id="rId1127"/>
+    <hyperlink ref="D507" r:id="rId1128" display="https://youtu.be/DfljaUwZsOk?si=ATC7K2_3a6QPXdsS"/>
+    <hyperlink ref="C508" r:id="rId1129"/>
+    <hyperlink ref="C510" r:id="rId1130"/>
+    <hyperlink ref="D510" r:id="rId1131" display="https://youtu.be/f7JOBJIC-NA?si=qACVSM1NauAdTfmG"/>
+    <hyperlink ref="E510" r:id="rId1132" display="https://www.geeksforgeeks.org/connect-n-ropes-minimum-cost/"/>
+    <hyperlink ref="C511" r:id="rId1133"/>
+    <hyperlink ref="D511" r:id="rId1134" display="https://youtu.be/FdzJmTCVyJU?si=I_7q86O10M1_5nTy"/>
+    <hyperlink ref="E511" r:id="rId1135" display="https://www.geeksforgeeks.org/find-maximum-meetings-in-one-room/"/>
+    <hyperlink ref="C512" r:id="rId1136"/>
+    <hyperlink ref="D512" r:id="rId1137" display="https://youtu.be/IbhQ3U5NHLI?si=PSp_XzWTzv4wQ57W"/>
+    <hyperlink ref="E512" r:id="rId1138" display="https://www.geeksforgeeks.org/minimum-cost-to-complete-given-tasks-if-cost-of-1-7-and-30-days-are-given/"/>
+    <hyperlink ref="C513" r:id="rId1139"/>
+    <hyperlink ref="E513" r:id="rId1140" display="https://www.geeksforgeeks.org/minimum-cost-to-process-m-tasks-where-switching-costs/"/>
+    <hyperlink ref="C514" r:id="rId1141"/>
+    <hyperlink ref="D514" r:id="rId1142" display="https://youtu.be/sKjKLN5JswQ?si=kF07TsHuwP_jmuzh"/>
+    <hyperlink ref="E514" r:id="rId1143" display="https://www.geeksforgeeks.org/minimize-refills-to-reach-end-of-path/"/>
+    <hyperlink ref="C517" r:id="rId1144"/>
+    <hyperlink ref="D517" r:id="rId1145" display="https://youtu.be/oobqoCJlHA0?si=HTMe5ROchxy4KAaU"/>
+    <hyperlink ref="E517" r:id="rId1146" display="https://www.geeksforgeeks.org/trie-insert-and-search/"/>
+    <hyperlink ref="C518" r:id="rId1147" display="https://www.geeksforgeeks.org/problems/word-break-trie--141631/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D518" r:id="rId1148" display="https://youtu.be/th4OnoGasMU?si=r6--sa8rf-0P2Hc0"/>
+    <hyperlink ref="E518" r:id="rId1149" display="https://www.geeksforgeeks.org/word-break-problem-trie-solution/"/>
+    <hyperlink ref="C519" r:id="rId1150"/>
+    <hyperlink ref="D519" r:id="rId1151" display="https://youtu.be/fhyIORFDD0k?si=llRsS8TY44gkz9s6"/>
+    <hyperlink ref="E519" r:id="rId1152" display="https://www.geeksforgeeks.org/longest-common-prefix-using-sorting/"/>
+    <hyperlink ref="C520" r:id="rId1153" display="https://www.geeksforgeeks.org/problems/maximum-xor-of-two-numbers-in-an-array/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D520" r:id="rId1154" display="https://youtu.be/jCuZCbXnpLo?si=bjswCkTxSANJnuQj"/>
+    <hyperlink ref="E520" r:id="rId1155" display="https://www.geeksforgeeks.org/maximum-xor-of-two-numbers-in-an-array/"/>
+    <hyperlink ref="C521" r:id="rId1156" display="https://www.geeksforgeeks.org/problems/unique-rows-in-boolean-matrix/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D521" r:id="rId1157" display="https://youtu.be/GixyVinjtFk?si=7THXd_L892zgFeIw"/>
+    <hyperlink ref="E521" r:id="rId1158" display="https://www.geeksforgeeks.org/print-unique-rows/"/>
+    <hyperlink ref="C522" r:id="rId1159"/>
+    <hyperlink ref="D522" r:id="rId1160" display="https://www.youtube.com/live/bs4MqQ_0ZS0?si=Xgos1T5uEzHu__1a"/>
+    <hyperlink ref="E522" r:id="rId1161" display="https://www.geeksforgeeks.org/count-of-strings-whose-prefix-match-with-the-given-string-to-a-given-length-k/"/>
+    <hyperlink ref="C525" r:id="rId1162"/>
+    <hyperlink ref="D525" r:id="rId1163" display="https://youtu.be/2I9XO8jwZCA?si=ldC-gp4Wv4Gra1z7"/>
+    <hyperlink ref="E525" r:id="rId1164" display="https://www.geeksforgeeks.org/write-your-own-atoi/"/>
+    <hyperlink ref="C526" r:id="rId1165"/>
+    <hyperlink ref="E526" r:id="rId1166" display="https://www.geeksforgeeks.org/look-and-say-sequence/"/>
+    <hyperlink ref="C527" r:id="rId1167" display="https://www.geeksforgeeks.org/problems/count-the-reversals0401/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D527" r:id="rId1168" display="https://youtu.be/8q1sma-qMsA?si=22qpLT56elmIfBgl"/>
+    <hyperlink ref="E527" r:id="rId1169" display="https://www.geeksforgeeks.org/minimum-number-of-bracket-reversals-needed-to-make-an-expression-balanced/"/>
+    <hyperlink ref="C528" r:id="rId1170"/>
+    <hyperlink ref="D528" r:id="rId1171" display="https://youtu.be/oxd_Z1osgCk?si=kxhwCfdV3t6M0IHB"/>
+    <hyperlink ref="E528" r:id="rId1172" display="https://www.geeksforgeeks.org/rabin-karp-algorithm-for-pattern-searching/"/>
+    <hyperlink ref="C529" r:id="rId1173"/>
+    <hyperlink ref="E529" r:id="rId1174" display="https://www.geeksforgeeks.org/boyer-moore-algorithm-for-pattern-searching/"/>
+    <hyperlink ref="C530" r:id="rId1175"/>
+    <hyperlink ref="D530" r:id="rId1176" display="https://youtu.be/ziteu2FpYsA?si=iLKlrPrn4Qn1Pl3G"/>
+    <hyperlink ref="E530" r:id="rId1177" display="https://www.geeksforgeeks.org/longest-prefix-also-suffix/"/>
+    <hyperlink ref="C531" r:id="rId1178"/>
+    <hyperlink ref="E531" r:id="rId1179" display="https://www.geeksforgeeks.org/longest-prefix-also-suffix/"/>
+    <hyperlink ref="C532" r:id="rId1180"/>
+    <hyperlink ref="D532" r:id="rId1181" display="https://youtu.be/w6LcypDgC4w?si=q2BwgPUVgXvVBs5K"/>
+    <hyperlink ref="E532" r:id="rId1182" display="https://www.geeksforgeeks.org/recursively-remove-adjacent-duplicates-given-string/"/>
+    <hyperlink ref="C533" r:id="rId1183"/>
+    <hyperlink ref="D533" r:id="rId1184" display="https://youtu.be/KEs5UyBJ39g?si=9hG4JdZkDb_a1sju"/>
+    <hyperlink ref="E533" r:id="rId1185" display="https://www.geeksforgeeks.org/string-hashing-using-polynomial-rolling-hash-function/"/>
+    <hyperlink ref="C534" r:id="rId1186"/>
+    <hyperlink ref="D534" r:id="rId1187" display="https://youtu.be/vzdNOK2oB2E?si=jgGJngudIz4L_4oP"/>
+    <hyperlink ref="E534" r:id="rId1188" display="https://www.geeksforgeeks.org/given-a-sequence-of-words-print-all-anagrams-together/"/>
+    <hyperlink ref="C535" r:id="rId1189"/>
+    <hyperlink ref="D535" r:id="rId1190" display="https://www.youtube.com/live/-1qq3hekxBw?si=zOa8LDear3iIsWRl"/>
+    <hyperlink ref="E535" r:id="rId1191" display="https://www.geeksforgeeks.org/z-algorithm-linear-time-pattern-searching-algorithm/"/>
+    <hyperlink ref="C536" r:id="rId1192" display="https://leetcode.com/problems/shortest-palindrome/"/>
+    <hyperlink ref="D536" r:id="rId1193" display="https://youtu.be/xPBLEj41rFU?si=04dcB7ymKkMft7VE"/>
+    <hyperlink ref="E536" r:id="rId1194" display="https://www.geeksforgeeks.org/minimum-insertions-to-form-shortest-palindrome/"/>
+    <hyperlink ref="C537" r:id="rId1195"/>
+    <hyperlink ref="D537" r:id="rId1196" display="https://youtu.be/DBcbRXAlE0U?si=Nm16p-kL_VVEuAAY"/>
+    <hyperlink ref="E537" r:id="rId1197" display="https://www.geeksforgeeks.org/given-array-strings-find-strings-can-chained-form-circle/"/>
+    <hyperlink ref="C538" r:id="rId1198" display="https://www.geeksforgeeks.org/problems/roman-number-to-integer3201/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="D538" r:id="rId1199" display="https://youtu.be/dlATMslQ6Uc?si=ImmwMRmjbHD-umKR"/>
+    <hyperlink ref="E538" r:id="rId1200" display="https://www.geeksforgeeks.org/converting-roman-numerals-decimal-lying-1-3999/"/>
+    <hyperlink ref="B544" r:id="rId1201"/>
+    <hyperlink ref="B545" r:id="rId1202"/>
+    <hyperlink ref="B546" r:id="rId1203" display="https://www.overleaf.com/articles/ravi-kukretis-resume/cxprrkxbccgb"/>
+    <hyperlink ref="C34" r:id="rId1204"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1205"/>

</xml_diff>

<commit_message>
recursion 3 problem add
</commit_message>
<xml_diff>
--- a/interview problems.xlsx
+++ b/interview problems.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1910" uniqueCount="991">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1911" uniqueCount="991">
   <si>
     <t>Curious freaks CODING SHEET by Nandhini</t>
   </si>
@@ -3892,13 +3892,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="45.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="66.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="55.7109375" style="3" customWidth="1"/>
     <col min="4" max="16384" width="30.85546875" style="3"/>
@@ -4636,7 +4636,9 @@
       <c r="E45" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F45" s="4"/>
+      <c r="F45" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G45" s="4"/>
     </row>
     <row r="46" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4659,7 +4661,7 @@
       <c r="B47" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="C47" s="22" t="s">
         <v>74</v>
       </c>
       <c r="D47" s="14" t="s">
@@ -4668,7 +4670,9 @@
       <c r="E47" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="17"/>
+      <c r="F47" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5203,7 +5207,9 @@
       <c r="E77" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F77" s="17"/>
+      <c r="F77" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G77" s="17"/>
     </row>
     <row r="78" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5222,7 +5228,9 @@
       <c r="E78" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F78" s="4"/>
+      <c r="F78" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G78" s="4"/>
     </row>
     <row r="79" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5232,7 +5240,7 @@
       <c r="B79" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C79" s="14" t="s">
+      <c r="C79" s="22" t="s">
         <v>134</v>
       </c>
       <c r="D79" s="15" t="s">
@@ -5241,7 +5249,9 @@
       <c r="E79" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F79" s="4"/>
+      <c r="F79" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G79" s="4"/>
     </row>
     <row r="80" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -22579,7 +22589,7 @@
     <hyperlink ref="E44" r:id="rId67" display="https://www.geeksforgeeks.org/introduction-to-map-data-structure-and-algorithm-tutorials/"/>
     <hyperlink ref="C45" r:id="rId68"/>
     <hyperlink ref="E45" r:id="rId69" display="https://www.geeksforgeeks.org/counting-frequencies-of-array-elements/"/>
-    <hyperlink ref="C47" r:id="rId70" display="https://www.geeksforgeeks.org/problems/key-pair5616/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="C47" r:id="rId70"/>
     <hyperlink ref="D47" r:id="rId71" display="https://youtu.be/UXDSeD9mN-k?si=0OalQrKPSoSeO6io"/>
     <hyperlink ref="E47" r:id="rId72" display="https://www.geeksforgeeks.org/check-if-pair-with-given-sum-exists-in-array/"/>
     <hyperlink ref="C48" r:id="rId73" display="https://www.geeksforgeeks.org/problems/triplet-sum-in-array-1587115621/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>

</xml_diff>

<commit_message>
Array and math completed
</commit_message>
<xml_diff>
--- a/interview problems.xlsx
+++ b/interview problems.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1911" uniqueCount="991">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="991">
   <si>
     <t>Curious freaks CODING SHEET by Nandhini</t>
   </si>
@@ -3892,8 +3892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" topLeftCell="A541" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C527" sqref="C527"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5270,7 +5270,9 @@
       <c r="E80" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F80" s="17"/>
+      <c r="F80" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G80" s="17"/>
     </row>
     <row r="81" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5280,7 +5282,7 @@
       <c r="B81" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C81" s="14" t="s">
+      <c r="C81" s="22" t="s">
         <v>138</v>
       </c>
       <c r="D81" s="14" t="s">
@@ -5289,7 +5291,9 @@
       <c r="E81" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F81" s="17"/>
+      <c r="F81" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G81" s="17"/>
     </row>
     <row r="82" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5299,7 +5303,7 @@
       <c r="B82" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C82" s="14" t="s">
+      <c r="C82" s="22" t="s">
         <v>140</v>
       </c>
       <c r="D82" s="15" t="s">
@@ -5308,7 +5312,9 @@
       <c r="E82" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="F82" s="4"/>
+      <c r="F82" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G82" s="4"/>
     </row>
     <row r="83" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5318,7 +5324,7 @@
       <c r="B83" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C83" s="14" t="s">
+      <c r="C83" s="22" t="s">
         <v>143</v>
       </c>
       <c r="D83" s="15" t="s">
@@ -5337,7 +5343,7 @@
       <c r="B84" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C84" s="14" t="s">
+      <c r="C84" s="22" t="s">
         <v>145</v>
       </c>
       <c r="D84" s="15" t="s">
@@ -22673,13 +22679,13 @@
     <hyperlink ref="C80" r:id="rId151" display="https://www.geeksforgeeks.org/problems/nth-fibonacci-number1335/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
     <hyperlink ref="D80" r:id="rId152" display="https://youtu.be/kvRjNm4rVBE?si=HoIm_q77BpGtePSF"/>
     <hyperlink ref="E80" r:id="rId153" display="https://www.geeksforgeeks.org/program-for-nth-fibonacci-number/"/>
-    <hyperlink ref="C81" r:id="rId154" display="https://www.geeksforgeeks.org/problems/power-of-numbers-1587115620/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article"/>
+    <hyperlink ref="C81" r:id="rId154"/>
     <hyperlink ref="D81" r:id="rId155" display="https://youtu.be/l0YC3876qxg?si=gpooiy_1Voz_M2b6"/>
     <hyperlink ref="E81" r:id="rId156" display="https://www.geeksforgeeks.org/write-a-c-program-to-calculate-powxn/"/>
     <hyperlink ref="C82" r:id="rId157"/>
     <hyperlink ref="D82" r:id="rId158" display="https://youtu.be/tNm_NNSB3_w?si=qRueLOLTmrBAtTTC"/>
     <hyperlink ref="E82" r:id="rId159" display="https://www.geeksforgeeks.org/c-programs-print-interesting-patterns/"/>
-    <hyperlink ref="C83" r:id="rId160" display="https://practice.geeksforgeeks.org/problems/implement-atoi/1?utm_source=geeksforgeeks&amp;utm_medium=ml_article_practice_tab&amp;utm_campaign=article_practice_tab"/>
+    <hyperlink ref="C83" r:id="rId160"/>
     <hyperlink ref="D83" r:id="rId161" display="https://youtu.be/cXf7NKgT13s?si=7CiE2Yq4IRTwI3vh"/>
     <hyperlink ref="E83" r:id="rId162" display="https://www.geeksforgeeks.org/recursive-implementation-of-atoi/"/>
     <hyperlink ref="C84" r:id="rId163"/>

</xml_diff>

<commit_message>
This is updated test class and interview excel
</commit_message>
<xml_diff>
--- a/interview problems.xlsx
+++ b/interview problems.xlsx
@@ -3571,6 +3571,21 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -3594,21 +3609,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3892,8 +3892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A541" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C527" sqref="C527"/>
+    <sheetView tabSelected="1" topLeftCell="A535" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C526" sqref="C526"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3905,103 +3905,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="29"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="32"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="26"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="41"/>
     </row>
     <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="32"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="47"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="35"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="50"/>
     </row>
     <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="38"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="53"/>
     </row>
     <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="55"/>
     </row>
     <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="43"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="58"/>
     </row>
     <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
@@ -4013,15 +4013,15 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="41"/>
     </row>
     <row r="12" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
@@ -5016,12 +5016,12 @@
       <c r="A66" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B66" s="44" t="s">
+      <c r="B66" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="C66" s="45"/>
-      <c r="D66" s="45"/>
-      <c r="E66" s="46"/>
+      <c r="C66" s="60"/>
+      <c r="D66" s="60"/>
+      <c r="E66" s="61"/>
       <c r="F66" s="12"/>
       <c r="G66" s="12"/>
     </row>
@@ -13767,24 +13767,24 @@
       <c r="G539" s="12"/>
     </row>
     <row r="540" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A540" s="24" t="s">
+      <c r="A540" s="39" t="s">
         <v>975</v>
       </c>
-      <c r="B540" s="25"/>
-      <c r="C540" s="25"/>
-      <c r="D540" s="25"/>
-      <c r="E540" s="26"/>
+      <c r="B540" s="40"/>
+      <c r="C540" s="40"/>
+      <c r="D540" s="40"/>
+      <c r="E540" s="41"/>
       <c r="F540" s="4"/>
       <c r="G540" s="4"/>
     </row>
     <row r="541" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A541" s="47" t="s">
+      <c r="A541" s="24" t="s">
         <v>986</v>
       </c>
-      <c r="B541" s="48"/>
-      <c r="C541" s="48"/>
-      <c r="D541" s="48"/>
-      <c r="E541" s="49"/>
+      <c r="B541" s="25"/>
+      <c r="C541" s="25"/>
+      <c r="D541" s="25"/>
+      <c r="E541" s="26"/>
       <c r="F541" s="17"/>
       <c r="G541" s="17"/>
     </row>
@@ -13810,12 +13810,12 @@
       <c r="A544" s="1" t="s">
         <v>976</v>
       </c>
-      <c r="B544" s="50" t="s">
+      <c r="B544" s="27" t="s">
         <v>977</v>
       </c>
-      <c r="C544" s="51"/>
-      <c r="D544" s="51"/>
-      <c r="E544" s="52"/>
+      <c r="C544" s="28"/>
+      <c r="D544" s="28"/>
+      <c r="E544" s="29"/>
       <c r="F544" s="17"/>
       <c r="G544" s="17"/>
     </row>
@@ -13823,12 +13823,12 @@
       <c r="A545" s="1" t="s">
         <v>978</v>
       </c>
-      <c r="B545" s="53" t="s">
+      <c r="B545" s="30" t="s">
         <v>979</v>
       </c>
-      <c r="C545" s="54"/>
-      <c r="D545" s="54"/>
-      <c r="E545" s="55"/>
+      <c r="C545" s="31"/>
+      <c r="D545" s="31"/>
+      <c r="E545" s="32"/>
       <c r="F545" s="17"/>
       <c r="G545" s="17"/>
     </row>
@@ -13836,25 +13836,25 @@
       <c r="A546" s="2" t="s">
         <v>980</v>
       </c>
-      <c r="B546" s="56" t="s">
+      <c r="B546" s="33" t="s">
         <v>981</v>
       </c>
-      <c r="C546" s="57"/>
-      <c r="D546" s="57"/>
-      <c r="E546" s="58"/>
+      <c r="C546" s="34"/>
+      <c r="D546" s="34"/>
+      <c r="E546" s="35"/>
       <c r="F546" s="17"/>
       <c r="G546" s="17"/>
     </row>
     <row r="547" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A547" s="59" t="s">
+      <c r="A547" s="36" t="s">
         <v>982</v>
       </c>
-      <c r="B547" s="60"/>
-      <c r="C547" s="60"/>
-      <c r="D547" s="60"/>
-      <c r="E547" s="60"/>
-      <c r="F547" s="60"/>
-      <c r="G547" s="61"/>
+      <c r="B547" s="37"/>
+      <c r="C547" s="37"/>
+      <c r="D547" s="37"/>
+      <c r="E547" s="37"/>
+      <c r="F547" s="37"/>
+      <c r="G547" s="38"/>
     </row>
     <row r="548" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A548" s="4"/>
@@ -22507,11 +22507,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A541:E541"/>
-    <mergeCell ref="B544:E544"/>
-    <mergeCell ref="B545:E545"/>
-    <mergeCell ref="B546:E546"/>
-    <mergeCell ref="A547:G547"/>
     <mergeCell ref="A540:E540"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:E2"/>
@@ -22524,6 +22519,11 @@
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="B66:E66"/>
+    <mergeCell ref="A541:E541"/>
+    <mergeCell ref="B544:E544"/>
+    <mergeCell ref="B545:E545"/>
+    <mergeCell ref="B546:E546"/>
+    <mergeCell ref="A547:G547"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="https://www.youtube.com/@curiousfreaks_"/>

</xml_diff>